<commit_message>
add AdvertAnalitycDAO and change ExcelReport
</commit_message>
<xml_diff>
--- a/ready/report1.xlsx
+++ b/ready/report1.xlsx
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="166">
   <si>
     <t>quality</t>
   </si>
@@ -579,19 +579,22 @@
     <t>828.0</t>
   </si>
   <si>
-    <t>0.36407767</t>
-  </si>
-  <si>
-    <t>78,86</t>
+    <t>7.0</t>
+  </si>
+  <si>
+    <t>0,85</t>
   </si>
   <si>
     <t>171.0</t>
   </si>
   <si>
-    <t>16,29</t>
-  </si>
-  <si>
-    <t>На долю планшетов и смартфонов приходится 16,29% трафика</t>
+    <t>0,00</t>
+  </si>
+  <si>
+    <t>51.0</t>
+  </si>
+  <si>
+    <t>На долю планшетов и смартфонов приходится 21,14% трафика</t>
   </si>
   <si>
     <t>младше 18 лет</t>
@@ -1146,102 +1149,6 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1265,6 +1172,102 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -10087,8 +10090,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="B1:U406"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A67" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B280" sqref="B280:D280"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A196" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="I210" sqref="I210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10139,52 +10142,52 @@
     </row>
     <row r="104" spans="6:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="105" spans="6:16" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="F105" s="126" t="s">
+      <c r="F105" s="110" t="s">
         <v>22</v>
       </c>
-      <c r="G105" s="126"/>
-      <c r="H105" s="126"/>
-      <c r="I105" s="126"/>
-      <c r="J105" s="126"/>
-      <c r="K105" s="126"/>
-      <c r="L105" s="126"/>
-      <c r="M105" s="126"/>
-      <c r="N105" s="126"/>
-      <c r="O105" s="126"/>
-      <c r="P105" s="126"/>
+      <c r="G105" s="110"/>
+      <c r="H105" s="110"/>
+      <c r="I105" s="110"/>
+      <c r="J105" s="110"/>
+      <c r="K105" s="110"/>
+      <c r="L105" s="110"/>
+      <c r="M105" s="110"/>
+      <c r="N105" s="110"/>
+      <c r="O105" s="110"/>
+      <c r="P105" s="110"/>
     </row>
     <row r="106" spans="6:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="110" spans="6:16" ht="21" x14ac:dyDescent="0.35">
       <c r="K110" s="96" t="s">
         <v>122</v>
       </c>
-      <c r="L110" s="127"/>
-      <c r="M110" s="127"/>
-      <c r="N110" s="127"/>
+      <c r="L110" s="111"/>
+      <c r="M110" s="111"/>
+      <c r="N110" s="111"/>
     </row>
     <row r="113" spans="9:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K113" s="96" t="s">
         <v>123</v>
       </c>
-      <c r="L113" s="127"/>
-      <c r="M113" s="127"/>
-      <c r="N113" s="127"/>
+      <c r="L113" s="111"/>
+      <c r="M113" s="111"/>
+      <c r="N113" s="111"/>
     </row>
     <row r="116" spans="9:14" ht="21" x14ac:dyDescent="0.35">
       <c r="K116" s="96" t="s">
         <v>124</v>
       </c>
-      <c r="L116" s="128"/>
-      <c r="M116" s="128"/>
-      <c r="N116" s="128"/>
+      <c r="L116" s="112"/>
+      <c r="M116" s="112"/>
+      <c r="N116" s="112"/>
     </row>
     <row r="120" spans="9:14" ht="21" x14ac:dyDescent="0.35">
       <c r="K120" s="96" t="s">
         <v>125</v>
       </c>
-      <c r="L120" s="127"/>
-      <c r="M120" s="127"/>
-      <c r="N120" s="127"/>
+      <c r="L120" s="111"/>
+      <c r="M120" s="111"/>
+      <c r="N120" s="111"/>
     </row>
     <row r="124" spans="9:14" ht="21" x14ac:dyDescent="0.35">
       <c r="I124" s="19"/>
@@ -10192,20 +10195,20 @@
       <c r="K124" s="96" t="s">
         <v>126</v>
       </c>
-      <c r="L124" s="125"/>
-      <c r="M124" s="125"/>
-      <c r="N124" s="125"/>
+      <c r="L124" s="109"/>
+      <c r="M124" s="109"/>
+      <c r="N124" s="109"/>
     </row>
     <row r="127" spans="9:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="128" spans="9:14" ht="21" x14ac:dyDescent="0.35">
       <c r="I128" s="96" t="s">
         <v>127</v>
       </c>
-      <c r="J128" s="129"/>
-      <c r="K128" s="129"/>
-      <c r="L128" s="129"/>
-      <c r="M128" s="129"/>
-      <c r="N128" s="129"/>
+      <c r="J128" s="113"/>
+      <c r="K128" s="113"/>
+      <c r="L128" s="113"/>
+      <c r="M128" s="113"/>
+      <c r="N128" s="113"/>
     </row>
     <row r="129" spans="6:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K129" s="16"/>
@@ -10214,35 +10217,35 @@
     </row>
     <row r="134" spans="6:13" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="137" spans="6:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F137" s="130" t="s">
+      <c r="F137" s="114" t="s">
         <v>23</v>
       </c>
-      <c r="G137" s="130"/>
-      <c r="H137" s="131" t="s">
+      <c r="G137" s="114"/>
+      <c r="H137" s="116" t="s">
         <v>24</v>
       </c>
-      <c r="I137" s="131"/>
-      <c r="J137" s="131"/>
-      <c r="K137" s="130" t="s">
+      <c r="I137" s="116"/>
+      <c r="J137" s="116"/>
+      <c r="K137" s="114" t="s">
         <v>25</v>
       </c>
-      <c r="L137" s="130"/>
+      <c r="L137" s="114"/>
       <c r="M137" s="86"/>
     </row>
     <row r="138" spans="6:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F138" s="84" t="s">
         <v>140</v>
       </c>
-      <c r="G138" s="120"/>
+      <c r="G138" s="115"/>
       <c r="H138" s="84" t="s">
         <v>141</v>
       </c>
-      <c r="I138" s="132"/>
-      <c r="J138" s="132"/>
+      <c r="I138" s="117"/>
+      <c r="J138" s="117"/>
       <c r="K138" s="84" t="s">
         <v>142</v>
       </c>
-      <c r="L138" s="120"/>
+      <c r="L138" s="115"/>
       <c r="M138" s="87"/>
     </row>
     <row r="139" spans="6:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10269,13 +10272,13 @@
       <c r="F141" s="72" t="s">
         <v>128</v>
       </c>
-      <c r="G141" s="112"/>
-      <c r="H141" s="120" t="s">
+      <c r="G141" s="118"/>
+      <c r="H141" s="115" t="s">
         <v>26</v>
       </c>
-      <c r="I141" s="120"/>
-      <c r="J141" s="120"/>
-      <c r="K141" s="120"/>
+      <c r="I141" s="115"/>
+      <c r="J141" s="115"/>
+      <c r="K141" s="115"/>
       <c r="L141" s="72" t="s">
         <v>129</v>
       </c>
@@ -10285,13 +10288,13 @@
       <c r="F142" s="84" t="s">
         <v>130</v>
       </c>
-      <c r="G142" s="111"/>
-      <c r="H142" s="119" t="s">
+      <c r="G142" s="119"/>
+      <c r="H142" s="120" t="s">
         <v>27</v>
       </c>
-      <c r="I142" s="119"/>
-      <c r="J142" s="119"/>
-      <c r="K142" s="119"/>
+      <c r="I142" s="120"/>
+      <c r="J142" s="120"/>
+      <c r="K142" s="120"/>
       <c r="L142" s="84" t="s">
         <v>131</v>
       </c>
@@ -10301,13 +10304,13 @@
       <c r="F143" s="72" t="s">
         <v>132</v>
       </c>
-      <c r="G143" s="112"/>
-      <c r="H143" s="120" t="s">
+      <c r="G143" s="118"/>
+      <c r="H143" s="115" t="s">
         <v>28</v>
       </c>
-      <c r="I143" s="120"/>
-      <c r="J143" s="120"/>
-      <c r="K143" s="120"/>
+      <c r="I143" s="115"/>
+      <c r="J143" s="115"/>
+      <c r="K143" s="115"/>
       <c r="L143" s="72" t="s">
         <v>133</v>
       </c>
@@ -10317,13 +10320,13 @@
       <c r="F144" s="84" t="s">
         <v>134</v>
       </c>
-      <c r="G144" s="111"/>
-      <c r="H144" s="119" t="s">
+      <c r="G144" s="119"/>
+      <c r="H144" s="120" t="s">
         <v>29</v>
       </c>
-      <c r="I144" s="119"/>
-      <c r="J144" s="119"/>
-      <c r="K144" s="119"/>
+      <c r="I144" s="120"/>
+      <c r="J144" s="120"/>
+      <c r="K144" s="120"/>
       <c r="L144" s="84" t="s">
         <v>135</v>
       </c>
@@ -10333,27 +10336,27 @@
       <c r="F145" s="72" t="s">
         <v>136</v>
       </c>
-      <c r="G145" s="112"/>
-      <c r="H145" s="120" t="s">
+      <c r="G145" s="118"/>
+      <c r="H145" s="115" t="s">
         <v>30</v>
       </c>
-      <c r="I145" s="120"/>
-      <c r="J145" s="120"/>
-      <c r="K145" s="120"/>
+      <c r="I145" s="115"/>
+      <c r="J145" s="115"/>
+      <c r="K145" s="115"/>
       <c r="L145" s="72" t="s">
         <v>137</v>
       </c>
       <c r="M145" s="88"/>
     </row>
     <row r="146" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F146" s="111"/>
-      <c r="G146" s="111"/>
-      <c r="H146" s="119" t="s">
+      <c r="F146" s="119"/>
+      <c r="G146" s="119"/>
+      <c r="H146" s="120" t="s">
         <v>31</v>
       </c>
-      <c r="I146" s="119"/>
-      <c r="J146" s="119"/>
-      <c r="K146" s="119"/>
+      <c r="I146" s="120"/>
+      <c r="J146" s="120"/>
+      <c r="K146" s="120"/>
       <c r="L146" s="68"/>
       <c r="M146" s="88"/>
     </row>
@@ -10361,13 +10364,13 @@
       <c r="F147" s="72" t="s">
         <v>138</v>
       </c>
-      <c r="G147" s="112"/>
-      <c r="H147" s="120" t="s">
+      <c r="G147" s="118"/>
+      <c r="H147" s="115" t="s">
         <v>32</v>
       </c>
-      <c r="I147" s="120"/>
-      <c r="J147" s="120"/>
-      <c r="K147" s="120"/>
+      <c r="I147" s="115"/>
+      <c r="J147" s="115"/>
+      <c r="K147" s="115"/>
       <c r="L147" s="72" t="s">
         <v>138</v>
       </c>
@@ -10377,13 +10380,13 @@
       <c r="F148" s="84" t="s">
         <v>139</v>
       </c>
-      <c r="G148" s="111"/>
-      <c r="H148" s="119" t="s">
+      <c r="G148" s="119"/>
+      <c r="H148" s="120" t="s">
         <v>33</v>
       </c>
-      <c r="I148" s="119"/>
-      <c r="J148" s="119"/>
-      <c r="K148" s="119"/>
+      <c r="I148" s="120"/>
+      <c r="J148" s="120"/>
+      <c r="K148" s="120"/>
       <c r="L148" s="84" t="s">
         <v>139</v>
       </c>
@@ -10447,24 +10450,24 @@
       <c r="U195" s="24"/>
     </row>
     <row r="198" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E198" s="121" t="s">
+      <c r="E198" s="123" t="s">
         <v>39</v>
       </c>
-      <c r="F198" s="121"/>
-      <c r="G198" s="122"/>
+      <c r="F198" s="123"/>
+      <c r="G198" s="124"/>
       <c r="H198" s="26"/>
-      <c r="I198" s="121" t="s">
-        <v>38</v>
-      </c>
-      <c r="J198" s="121"/>
-      <c r="K198" s="123"/>
+      <c r="I198" s="123" t="s">
+        <v>40</v>
+      </c>
+      <c r="J198" s="123"/>
+      <c r="K198" s="125"/>
       <c r="L198" s="26"/>
       <c r="M198" s="26"/>
-      <c r="N198" s="121" t="s">
-        <v>40</v>
-      </c>
-      <c r="O198" s="121"/>
-      <c r="P198" s="123"/>
+      <c r="N198" s="123" t="s">
+        <v>38</v>
+      </c>
+      <c r="O198" s="123"/>
+      <c r="P198" s="125"/>
     </row>
     <row r="199" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E199" s="27"/>
@@ -10540,18 +10543,20 @@
       <c r="F205" s="97" t="s">
         <v>152</v>
       </c>
-      <c r="G205" s="110"/>
+      <c r="G205" s="122"/>
       <c r="H205" s="90"/>
       <c r="I205" s="97" t="s">
         <v>155</v>
       </c>
-      <c r="J205" s="110"/>
-      <c r="K205" s="110"/>
+      <c r="J205" s="122"/>
+      <c r="K205" s="122"/>
       <c r="L205" s="90"/>
       <c r="M205" s="90"/>
-      <c r="N205" s="110"/>
-      <c r="O205" s="110"/>
-      <c r="P205" s="110"/>
+      <c r="N205" s="97" t="s">
+        <v>157</v>
+      </c>
+      <c r="O205" s="122"/>
+      <c r="P205" s="122"/>
     </row>
     <row r="206" spans="2:21" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D206" s="93" t="s">
@@ -10561,18 +10566,20 @@
       <c r="F206" s="96" t="s">
         <v>153</v>
       </c>
-      <c r="G206" s="124"/>
+      <c r="G206" s="126"/>
       <c r="H206" s="91"/>
       <c r="I206" s="96" t="s">
         <v>139</v>
       </c>
-      <c r="J206" s="124"/>
-      <c r="K206" s="124"/>
+      <c r="J206" s="126"/>
+      <c r="K206" s="126"/>
       <c r="L206" s="91"/>
       <c r="M206" s="91"/>
-      <c r="N206" s="124"/>
-      <c r="O206" s="124"/>
-      <c r="P206" s="124"/>
+      <c r="N206" s="96" t="s">
+        <v>139</v>
+      </c>
+      <c r="O206" s="126"/>
+      <c r="P206" s="126"/>
     </row>
     <row r="207" spans="2:21" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D207" s="92" t="s">
@@ -10582,18 +10589,20 @@
       <c r="F207" s="97" t="s">
         <v>154</v>
       </c>
-      <c r="G207" s="110"/>
+      <c r="G207" s="122"/>
       <c r="H207" s="90"/>
       <c r="I207" s="97" t="s">
         <v>156</v>
       </c>
-      <c r="J207" s="110"/>
-      <c r="K207" s="110"/>
+      <c r="J207" s="122"/>
+      <c r="K207" s="122"/>
       <c r="L207" s="90"/>
       <c r="M207" s="90"/>
-      <c r="N207" s="110"/>
-      <c r="O207" s="110"/>
-      <c r="P207" s="110"/>
+      <c r="N207" s="97" t="s">
+        <v>156</v>
+      </c>
+      <c r="O207" s="122"/>
+      <c r="P207" s="122"/>
     </row>
     <row r="208" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E208" s="23"/>
@@ -10603,7 +10612,7 @@
       <c r="B211" s="89"/>
       <c r="C211" s="89"/>
       <c r="D211" s="78" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="E211" s="89"/>
       <c r="F211" s="89"/>
@@ -10621,19 +10630,19 @@
       <c r="J212" s="42"/>
     </row>
     <row r="229" spans="7:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="G229" s="106" t="s">
+      <c r="G229" s="121" t="s">
         <v>50</v>
       </c>
-      <c r="H229" s="106"/>
-      <c r="I229" s="106"/>
-      <c r="J229" s="106"/>
-      <c r="K229" s="106"/>
-      <c r="L229" s="106"/>
+      <c r="H229" s="121"/>
+      <c r="I229" s="121"/>
+      <c r="J229" s="121"/>
+      <c r="K229" s="121"/>
+      <c r="L229" s="121"/>
       <c r="M229" s="25"/>
     </row>
     <row r="259" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D259" s="78" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E259" s="99"/>
       <c r="F259" s="99"/>
@@ -10643,7 +10652,7 @@
     </row>
     <row r="260" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D260" s="78" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="E260" s="99"/>
       <c r="F260" s="99"/>
@@ -10652,28 +10661,28 @@
       <c r="J260" s="98"/>
     </row>
     <row r="263" spans="2:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="G263" s="106" t="s">
+      <c r="G263" s="121" t="s">
         <v>44</v>
       </c>
-      <c r="H263" s="106"/>
-      <c r="I263" s="106"/>
-      <c r="J263" s="106"/>
-      <c r="K263" s="106"/>
-      <c r="L263" s="106"/>
+      <c r="H263" s="121"/>
+      <c r="I263" s="121"/>
+      <c r="J263" s="121"/>
+      <c r="K263" s="121"/>
+      <c r="L263" s="121"/>
       <c r="M263" s="25"/>
     </row>
     <row r="266" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B266" s="115" t="s">
+      <c r="B266" s="130" t="s">
         <v>51</v>
       </c>
-      <c r="C266" s="115"/>
-      <c r="D266" s="115"/>
+      <c r="C266" s="130"/>
+      <c r="D266" s="130"/>
       <c r="E266" s="26"/>
       <c r="F266" s="26"/>
-      <c r="G266" s="115" t="s">
+      <c r="G266" s="130" t="s">
         <v>52</v>
       </c>
-      <c r="H266" s="115"/>
+      <c r="H266" s="130"/>
     </row>
     <row r="267" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E267" s="37"/>
@@ -10712,23 +10721,23 @@
       <c r="E278" s="37"/>
     </row>
     <row r="279" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B279" s="116" t="s">
+      <c r="B279" s="131" t="s">
         <v>55</v>
       </c>
-      <c r="C279" s="116"/>
-      <c r="D279" s="116"/>
+      <c r="C279" s="131"/>
+      <c r="D279" s="131"/>
       <c r="E279" s="37"/>
-      <c r="G279" s="116" t="s">
+      <c r="G279" s="131" t="s">
         <v>55</v>
       </c>
-      <c r="H279" s="116"/>
+      <c r="H279" s="131"/>
     </row>
     <row r="280" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B280" s="116"/>
-      <c r="C280" s="116"/>
-      <c r="D280" s="116"/>
-      <c r="G280" s="116"/>
-      <c r="H280" s="116"/>
+      <c r="B280" s="131"/>
+      <c r="C280" s="131"/>
+      <c r="D280" s="131"/>
+      <c r="G280" s="131"/>
+      <c r="H280" s="131"/>
     </row>
     <row r="282" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B282" s="26"/>
@@ -10743,49 +10752,49 @@
       <c r="E283" s="26"/>
     </row>
     <row r="297" spans="7:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="G297" s="102" t="s">
+      <c r="G297" s="132" t="s">
         <v>59</v>
       </c>
-      <c r="H297" s="102"/>
-      <c r="I297" s="102"/>
-      <c r="J297" s="102"/>
-      <c r="K297" s="102"/>
-      <c r="L297" s="102"/>
+      <c r="H297" s="132"/>
+      <c r="I297" s="132"/>
+      <c r="J297" s="132"/>
+      <c r="K297" s="132"/>
+      <c r="L297" s="132"/>
     </row>
     <row r="327" spans="4:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="D327" s="113" t="str">
+      <c r="D327" s="128" t="str">
         <f>"Сеансов больше всего по "&amp;popularDayOfWeek</f>
         <v xml:space="preserve">Сеансов больше всего по </v>
       </c>
-      <c r="E327" s="113"/>
-      <c r="F327" s="113"/>
-      <c r="G327" s="113"/>
-      <c r="H327" s="113"/>
-      <c r="I327" s="113"/>
-      <c r="J327" s="113"/>
-      <c r="K327" s="113"/>
+      <c r="E327" s="128"/>
+      <c r="F327" s="128"/>
+      <c r="G327" s="128"/>
+      <c r="H327" s="128"/>
+      <c r="I327" s="128"/>
+      <c r="J327" s="128"/>
+      <c r="K327" s="128"/>
     </row>
     <row r="328" spans="4:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="D328" s="113" t="str">
+      <c r="D328" s="128" t="str">
         <f>"Коэф. конверсий выше по "&amp;moreConversionDayOfWeek</f>
         <v xml:space="preserve">Коэф. конверсий выше по </v>
       </c>
-      <c r="E328" s="113"/>
-      <c r="F328" s="113"/>
-      <c r="G328" s="113"/>
-      <c r="H328" s="113"/>
-      <c r="I328" s="113"/>
-      <c r="J328" s="113"/>
-      <c r="K328" s="113"/>
+      <c r="E328" s="128"/>
+      <c r="F328" s="128"/>
+      <c r="G328" s="128"/>
+      <c r="H328" s="128"/>
+      <c r="I328" s="128"/>
+      <c r="J328" s="128"/>
+      <c r="K328" s="128"/>
     </row>
     <row r="331" spans="4:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="G331" s="106" t="s">
+      <c r="G331" s="121" t="s">
         <v>69</v>
       </c>
-      <c r="H331" s="106"/>
-      <c r="I331" s="106"/>
-      <c r="J331" s="106"/>
-      <c r="K331" s="106"/>
+      <c r="H331" s="121"/>
+      <c r="I331" s="121"/>
+      <c r="J331" s="121"/>
+      <c r="K331" s="121"/>
     </row>
     <row r="361" spans="4:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D361" s="26" t="s">
@@ -10795,136 +10804,136 @@
       <c r="F361" s="26"/>
       <c r="G361" s="26"/>
       <c r="H361" s="26"/>
-      <c r="K361" s="114">
+      <c r="K361" s="129">
         <f>popularHours</f>
         <v>0</v>
       </c>
-      <c r="L361" s="114"/>
-      <c r="M361" s="114"/>
-      <c r="N361" s="114"/>
+      <c r="L361" s="129"/>
+      <c r="M361" s="129"/>
+      <c r="N361" s="129"/>
     </row>
     <row r="366" spans="4:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="F366" s="102" t="s">
+      <c r="F366" s="132" t="s">
         <v>71</v>
       </c>
-      <c r="G366" s="102"/>
-      <c r="H366" s="102"/>
-      <c r="I366" s="102"/>
-      <c r="J366" s="102"/>
-      <c r="K366" s="102"/>
-      <c r="L366" s="102"/>
+      <c r="G366" s="132"/>
+      <c r="H366" s="132"/>
+      <c r="I366" s="132"/>
+      <c r="J366" s="132"/>
+      <c r="K366" s="132"/>
+      <c r="L366" s="132"/>
       <c r="M366" s="43"/>
     </row>
     <row r="370" spans="2:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B370" s="138" t="s">
+      <c r="B370" s="106" t="s">
         <v>72</v>
       </c>
-      <c r="C370" s="138"/>
-      <c r="D370" s="138"/>
-      <c r="E370" s="138"/>
-      <c r="F370" s="138"/>
-      <c r="G370" s="138"/>
-      <c r="H370" s="136">
+      <c r="C370" s="106"/>
+      <c r="D370" s="106"/>
+      <c r="E370" s="106"/>
+      <c r="F370" s="106"/>
+      <c r="G370" s="106"/>
+      <c r="H370" s="104">
         <f>keyWasClicked</f>
         <v>0</v>
       </c>
-      <c r="I370" s="136"/>
+      <c r="I370" s="104"/>
     </row>
     <row r="371" spans="2:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B371" s="139" t="s">
+      <c r="B371" s="107" t="s">
         <v>73</v>
       </c>
-      <c r="C371" s="139"/>
-      <c r="D371" s="139"/>
-      <c r="E371" s="139"/>
-      <c r="F371" s="139"/>
-      <c r="G371" s="139"/>
-      <c r="H371" s="137">
+      <c r="C371" s="107"/>
+      <c r="D371" s="107"/>
+      <c r="E371" s="107"/>
+      <c r="F371" s="107"/>
+      <c r="G371" s="107"/>
+      <c r="H371" s="105">
         <f>keyReachGoal</f>
         <v>0</v>
       </c>
-      <c r="I371" s="137"/>
+      <c r="I371" s="105"/>
     </row>
     <row r="372" spans="2:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B372" s="140" t="s">
+      <c r="B372" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="C372" s="140"/>
-      <c r="D372" s="140"/>
-      <c r="E372" s="140"/>
-      <c r="F372" s="140"/>
-      <c r="G372" s="140"/>
-      <c r="H372" s="136">
+      <c r="C372" s="108"/>
+      <c r="D372" s="108"/>
+      <c r="E372" s="108"/>
+      <c r="F372" s="108"/>
+      <c r="G372" s="108"/>
+      <c r="H372" s="104">
         <f>keyHasConversationPer</f>
         <v>0</v>
       </c>
-      <c r="I372" s="136"/>
+      <c r="I372" s="104"/>
     </row>
     <row r="376" spans="2:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K376" s="117" t="s">
+      <c r="K376" s="133" t="s">
         <v>83</v>
       </c>
-      <c r="L376" s="117"/>
-      <c r="M376" s="117"/>
-      <c r="N376" s="117"/>
-      <c r="O376" s="133">
+      <c r="L376" s="133"/>
+      <c r="M376" s="133"/>
+      <c r="N376" s="133"/>
+      <c r="O376" s="101">
         <f>sendAll</f>
         <v>0</v>
       </c>
-      <c r="P376" s="133"/>
-      <c r="Q376" s="133"/>
+      <c r="P376" s="101"/>
+      <c r="Q376" s="101"/>
     </row>
     <row r="377" spans="2:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K377" s="118" t="s">
+      <c r="K377" s="134" t="s">
         <v>84</v>
       </c>
-      <c r="L377" s="118"/>
-      <c r="M377" s="118"/>
-      <c r="N377" s="118"/>
-      <c r="O377" s="134">
+      <c r="L377" s="134"/>
+      <c r="M377" s="134"/>
+      <c r="N377" s="134"/>
+      <c r="O377" s="102">
         <f>costConversation</f>
         <v>0</v>
       </c>
-      <c r="P377" s="134"/>
-      <c r="Q377" s="134"/>
+      <c r="P377" s="102"/>
+      <c r="Q377" s="102"/>
     </row>
     <row r="378" spans="2:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K378" s="117" t="s">
+      <c r="K378" s="133" t="s">
         <v>85</v>
       </c>
-      <c r="L378" s="117"/>
-      <c r="M378" s="117"/>
-      <c r="N378" s="117"/>
-      <c r="O378" s="135">
+      <c r="L378" s="133"/>
+      <c r="M378" s="133"/>
+      <c r="N378" s="133"/>
+      <c r="O378" s="103">
         <f>effecientConversation</f>
         <v>0</v>
       </c>
-      <c r="P378" s="135"/>
-      <c r="Q378" s="135"/>
+      <c r="P378" s="103"/>
+      <c r="Q378" s="103"/>
     </row>
     <row r="388" spans="3:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="G388" s="102" t="s">
+      <c r="G388" s="132" t="s">
         <v>86</v>
       </c>
-      <c r="H388" s="102"/>
-      <c r="I388" s="102"/>
-      <c r="J388" s="102"/>
-      <c r="K388" s="102"/>
-      <c r="L388" s="102"/>
+      <c r="H388" s="132"/>
+      <c r="I388" s="132"/>
+      <c r="J388" s="132"/>
+      <c r="K388" s="132"/>
+      <c r="L388" s="132"/>
       <c r="M388" s="43"/>
     </row>
     <row r="391" spans="3:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C391" s="109" t="s">
+      <c r="C391" s="139" t="s">
         <v>87</v>
       </c>
-      <c r="D391" s="109"/>
-      <c r="E391" s="109"/>
-      <c r="F391" s="109" t="s">
+      <c r="D391" s="139"/>
+      <c r="E391" s="139"/>
+      <c r="F391" s="139" t="s">
         <v>88</v>
       </c>
-      <c r="G391" s="109"/>
-      <c r="H391" s="109"/>
-      <c r="I391" s="109"/>
+      <c r="G391" s="139"/>
+      <c r="H391" s="139"/>
+      <c r="I391" s="139"/>
       <c r="J391" s="52"/>
       <c r="K391" s="53" t="s">
         <v>89</v>
@@ -10936,275 +10945,325 @@
       <c r="N391" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="O391" s="109" t="s">
+      <c r="O391" s="139" t="s">
         <v>29</v>
       </c>
-      <c r="P391" s="109"/>
+      <c r="P391" s="139"/>
     </row>
     <row r="392" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C392" s="107"/>
-      <c r="D392" s="107"/>
-      <c r="E392" s="107"/>
-      <c r="F392" s="107"/>
-      <c r="G392" s="107"/>
-      <c r="H392" s="107"/>
-      <c r="I392" s="107"/>
+      <c r="C392" s="138"/>
+      <c r="D392" s="138"/>
+      <c r="E392" s="138"/>
+      <c r="F392" s="138"/>
+      <c r="G392" s="138"/>
+      <c r="H392" s="138"/>
+      <c r="I392" s="138"/>
       <c r="J392" s="47"/>
       <c r="K392" s="48"/>
       <c r="L392" s="49"/>
       <c r="M392" s="49"/>
       <c r="N392" s="47"/>
-      <c r="O392" s="107"/>
-      <c r="P392" s="107"/>
+      <c r="O392" s="138"/>
+      <c r="P392" s="138"/>
     </row>
     <row r="393" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C393" s="108"/>
-      <c r="D393" s="108"/>
-      <c r="E393" s="108"/>
-      <c r="F393" s="108"/>
-      <c r="G393" s="108"/>
-      <c r="H393" s="108"/>
-      <c r="I393" s="108"/>
+      <c r="C393" s="127"/>
+      <c r="D393" s="127"/>
+      <c r="E393" s="127"/>
+      <c r="F393" s="127"/>
+      <c r="G393" s="127"/>
+      <c r="H393" s="127"/>
+      <c r="I393" s="127"/>
       <c r="J393" s="46"/>
       <c r="K393" s="50"/>
       <c r="L393" s="51"/>
       <c r="M393" s="51"/>
       <c r="N393" s="46"/>
-      <c r="O393" s="108"/>
-      <c r="P393" s="108"/>
+      <c r="O393" s="127"/>
+      <c r="P393" s="127"/>
     </row>
     <row r="394" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C394" s="107"/>
-      <c r="D394" s="107"/>
-      <c r="E394" s="107"/>
-      <c r="F394" s="107"/>
-      <c r="G394" s="107"/>
-      <c r="H394" s="107"/>
-      <c r="I394" s="107"/>
+      <c r="C394" s="138"/>
+      <c r="D394" s="138"/>
+      <c r="E394" s="138"/>
+      <c r="F394" s="138"/>
+      <c r="G394" s="138"/>
+      <c r="H394" s="138"/>
+      <c r="I394" s="138"/>
       <c r="J394" s="47"/>
       <c r="K394" s="48"/>
       <c r="L394" s="49"/>
       <c r="M394" s="49"/>
       <c r="N394" s="47"/>
-      <c r="O394" s="107"/>
-      <c r="P394" s="107"/>
+      <c r="O394" s="138"/>
+      <c r="P394" s="138"/>
     </row>
     <row r="395" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C395" s="108"/>
-      <c r="D395" s="108"/>
-      <c r="E395" s="108"/>
-      <c r="F395" s="108"/>
-      <c r="G395" s="108"/>
-      <c r="H395" s="108"/>
-      <c r="I395" s="108"/>
+      <c r="C395" s="127"/>
+      <c r="D395" s="127"/>
+      <c r="E395" s="127"/>
+      <c r="F395" s="127"/>
+      <c r="G395" s="127"/>
+      <c r="H395" s="127"/>
+      <c r="I395" s="127"/>
       <c r="J395" s="46"/>
       <c r="K395" s="50"/>
       <c r="L395" s="51"/>
       <c r="M395" s="51"/>
       <c r="N395" s="46"/>
-      <c r="O395" s="108"/>
-      <c r="P395" s="108"/>
+      <c r="O395" s="127"/>
+      <c r="P395" s="127"/>
     </row>
     <row r="396" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C396" s="107"/>
-      <c r="D396" s="107"/>
-      <c r="E396" s="107"/>
-      <c r="F396" s="107"/>
-      <c r="G396" s="107"/>
-      <c r="H396" s="107"/>
-      <c r="I396" s="107"/>
+      <c r="C396" s="138"/>
+      <c r="D396" s="138"/>
+      <c r="E396" s="138"/>
+      <c r="F396" s="138"/>
+      <c r="G396" s="138"/>
+      <c r="H396" s="138"/>
+      <c r="I396" s="138"/>
       <c r="J396" s="47"/>
       <c r="K396" s="48"/>
       <c r="L396" s="49"/>
       <c r="M396" s="49"/>
       <c r="N396" s="47"/>
-      <c r="O396" s="107"/>
-      <c r="P396" s="107"/>
+      <c r="O396" s="138"/>
+      <c r="P396" s="138"/>
     </row>
     <row r="397" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C397" s="104"/>
-      <c r="D397" s="104"/>
-      <c r="E397" s="104"/>
-      <c r="F397" s="104"/>
-      <c r="G397" s="104"/>
-      <c r="H397" s="104"/>
-      <c r="I397" s="104"/>
+      <c r="C397" s="135"/>
+      <c r="D397" s="135"/>
+      <c r="E397" s="135"/>
+      <c r="F397" s="135"/>
+      <c r="G397" s="135"/>
+      <c r="H397" s="135"/>
+      <c r="I397" s="135"/>
       <c r="J397" s="55"/>
       <c r="K397" s="56"/>
       <c r="L397" s="57"/>
       <c r="M397" s="57"/>
       <c r="N397" s="55"/>
-      <c r="O397" s="104"/>
-      <c r="P397" s="104"/>
+      <c r="O397" s="135"/>
+      <c r="P397" s="135"/>
     </row>
     <row r="398" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C398" s="103"/>
-      <c r="D398" s="103"/>
-      <c r="E398" s="103"/>
-      <c r="F398" s="103"/>
-      <c r="G398" s="103"/>
-      <c r="H398" s="103"/>
-      <c r="I398" s="103"/>
+      <c r="C398" s="140"/>
+      <c r="D398" s="140"/>
+      <c r="E398" s="140"/>
+      <c r="F398" s="140"/>
+      <c r="G398" s="140"/>
+      <c r="H398" s="140"/>
+      <c r="I398" s="140"/>
       <c r="J398" s="58"/>
       <c r="K398" s="59"/>
       <c r="L398" s="60"/>
       <c r="M398" s="60"/>
       <c r="N398" s="58"/>
-      <c r="O398" s="103"/>
-      <c r="P398" s="103"/>
+      <c r="O398" s="140"/>
+      <c r="P398" s="140"/>
     </row>
     <row r="399" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C399" s="104"/>
-      <c r="D399" s="104"/>
-      <c r="E399" s="104"/>
-      <c r="F399" s="104"/>
-      <c r="G399" s="104"/>
-      <c r="H399" s="104"/>
-      <c r="I399" s="104"/>
+      <c r="C399" s="135"/>
+      <c r="D399" s="135"/>
+      <c r="E399" s="135"/>
+      <c r="F399" s="135"/>
+      <c r="G399" s="135"/>
+      <c r="H399" s="135"/>
+      <c r="I399" s="135"/>
       <c r="J399" s="55"/>
       <c r="K399" s="56"/>
       <c r="L399" s="57"/>
       <c r="M399" s="57"/>
       <c r="N399" s="55"/>
-      <c r="O399" s="104"/>
-      <c r="P399" s="104"/>
+      <c r="O399" s="135"/>
+      <c r="P399" s="135"/>
     </row>
     <row r="400" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C400" s="103"/>
-      <c r="D400" s="103"/>
-      <c r="E400" s="103"/>
-      <c r="F400" s="103"/>
-      <c r="G400" s="103"/>
-      <c r="H400" s="103"/>
-      <c r="I400" s="103"/>
+      <c r="C400" s="140"/>
+      <c r="D400" s="140"/>
+      <c r="E400" s="140"/>
+      <c r="F400" s="140"/>
+      <c r="G400" s="140"/>
+      <c r="H400" s="140"/>
+      <c r="I400" s="140"/>
       <c r="J400" s="58"/>
       <c r="K400" s="59"/>
       <c r="L400" s="60"/>
       <c r="M400" s="60"/>
       <c r="N400" s="58"/>
-      <c r="O400" s="103"/>
-      <c r="P400" s="103"/>
+      <c r="O400" s="140"/>
+      <c r="P400" s="140"/>
     </row>
     <row r="401" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C401" s="104"/>
-      <c r="D401" s="104"/>
-      <c r="E401" s="104"/>
-      <c r="F401" s="104"/>
-      <c r="G401" s="104"/>
-      <c r="H401" s="104"/>
-      <c r="I401" s="104"/>
+      <c r="C401" s="135"/>
+      <c r="D401" s="135"/>
+      <c r="E401" s="135"/>
+      <c r="F401" s="135"/>
+      <c r="G401" s="135"/>
+      <c r="H401" s="135"/>
+      <c r="I401" s="135"/>
       <c r="J401" s="55"/>
       <c r="K401" s="56"/>
       <c r="L401" s="57"/>
       <c r="M401" s="57"/>
       <c r="N401" s="55"/>
-      <c r="O401" s="104"/>
-      <c r="P401" s="104"/>
+      <c r="O401" s="135"/>
+      <c r="P401" s="135"/>
     </row>
     <row r="402" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C402" s="101"/>
-      <c r="D402" s="101"/>
-      <c r="E402" s="101"/>
-      <c r="F402" s="101"/>
-      <c r="G402" s="101"/>
-      <c r="H402" s="101"/>
-      <c r="I402" s="101"/>
+      <c r="C402" s="136"/>
+      <c r="D402" s="136"/>
+      <c r="E402" s="136"/>
+      <c r="F402" s="136"/>
+      <c r="G402" s="136"/>
+      <c r="H402" s="136"/>
+      <c r="I402" s="136"/>
       <c r="J402" s="64"/>
       <c r="K402" s="65"/>
       <c r="L402" s="66"/>
       <c r="M402" s="66"/>
       <c r="N402" s="64"/>
-      <c r="O402" s="101"/>
-      <c r="P402" s="101"/>
+      <c r="O402" s="136"/>
+      <c r="P402" s="136"/>
     </row>
     <row r="403" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C403" s="105"/>
-      <c r="D403" s="105"/>
-      <c r="E403" s="105"/>
-      <c r="F403" s="105"/>
-      <c r="G403" s="105"/>
-      <c r="H403" s="105"/>
-      <c r="I403" s="105"/>
+      <c r="C403" s="137"/>
+      <c r="D403" s="137"/>
+      <c r="E403" s="137"/>
+      <c r="F403" s="137"/>
+      <c r="G403" s="137"/>
+      <c r="H403" s="137"/>
+      <c r="I403" s="137"/>
       <c r="J403" s="61"/>
       <c r="K403" s="62"/>
       <c r="L403" s="63"/>
       <c r="M403" s="63"/>
       <c r="N403" s="61"/>
-      <c r="O403" s="105"/>
-      <c r="P403" s="105"/>
+      <c r="O403" s="137"/>
+      <c r="P403" s="137"/>
     </row>
     <row r="404" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C404" s="101"/>
-      <c r="D404" s="101"/>
-      <c r="E404" s="101"/>
-      <c r="F404" s="101"/>
-      <c r="G404" s="101"/>
-      <c r="H404" s="101"/>
-      <c r="I404" s="101"/>
+      <c r="C404" s="136"/>
+      <c r="D404" s="136"/>
+      <c r="E404" s="136"/>
+      <c r="F404" s="136"/>
+      <c r="G404" s="136"/>
+      <c r="H404" s="136"/>
+      <c r="I404" s="136"/>
       <c r="J404" s="64"/>
       <c r="K404" s="65"/>
       <c r="L404" s="66"/>
       <c r="M404" s="66"/>
       <c r="N404" s="64"/>
-      <c r="O404" s="101"/>
-      <c r="P404" s="101"/>
+      <c r="O404" s="136"/>
+      <c r="P404" s="136"/>
     </row>
     <row r="405" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C405" s="105"/>
-      <c r="D405" s="105"/>
-      <c r="E405" s="105"/>
-      <c r="F405" s="105"/>
-      <c r="G405" s="105"/>
-      <c r="H405" s="105"/>
-      <c r="I405" s="105"/>
+      <c r="C405" s="137"/>
+      <c r="D405" s="137"/>
+      <c r="E405" s="137"/>
+      <c r="F405" s="137"/>
+      <c r="G405" s="137"/>
+      <c r="H405" s="137"/>
+      <c r="I405" s="137"/>
       <c r="J405" s="61"/>
       <c r="K405" s="62"/>
       <c r="L405" s="63"/>
       <c r="M405" s="63"/>
       <c r="N405" s="61"/>
-      <c r="O405" s="105"/>
-      <c r="P405" s="105"/>
+      <c r="O405" s="137"/>
+      <c r="P405" s="137"/>
     </row>
     <row r="406" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C406" s="101"/>
-      <c r="D406" s="101"/>
-      <c r="E406" s="101"/>
-      <c r="F406" s="101"/>
-      <c r="G406" s="101"/>
-      <c r="H406" s="101"/>
-      <c r="I406" s="101"/>
+      <c r="C406" s="136"/>
+      <c r="D406" s="136"/>
+      <c r="E406" s="136"/>
+      <c r="F406" s="136"/>
+      <c r="G406" s="136"/>
+      <c r="H406" s="136"/>
+      <c r="I406" s="136"/>
       <c r="J406" s="64"/>
       <c r="K406" s="65"/>
       <c r="L406" s="66"/>
       <c r="M406" s="66"/>
       <c r="N406" s="64"/>
-      <c r="O406" s="101"/>
-      <c r="P406" s="101"/>
+      <c r="O406" s="136"/>
+      <c r="P406" s="136"/>
     </row>
   </sheetData>
   <mergeCells count="118">
-    <mergeCell ref="O376:Q376"/>
-    <mergeCell ref="O377:Q377"/>
-    <mergeCell ref="O378:Q378"/>
-    <mergeCell ref="H370:I370"/>
-    <mergeCell ref="H371:I371"/>
-    <mergeCell ref="H372:I372"/>
-    <mergeCell ref="B370:G370"/>
-    <mergeCell ref="B371:G371"/>
-    <mergeCell ref="B372:G372"/>
-    <mergeCell ref="K124:N124"/>
-    <mergeCell ref="F105:P105"/>
-    <mergeCell ref="K110:N110"/>
-    <mergeCell ref="K116:N116"/>
-    <mergeCell ref="K113:N113"/>
-    <mergeCell ref="K120:N120"/>
-    <mergeCell ref="I128:N128"/>
-    <mergeCell ref="F137:G137"/>
-    <mergeCell ref="F138:G138"/>
-    <mergeCell ref="H137:J137"/>
-    <mergeCell ref="H138:J138"/>
-    <mergeCell ref="K137:L137"/>
-    <mergeCell ref="K138:L138"/>
+    <mergeCell ref="C406:E406"/>
+    <mergeCell ref="F406:I406"/>
+    <mergeCell ref="O406:P406"/>
+    <mergeCell ref="G388:L388"/>
+    <mergeCell ref="C400:E400"/>
+    <mergeCell ref="F400:I400"/>
+    <mergeCell ref="O400:P400"/>
+    <mergeCell ref="C401:E401"/>
+    <mergeCell ref="F401:I401"/>
+    <mergeCell ref="O401:P401"/>
+    <mergeCell ref="C402:E402"/>
+    <mergeCell ref="F402:I402"/>
+    <mergeCell ref="O402:P402"/>
+    <mergeCell ref="C398:E398"/>
+    <mergeCell ref="F398:I398"/>
+    <mergeCell ref="O398:P398"/>
+    <mergeCell ref="C399:E399"/>
+    <mergeCell ref="F399:I399"/>
+    <mergeCell ref="O399:P399"/>
+    <mergeCell ref="C403:E403"/>
+    <mergeCell ref="F403:I403"/>
+    <mergeCell ref="O403:P403"/>
+    <mergeCell ref="C404:E404"/>
+    <mergeCell ref="C397:E397"/>
+    <mergeCell ref="F397:I397"/>
+    <mergeCell ref="O397:P397"/>
+    <mergeCell ref="F404:I404"/>
+    <mergeCell ref="O404:P404"/>
+    <mergeCell ref="C405:E405"/>
+    <mergeCell ref="F405:I405"/>
+    <mergeCell ref="O405:P405"/>
+    <mergeCell ref="L191:O191"/>
+    <mergeCell ref="C394:E394"/>
+    <mergeCell ref="F394:I394"/>
+    <mergeCell ref="O394:P394"/>
+    <mergeCell ref="C395:E395"/>
+    <mergeCell ref="F395:I395"/>
+    <mergeCell ref="O395:P395"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="F396:I396"/>
+    <mergeCell ref="O396:P396"/>
+    <mergeCell ref="O391:P391"/>
+    <mergeCell ref="C391:E391"/>
+    <mergeCell ref="F391:I391"/>
+    <mergeCell ref="C392:E392"/>
+    <mergeCell ref="F392:I392"/>
+    <mergeCell ref="O392:P392"/>
+    <mergeCell ref="C393:E393"/>
+    <mergeCell ref="F393:I393"/>
+    <mergeCell ref="O393:P393"/>
+    <mergeCell ref="I205:K205"/>
+    <mergeCell ref="F146:G146"/>
+    <mergeCell ref="F147:G147"/>
+    <mergeCell ref="F148:G148"/>
+    <mergeCell ref="F145:G145"/>
+    <mergeCell ref="F143:G143"/>
+    <mergeCell ref="F144:G144"/>
+    <mergeCell ref="D327:K327"/>
+    <mergeCell ref="D328:K328"/>
+    <mergeCell ref="G331:K331"/>
+    <mergeCell ref="K361:N361"/>
+    <mergeCell ref="B266:D266"/>
+    <mergeCell ref="G266:H266"/>
+    <mergeCell ref="B280:D280"/>
+    <mergeCell ref="G280:H280"/>
+    <mergeCell ref="B279:D279"/>
+    <mergeCell ref="G279:H279"/>
+    <mergeCell ref="G297:L297"/>
+    <mergeCell ref="F366:L366"/>
+    <mergeCell ref="K376:N376"/>
+    <mergeCell ref="K377:N377"/>
+    <mergeCell ref="K378:N378"/>
     <mergeCell ref="F141:G141"/>
     <mergeCell ref="F142:G142"/>
     <mergeCell ref="H146:K146"/>
@@ -11229,78 +11288,28 @@
     <mergeCell ref="I207:K207"/>
     <mergeCell ref="N206:P206"/>
     <mergeCell ref="N207:P207"/>
-    <mergeCell ref="F393:I393"/>
-    <mergeCell ref="O393:P393"/>
-    <mergeCell ref="I205:K205"/>
-    <mergeCell ref="F146:G146"/>
-    <mergeCell ref="F147:G147"/>
-    <mergeCell ref="F148:G148"/>
-    <mergeCell ref="F145:G145"/>
-    <mergeCell ref="F143:G143"/>
-    <mergeCell ref="F144:G144"/>
-    <mergeCell ref="D327:K327"/>
-    <mergeCell ref="D328:K328"/>
-    <mergeCell ref="G331:K331"/>
-    <mergeCell ref="K361:N361"/>
-    <mergeCell ref="B266:D266"/>
-    <mergeCell ref="G266:H266"/>
-    <mergeCell ref="B280:D280"/>
-    <mergeCell ref="G280:H280"/>
-    <mergeCell ref="B279:D279"/>
-    <mergeCell ref="G279:H279"/>
-    <mergeCell ref="G297:L297"/>
-    <mergeCell ref="F366:L366"/>
-    <mergeCell ref="K376:N376"/>
-    <mergeCell ref="K377:N377"/>
-    <mergeCell ref="K378:N378"/>
-    <mergeCell ref="F397:I397"/>
-    <mergeCell ref="O397:P397"/>
-    <mergeCell ref="F404:I404"/>
-    <mergeCell ref="O404:P404"/>
-    <mergeCell ref="C405:E405"/>
-    <mergeCell ref="F405:I405"/>
-    <mergeCell ref="O405:P405"/>
-    <mergeCell ref="L191:O191"/>
-    <mergeCell ref="C394:E394"/>
-    <mergeCell ref="F394:I394"/>
-    <mergeCell ref="O394:P394"/>
-    <mergeCell ref="C395:E395"/>
-    <mergeCell ref="F395:I395"/>
-    <mergeCell ref="O395:P395"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="F396:I396"/>
-    <mergeCell ref="O396:P396"/>
-    <mergeCell ref="O391:P391"/>
-    <mergeCell ref="C391:E391"/>
-    <mergeCell ref="F391:I391"/>
-    <mergeCell ref="C392:E392"/>
-    <mergeCell ref="F392:I392"/>
-    <mergeCell ref="O392:P392"/>
-    <mergeCell ref="C393:E393"/>
-    <mergeCell ref="C406:E406"/>
-    <mergeCell ref="F406:I406"/>
-    <mergeCell ref="O406:P406"/>
-    <mergeCell ref="G388:L388"/>
-    <mergeCell ref="C400:E400"/>
-    <mergeCell ref="F400:I400"/>
-    <mergeCell ref="O400:P400"/>
-    <mergeCell ref="C401:E401"/>
-    <mergeCell ref="F401:I401"/>
-    <mergeCell ref="O401:P401"/>
-    <mergeCell ref="C402:E402"/>
-    <mergeCell ref="F402:I402"/>
-    <mergeCell ref="O402:P402"/>
-    <mergeCell ref="C398:E398"/>
-    <mergeCell ref="F398:I398"/>
-    <mergeCell ref="O398:P398"/>
-    <mergeCell ref="C399:E399"/>
-    <mergeCell ref="F399:I399"/>
-    <mergeCell ref="O399:P399"/>
-    <mergeCell ref="C403:E403"/>
-    <mergeCell ref="F403:I403"/>
-    <mergeCell ref="O403:P403"/>
-    <mergeCell ref="C404:E404"/>
-    <mergeCell ref="C397:E397"/>
+    <mergeCell ref="K124:N124"/>
+    <mergeCell ref="F105:P105"/>
+    <mergeCell ref="K110:N110"/>
+    <mergeCell ref="K116:N116"/>
+    <mergeCell ref="K113:N113"/>
+    <mergeCell ref="K120:N120"/>
+    <mergeCell ref="I128:N128"/>
+    <mergeCell ref="F137:G137"/>
+    <mergeCell ref="F138:G138"/>
+    <mergeCell ref="H137:J137"/>
+    <mergeCell ref="H138:J138"/>
+    <mergeCell ref="K137:L137"/>
+    <mergeCell ref="K138:L138"/>
+    <mergeCell ref="O376:Q376"/>
+    <mergeCell ref="O377:Q377"/>
+    <mergeCell ref="O378:Q378"/>
+    <mergeCell ref="H370:I370"/>
+    <mergeCell ref="H371:I371"/>
+    <mergeCell ref="H372:I372"/>
+    <mergeCell ref="B370:G370"/>
+    <mergeCell ref="B371:G371"/>
+    <mergeCell ref="B372:G372"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="95" orientation="landscape" r:id="rId1"/>
@@ -11502,7 +11511,7 @@
         <v>141.0</v>
       </c>
       <c r="L2" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="M2" t="n">
         <v>30.0</v>
@@ -11540,7 +11549,7 @@
         <v>1.0</v>
       </c>
       <c r="L3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="M3" t="n">
         <v>182.0</v>
@@ -11578,7 +11587,7 @@
         <v>26.0</v>
       </c>
       <c r="L4" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="M4" t="n">
         <v>317.0</v>
@@ -11616,7 +11625,7 @@
         <v>18.0</v>
       </c>
       <c r="L5" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="M5" t="n">
         <v>77.0</v>
@@ -11654,7 +11663,7 @@
         <v>143.0</v>
       </c>
       <c r="L6" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="M6" t="n">
         <v>352.0</v>
@@ -11703,7 +11712,7 @@
         <v>121</v>
       </c>
       <c r="H8" t="n">
-        <v>6.0</v>
+        <v>7.0</v>
       </c>
       <c r="I8" t="n">
         <v>44.0</v>

</xml_diff>

<commit_message>
add ExcelMaleOfFemale, ExcelWeek, MaleOrFemale
</commit_message>
<xml_diff>
--- a/ready/report1.xlsx
+++ b/ready/report1.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17426"/>
-  <workbookPr codeName="ЭтаКнига" defaultThemeVersion="164011"/>
-  <mc:AlternateContent>
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\GitHub\analytics\template\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr codeName="ЭтаКнига"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
@@ -20,7 +15,7 @@
   <definedNames>
     <definedName name="averCostOfAvert">report!$K$138</definedName>
     <definedName name="cost">report!$F$138</definedName>
-    <definedName name="costConversation">ChanelTrafic!$AG$2</definedName>
+    <definedName name="costConversation">ChanelTrafic!$AE$2</definedName>
     <definedName name="countAdvert">report!$H$138</definedName>
     <definedName name="countConversation">ChanelTrafic!$H$2:$H$8</definedName>
     <definedName name="countGetGoals">report!$K$120</definedName>
@@ -32,19 +27,19 @@
     <definedName name="detailConversation">report!$D$64</definedName>
     <definedName name="detailVisited">report!$D$63</definedName>
     <definedName name="effecientConversation">report!$K$124</definedName>
-    <definedName name="effectConversationPer">ChanelTrafic!$AH$2</definedName>
+    <definedName name="effectConversationPer">ChanelTrafic!$AF$2</definedName>
     <definedName name="femaleConversation">report!$B$280</definedName>
     <definedName name="femaleConversationPer">report!$B$280</definedName>
     <definedName name="goal">ChanelTrafic!$E$2:$E$2</definedName>
     <definedName name="goalQuality">ChanelTrafic!$F$2:$F$2</definedName>
-    <definedName name="hoursOfDay">ChanelTrafic!$W$2:$W$25</definedName>
-    <definedName name="hoursOfDayConversation">ChanelTrafic!$Y$2:$Y$25</definedName>
-    <definedName name="hoursOfDayVisited">ChanelTrafic!$X$2:$X$25</definedName>
+    <definedName name="hoursOfDay">ChanelTrafic!$U$2:$U$25</definedName>
+    <definedName name="hoursOfDayConversation">ChanelTrafic!$W$2:$W$25</definedName>
+    <definedName name="hoursOfDayVisited">ChanelTrafic!$V$2:$V$25</definedName>
     <definedName name="itemsQualPerTabAndMob">report!$D$211</definedName>
-    <definedName name="keyHasConversationPer">ChanelTrafic!$AD$2</definedName>
-    <definedName name="keyReachGoal">ChanelTrafic!$AC$2</definedName>
-    <definedName name="keyWasClicked">ChanelTrafic!$AA$2</definedName>
-    <definedName name="keyWasNotReachGoal">ChanelTrafic!$AB$2</definedName>
+    <definedName name="keyHasConversationPer">ChanelTrafic!$AB$2</definedName>
+    <definedName name="keyReachGoal">ChanelTrafic!$AA$2</definedName>
+    <definedName name="keyWasClicked">ChanelTrafic!$Y$2</definedName>
+    <definedName name="keyWasNotReachGoal">ChanelTrafic!$Z$2</definedName>
     <definedName name="maleConversationPer">report!$G$280</definedName>
     <definedName name="maleOrFemale">ChanelTrafic!$O$2:$O$3</definedName>
     <definedName name="maleOrFemaleConverstionPer">ChanelTrafic!$Q$2:$Q$3</definedName>
@@ -53,13 +48,13 @@
     <definedName name="mobilConversationPer">report!$N$207</definedName>
     <definedName name="mobilVisited">report!$N$205</definedName>
     <definedName name="moreConversation">report!$D$32</definedName>
-    <definedName name="moreConversionDayOfWeek">ChanelTrafic!$V$2</definedName>
+    <definedName name="moreConversionDayOfWeek">report!$D$328</definedName>
     <definedName name="moreVisited">report!$D$31</definedName>
     <definedName name="pcConversation">report!$F$206</definedName>
     <definedName name="pcConversationPer">report!$F$207</definedName>
     <definedName name="pcVisited">report!$F$205</definedName>
-    <definedName name="popularDayOfWeek">ChanelTrafic!$U$2</definedName>
-    <definedName name="popularHours">ChanelTrafic!$Z$2</definedName>
+    <definedName name="popularDayOfWeek">report!$D$327</definedName>
+    <definedName name="popularHours">ChanelTrafic!$X$2</definedName>
     <definedName name="quality">ChanelTrafic!$A$2:$A$7</definedName>
     <definedName name="qualityClick">report!$K$113</definedName>
     <definedName name="qualityDetail">ChanelTrafic!$C$2:$C$7</definedName>
@@ -87,8 +82,8 @@
     <definedName name="userVisited">ChanelTrafic!$M$2:$M$6</definedName>
     <definedName name="visited">ChanelTrafic!#REF!</definedName>
     <definedName name="visitedDiv10">ChanelTrafic!$I$2:$I$8</definedName>
-    <definedName name="wasSpend">ChanelTrafic!$AE$2</definedName>
-    <definedName name="wasSpendNotReachGoal">ChanelTrafic!$AF$2</definedName>
+    <definedName name="wasSpend">ChanelTrafic!$AC$2</definedName>
+    <definedName name="wasSpendNotReachGoal">ChanelTrafic!$AD$2</definedName>
     <definedName name="whichConversationMore">report!$B$283</definedName>
     <definedName name="whoMoreOnSite">report!$B$282</definedName>
     <definedName name="yaFindAvrCostClick">report!$F$145</definedName>
@@ -108,9 +103,9 @@
     <definedName name="yaNetGetGoal">report!$L$146</definedName>
     <definedName name="yaNetShow">report!$L$142</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -118,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="180">
   <si>
     <t>quality</t>
   </si>
@@ -616,17 +611,59 @@
   </si>
   <si>
     <t>Нет конверсии</t>
+  </si>
+  <si>
+    <t>мужской</t>
+  </si>
+  <si>
+    <t>женский</t>
+  </si>
+  <si>
+    <t>На сайте больше женщин</t>
+  </si>
+  <si>
+    <t>Коэф. конверсии выше у женщин</t>
+  </si>
+  <si>
+    <t>�</t>
+  </si>
+  <si>
+    <t>Пятница</t>
+  </si>
+  <si>
+    <t>Понедельник</t>
+  </si>
+  <si>
+    <t>Вторник</t>
+  </si>
+  <si>
+    <t>Среда</t>
+  </si>
+  <si>
+    <t>Четверг</t>
+  </si>
+  <si>
+    <t>Суббота</t>
+  </si>
+  <si>
+    <t>Воскресенье</t>
+  </si>
+  <si>
+    <t>Коэф. конверсий выше в Пятница</t>
+  </si>
+  <si>
+    <t>Сеансов больше в Среда</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
-    <numFmt numFmtId="164" formatCode="_-* #,##0.00&quot;р.&quot;_-;\-* #,##0.00&quot;р.&quot;_-;_-* &quot;-&quot;??&quot;р.&quot;_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
-    <numFmt numFmtId="167" formatCode="#,##0.00&quot;р.&quot;"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_р_._-;\-* #,##0.00_р_._-;_-* &quot;-&quot;??_р_._-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00&quot;р.&quot;_-;\-* #,##0.00&quot;р.&quot;_-;_-* &quot;-&quot;??&quot;р.&quot;_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00&quot;р.&quot;"/>
   </numFmts>
   <fonts count="16" x14ac:knownFonts="1">
     <font>
@@ -927,11 +964,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="147">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -956,7 +993,7 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="167" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1086,7 +1123,7 @@
     <xf numFmtId="1" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1104,7 +1141,7 @@
     <xf numFmtId="1" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1135,7 +1172,7 @@
     <xf numFmtId="1" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1149,10 +1186,103 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="2" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="10" fillId="4" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1172,102 +1302,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="9" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="10" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1304,7 +1338,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -1358,23 +1392,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx2"/>
-              </a:solidFill>
-              <a:latin typeface="+mj-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1422,7 +1439,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000004-AA7C-4F56-B0BD-6A18C5CDB58F}"/>
               </c:ext>
@@ -1463,7 +1480,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-AA7C-4F56-B0BD-6A18C5CDB58F}"/>
               </c:ext>
@@ -1504,7 +1521,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000005-AA7C-4F56-B0BD-6A18C5CDB58F}"/>
               </c:ext>
@@ -1545,7 +1562,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000007-63C9-44E4-A4B2-57FCDFD4273E}"/>
               </c:ext>
@@ -1586,7 +1603,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000009-63C9-44E4-A4B2-57FCDFD4273E}"/>
               </c:ext>
@@ -1627,7 +1644,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{0000000B-63C9-44E4-A4B2-57FCDFD4273E}"/>
               </c:ext>
@@ -1680,7 +1697,7 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -1702,7 +1719,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-AA7C-4F56-B0BD-6A18C5CDB58F}"/>
             </c:ext>
@@ -1798,7 +1815,7 @@
 </file>
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -1840,7 +1857,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1855,7 +1872,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-502B-4C03-A6BF-71561E7105D5}"/>
             </c:ext>
@@ -1883,7 +1900,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1898,7 +1915,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-502B-4C03-A6BF-71561E7105D5}"/>
             </c:ext>
@@ -1926,7 +1943,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -1941,7 +1958,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-502B-4C03-A6BF-71561E7105D5}"/>
             </c:ext>
@@ -1956,11 +1973,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="133063040"/>
-        <c:axId val="133064576"/>
+        <c:axId val="127053184"/>
+        <c:axId val="127059072"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133063040"/>
+        <c:axId val="127053184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1969,7 +1986,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133064576"/>
+        <c:crossAx val="127059072"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1977,7 +1994,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133064576"/>
+        <c:axId val="127059072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1998,7 +2015,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133063040"/>
+        <c:crossAx val="127053184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2047,7 +2064,7 @@
 </file>
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -2089,7 +2106,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -2112,7 +2129,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-7F08-4288-8CAF-44F2095103FB}"/>
             </c:ext>
@@ -2140,7 +2157,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -2163,7 +2180,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-7F08-4288-8CAF-44F2095103FB}"/>
             </c:ext>
@@ -2191,7 +2208,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -2214,7 +2231,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-7F08-4288-8CAF-44F2095103FB}"/>
             </c:ext>
@@ -2229,11 +2246,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="133096960"/>
-        <c:axId val="133098496"/>
+        <c:axId val="127095552"/>
+        <c:axId val="127097088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="133096960"/>
+        <c:axId val="127095552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2243,7 +2260,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133098496"/>
+        <c:crossAx val="127097088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2251,7 +2268,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133098496"/>
+        <c:axId val="127097088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2261,7 +2278,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133096960"/>
+        <c:crossAx val="127095552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2300,7 +2317,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -2347,26 +2364,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2416,7 +2413,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1FE8-4CC8-A3E6-CD574745982A}"/>
             </c:ext>
@@ -2431,11 +2428,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="182"/>
-        <c:axId val="96605696"/>
-        <c:axId val="96607232"/>
+        <c:axId val="98371072"/>
+        <c:axId val="98372608"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="96605696"/>
+        <c:axId val="98371072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2478,7 +2475,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96607232"/>
+        <c:crossAx val="98372608"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2486,7 +2483,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96607232"/>
+        <c:axId val="98372608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2532,7 +2529,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96605696"/>
+        <c:crossAx val="98371072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2577,7 +2574,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -2646,7 +2643,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000001-5B18-40B8-9E6F-B2250215750F}"/>
               </c:ext>
@@ -2666,7 +2663,7 @@
               </a:ln>
               <a:effectLst/>
             </c:spPr>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000003-5B18-40B8-9E6F-B2250215750F}"/>
               </c:ext>
@@ -2723,7 +2720,7 @@
                 <a:effectLst/>
               </c:spPr>
             </c:leaderLines>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -2745,7 +2742,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-5B18-40B8-9E6F-B2250215750F}"/>
             </c:ext>
@@ -2834,7 +2831,7 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -2886,26 +2883,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2948,7 +2925,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-6DCE-4170-A8BA-4BE124766687}"/>
             </c:ext>
@@ -3007,7 +2984,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="1"/>
                 <c15:leaderLines>
@@ -3060,7 +3037,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-6DCE-4170-A8BA-4BE124766687}"/>
             </c:ext>
@@ -3076,11 +3053,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="96660096"/>
-        <c:axId val="96661888"/>
+        <c:axId val="99708928"/>
+        <c:axId val="99710464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="96660096"/>
+        <c:axId val="99708928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3123,7 +3100,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96661888"/>
+        <c:crossAx val="99710464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3131,7 +3108,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96661888"/>
+        <c:axId val="99710464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3182,7 +3159,7 @@
             <a:endParaRPr lang="ru-RU"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96660096"/>
+        <c:crossAx val="99708928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3258,7 +3235,7 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3295,7 +3272,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -3317,7 +3294,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-9533-424E-9DFF-B9454BE51E98}"/>
             </c:ext>
@@ -3369,7 +3346,7 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3421,7 +3398,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -3445,7 +3422,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1C8B-4851-BE55-E5C0FF949603}"/>
             </c:ext>
@@ -3483,7 +3460,7 @@
             <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="0"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:showLeaderLines val="0"/>
               </c:ext>
@@ -3507,7 +3484,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1C8B-4851-BE55-E5C0FF949603}"/>
             </c:ext>
@@ -3522,11 +3499,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="132593536"/>
-        <c:axId val="132595072"/>
+        <c:axId val="120778752"/>
+        <c:axId val="120780288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="132593536"/>
+        <c:axId val="120778752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3536,7 +3513,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132595072"/>
+        <c:crossAx val="120780288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3544,7 +3521,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="132595072"/>
+        <c:axId val="120780288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3555,7 +3532,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="132593536"/>
+        <c:crossAx val="120778752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3577,7 +3554,7 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3597,9 +3574,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr b="0">
-                <a:latin typeface="+mj-lt"/>
-              </a:defRPr>
+              <a:defRPr/>
             </a:pPr>
             <a:r>
               <a:rPr lang="ru-RU" b="0">
@@ -3610,7 +3585,7 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:overlay val="0"/>
+      <c:overlay val="1"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -3624,7 +3599,7 @@
             <c:idx val="0"/>
             <c:bubble3D val="0"/>
             <c:explosion val="6"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                 <c16:uniqueId val="{00000000-1576-4393-8E4F-7B3A075ADDFE}"/>
               </c:ext>
@@ -3639,13 +3614,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
+            <c:showVal val="1"/>
             <c:showCatName val="1"/>
             <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
+            <c:showPercent val="0"/>
             <c:showBubbleSize val="0"/>
             <c:showLeaderLines val="1"/>
-            <c:extLst>
+            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
             </c:extLst>
           </c:dLbls>
@@ -3660,14 +3635,14 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ChanelTrafic!$P$2:$P$3</c:f>
+              <c:f>[0]!maleOrFemaleVisited</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1576-4393-8E4F-7B3A075ADDFE}"/>
             </c:ext>
@@ -3675,10 +3650,10 @@
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="1"/>
           <c:showSerName val="0"/>
-          <c:showPercent val="1"/>
+          <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
           <c:showLeaderLines val="1"/>
         </c:dLbls>
@@ -3703,7 +3678,7 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3746,7 +3721,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3EA3-48D1-8E98-DC97D53A6E0F}"/>
             </c:ext>
@@ -3776,7 +3751,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3EA3-48D1-8E98-DC97D53A6E0F}"/>
             </c:ext>
@@ -3790,11 +3765,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133451776"/>
-        <c:axId val="133453312"/>
+        <c:axId val="126711680"/>
+        <c:axId val="126713216"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="133451776"/>
+        <c:axId val="126711680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3804,7 +3779,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133453312"/>
+        <c:crossAx val="126713216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3812,7 +3787,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133453312"/>
+        <c:axId val="126713216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3823,13 +3798,14 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133451776"/>
+        <c:crossAx val="126711680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="t"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3862,7 +3838,7 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
   <c:roundedCorners val="0"/>
@@ -3896,7 +3872,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-5324-4B7B-AB47-40E0FE10B1A4}"/>
             </c:ext>
@@ -3917,7 +3893,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-5324-4B7B-AB47-40E0FE10B1A4}"/>
             </c:ext>
@@ -3931,11 +3907,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133475712"/>
-        <c:axId val="133481600"/>
+        <c:axId val="126729216"/>
+        <c:axId val="127009536"/>
       </c:areaChart>
       <c:catAx>
-        <c:axId val="133475712"/>
+        <c:axId val="126729216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3944,7 +3920,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133481600"/>
+        <c:crossAx val="127009536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3952,7 +3928,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="133481600"/>
+        <c:axId val="127009536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3963,13 +3939,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133475712"/>
+        <c:crossAx val="126729216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -7353,6 +7330,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{AFF118AE-0192-452D-9AB7-AD9749DBEBF5}" type="pres">
       <dgm:prSet presAssocID="{D0B5C048-8C24-4F76-8C9D-7762D594F997}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7362,6 +7346,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{79388EF3-A8BE-4117-ACBA-8A08FF47472A}" type="pres">
       <dgm:prSet presAssocID="{A43066EC-58A2-4A7D-AF6B-37D46EA26464}" presName="Name8" presStyleCnt="0"/>
@@ -7375,6 +7366,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{673D1501-484B-4334-879E-3653F69F415A}" type="pres">
       <dgm:prSet presAssocID="{A43066EC-58A2-4A7D-AF6B-37D46EA26464}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7384,6 +7382,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{47D67E14-1695-4B93-9EB1-4CC623CC53C2}" type="pres">
       <dgm:prSet presAssocID="{93154AA3-294E-4A72-A452-A70CA494AC1C}" presName="Name8" presStyleCnt="0"/>
@@ -7397,6 +7402,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{E32FEE9D-FC56-4633-B235-BB4BC8FB2096}" type="pres">
       <dgm:prSet presAssocID="{93154AA3-294E-4A72-A452-A70CA494AC1C}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7406,6 +7418,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{8AAD1D77-9DFF-4406-995B-9E373EE560D6}" type="pres">
       <dgm:prSet presAssocID="{6F6CEB40-F018-40B7-B43C-BB0F608C1737}" presName="Name8" presStyleCnt="0"/>
@@ -7419,6 +7438,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{166B6DC3-E48C-470D-B319-D777F3D4DA8C}" type="pres">
       <dgm:prSet presAssocID="{6F6CEB40-F018-40B7-B43C-BB0F608C1737}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7428,6 +7454,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{7A3E38AC-ABE0-44B1-ABFE-C71AA69B5E79}" type="pres">
       <dgm:prSet presAssocID="{DFB816DE-9FE1-4A03-BBE3-E92EDD0106A3}" presName="Name8" presStyleCnt="0"/>
@@ -7441,6 +7474,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{53E7FBCA-B0EF-4CD3-9E52-80F3A839A7EA}" type="pres">
       <dgm:prSet presAssocID="{DFB816DE-9FE1-4A03-BBE3-E92EDD0106A3}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7450,6 +7490,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{40A0CFF3-5D9A-46B0-B3E9-C705D72172EE}" type="pres">
       <dgm:prSet presAssocID="{9672259E-8D62-4911-A026-2E23FD52D48A}" presName="Name8" presStyleCnt="0"/>
@@ -7463,6 +7510,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
     <dgm:pt modelId="{22C6AEA5-B4B3-41C7-AE03-AA0A4D4EB3BF}" type="pres">
       <dgm:prSet presAssocID="{9672259E-8D62-4911-A026-2E23FD52D48A}" presName="levelTx" presStyleLbl="revTx" presStyleIdx="0" presStyleCnt="0">
@@ -7472,6 +7526,13 @@
         </dgm:presLayoutVars>
       </dgm:prSet>
       <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </dgm:t>
     </dgm:pt>
   </dgm:ptLst>
   <dgm:cxnLst>
@@ -7539,7 +7600,7 @@
       <dsp:spPr>
         <a:xfrm rot="10800000">
           <a:off x="0" y="217155"/>
-          <a:ext cx="4721039" cy="836627"/>
+          <a:ext cx="4721038" cy="836627"/>
         </a:xfrm>
         <a:prstGeom prst="trapezoid">
           <a:avLst>
@@ -7589,7 +7650,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
+          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7599,7 +7660,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="ru-RU" sz="2000" kern="1200">
@@ -7677,7 +7737,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
+          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7687,7 +7747,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="ru-RU" sz="2000" kern="1200">
@@ -7765,7 +7824,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
+          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7775,7 +7834,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="ru-RU" sz="2000" kern="1200">
@@ -7853,7 +7911,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
+          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7863,7 +7921,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="ru-RU" sz="2000" kern="1200">
@@ -7941,7 +7998,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
+          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -7951,7 +8008,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="ru-RU" sz="2000" kern="1200">
@@ -8026,7 +8082,7 @@
         </a:bodyPr>
         <a:lstStyle/>
         <a:p>
-          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="889000">
+          <a:pPr lvl="0" algn="ctr" defTabSz="889000">
             <a:lnSpc>
               <a:spcPct val="90000"/>
             </a:lnSpc>
@@ -8036,7 +8092,6 @@
             <a:spcAft>
               <a:spcPct val="35000"/>
             </a:spcAft>
-            <a:buNone/>
           </a:pPr>
           <a:r>
             <a:rPr lang="en-US" sz="2000" kern="1200">
@@ -9606,7 +9661,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>493058</xdr:colOff>
+      <xdr:colOff>381000</xdr:colOff>
       <xdr:row>280</xdr:row>
       <xdr:rowOff>134472</xdr:rowOff>
     </xdr:to>
@@ -10090,8 +10145,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="B1:U406"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A196" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="I210" sqref="I210"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A308" zoomScale="70" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D328" sqref="D328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10142,52 +10197,52 @@
     </row>
     <row r="104" spans="6:16" ht="39.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="105" spans="6:16" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="F105" s="110" t="s">
+      <c r="F105" s="125" t="s">
         <v>22</v>
       </c>
-      <c r="G105" s="110"/>
-      <c r="H105" s="110"/>
-      <c r="I105" s="110"/>
-      <c r="J105" s="110"/>
-      <c r="K105" s="110"/>
-      <c r="L105" s="110"/>
-      <c r="M105" s="110"/>
-      <c r="N105" s="110"/>
-      <c r="O105" s="110"/>
-      <c r="P105" s="110"/>
+      <c r="G105" s="125"/>
+      <c r="H105" s="125"/>
+      <c r="I105" s="125"/>
+      <c r="J105" s="125"/>
+      <c r="K105" s="125"/>
+      <c r="L105" s="125"/>
+      <c r="M105" s="125"/>
+      <c r="N105" s="125"/>
+      <c r="O105" s="125"/>
+      <c r="P105" s="125"/>
     </row>
     <row r="106" spans="6:16" ht="26.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="110" spans="6:16" ht="21" x14ac:dyDescent="0.35">
       <c r="K110" s="96" t="s">
         <v>122</v>
       </c>
-      <c r="L110" s="111"/>
-      <c r="M110" s="111"/>
-      <c r="N110" s="111"/>
+      <c r="L110" s="126"/>
+      <c r="M110" s="126"/>
+      <c r="N110" s="126"/>
     </row>
     <row r="113" spans="9:14" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K113" s="96" t="s">
         <v>123</v>
       </c>
-      <c r="L113" s="111"/>
-      <c r="M113" s="111"/>
-      <c r="N113" s="111"/>
+      <c r="L113" s="126"/>
+      <c r="M113" s="126"/>
+      <c r="N113" s="126"/>
     </row>
     <row r="116" spans="9:14" ht="21" x14ac:dyDescent="0.35">
       <c r="K116" s="96" t="s">
         <v>124</v>
       </c>
-      <c r="L116" s="112"/>
-      <c r="M116" s="112"/>
-      <c r="N116" s="112"/>
+      <c r="L116" s="127"/>
+      <c r="M116" s="127"/>
+      <c r="N116" s="127"/>
     </row>
     <row r="120" spans="9:14" ht="21" x14ac:dyDescent="0.35">
       <c r="K120" s="96" t="s">
         <v>125</v>
       </c>
-      <c r="L120" s="111"/>
-      <c r="M120" s="111"/>
-      <c r="N120" s="111"/>
+      <c r="L120" s="126"/>
+      <c r="M120" s="126"/>
+      <c r="N120" s="126"/>
     </row>
     <row r="124" spans="9:14" ht="21" x14ac:dyDescent="0.35">
       <c r="I124" s="19"/>
@@ -10195,20 +10250,20 @@
       <c r="K124" s="96" t="s">
         <v>126</v>
       </c>
-      <c r="L124" s="109"/>
-      <c r="M124" s="109"/>
-      <c r="N124" s="109"/>
+      <c r="L124" s="124"/>
+      <c r="M124" s="124"/>
+      <c r="N124" s="124"/>
     </row>
     <row r="127" spans="9:14" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="128" spans="9:14" ht="21" x14ac:dyDescent="0.35">
       <c r="I128" s="96" t="s">
         <v>127</v>
       </c>
-      <c r="J128" s="113"/>
-      <c r="K128" s="113"/>
-      <c r="L128" s="113"/>
-      <c r="M128" s="113"/>
-      <c r="N128" s="113"/>
+      <c r="J128" s="128"/>
+      <c r="K128" s="128"/>
+      <c r="L128" s="128"/>
+      <c r="M128" s="128"/>
+      <c r="N128" s="128"/>
     </row>
     <row r="129" spans="6:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K129" s="16"/>
@@ -10217,35 +10272,35 @@
     </row>
     <row r="134" spans="6:13" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="137" spans="6:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F137" s="114" t="s">
+      <c r="F137" s="129" t="s">
         <v>23</v>
       </c>
-      <c r="G137" s="114"/>
-      <c r="H137" s="116" t="s">
+      <c r="G137" s="129"/>
+      <c r="H137" s="130" t="s">
         <v>24</v>
       </c>
-      <c r="I137" s="116"/>
-      <c r="J137" s="116"/>
-      <c r="K137" s="114" t="s">
+      <c r="I137" s="130"/>
+      <c r="J137" s="130"/>
+      <c r="K137" s="129" t="s">
         <v>25</v>
       </c>
-      <c r="L137" s="114"/>
+      <c r="L137" s="129"/>
       <c r="M137" s="86"/>
     </row>
     <row r="138" spans="6:13" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F138" s="84" t="s">
         <v>140</v>
       </c>
-      <c r="G138" s="115"/>
+      <c r="G138" s="119"/>
       <c r="H138" s="84" t="s">
         <v>141</v>
       </c>
-      <c r="I138" s="117"/>
-      <c r="J138" s="117"/>
+      <c r="I138" s="131"/>
+      <c r="J138" s="131"/>
       <c r="K138" s="84" t="s">
         <v>142</v>
       </c>
-      <c r="L138" s="115"/>
+      <c r="L138" s="119"/>
       <c r="M138" s="87"/>
     </row>
     <row r="139" spans="6:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10272,13 +10327,13 @@
       <c r="F141" s="72" t="s">
         <v>128</v>
       </c>
-      <c r="G141" s="118"/>
-      <c r="H141" s="115" t="s">
+      <c r="G141" s="112"/>
+      <c r="H141" s="119" t="s">
         <v>26</v>
       </c>
-      <c r="I141" s="115"/>
-      <c r="J141" s="115"/>
-      <c r="K141" s="115"/>
+      <c r="I141" s="119"/>
+      <c r="J141" s="119"/>
+      <c r="K141" s="119"/>
       <c r="L141" s="72" t="s">
         <v>129</v>
       </c>
@@ -10288,13 +10343,13 @@
       <c r="F142" s="84" t="s">
         <v>130</v>
       </c>
-      <c r="G142" s="119"/>
-      <c r="H142" s="120" t="s">
+      <c r="G142" s="111"/>
+      <c r="H142" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="I142" s="120"/>
-      <c r="J142" s="120"/>
-      <c r="K142" s="120"/>
+      <c r="I142" s="118"/>
+      <c r="J142" s="118"/>
+      <c r="K142" s="118"/>
       <c r="L142" s="84" t="s">
         <v>131</v>
       </c>
@@ -10304,13 +10359,13 @@
       <c r="F143" s="72" t="s">
         <v>132</v>
       </c>
-      <c r="G143" s="118"/>
-      <c r="H143" s="115" t="s">
+      <c r="G143" s="112"/>
+      <c r="H143" s="119" t="s">
         <v>28</v>
       </c>
-      <c r="I143" s="115"/>
-      <c r="J143" s="115"/>
-      <c r="K143" s="115"/>
+      <c r="I143" s="119"/>
+      <c r="J143" s="119"/>
+      <c r="K143" s="119"/>
       <c r="L143" s="72" t="s">
         <v>133</v>
       </c>
@@ -10320,13 +10375,13 @@
       <c r="F144" s="84" t="s">
         <v>134</v>
       </c>
-      <c r="G144" s="119"/>
-      <c r="H144" s="120" t="s">
+      <c r="G144" s="111"/>
+      <c r="H144" s="118" t="s">
         <v>29</v>
       </c>
-      <c r="I144" s="120"/>
-      <c r="J144" s="120"/>
-      <c r="K144" s="120"/>
+      <c r="I144" s="118"/>
+      <c r="J144" s="118"/>
+      <c r="K144" s="118"/>
       <c r="L144" s="84" t="s">
         <v>135</v>
       </c>
@@ -10336,27 +10391,27 @@
       <c r="F145" s="72" t="s">
         <v>136</v>
       </c>
-      <c r="G145" s="118"/>
-      <c r="H145" s="115" t="s">
+      <c r="G145" s="112"/>
+      <c r="H145" s="119" t="s">
         <v>30</v>
       </c>
-      <c r="I145" s="115"/>
-      <c r="J145" s="115"/>
-      <c r="K145" s="115"/>
+      <c r="I145" s="119"/>
+      <c r="J145" s="119"/>
+      <c r="K145" s="119"/>
       <c r="L145" s="72" t="s">
         <v>137</v>
       </c>
       <c r="M145" s="88"/>
     </row>
     <row r="146" spans="6:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F146" s="119"/>
-      <c r="G146" s="119"/>
-      <c r="H146" s="120" t="s">
+      <c r="F146" s="111"/>
+      <c r="G146" s="111"/>
+      <c r="H146" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="I146" s="120"/>
-      <c r="J146" s="120"/>
-      <c r="K146" s="120"/>
+      <c r="I146" s="118"/>
+      <c r="J146" s="118"/>
+      <c r="K146" s="118"/>
       <c r="L146" s="68"/>
       <c r="M146" s="88"/>
     </row>
@@ -10364,13 +10419,13 @@
       <c r="F147" s="72" t="s">
         <v>138</v>
       </c>
-      <c r="G147" s="118"/>
-      <c r="H147" s="115" t="s">
+      <c r="G147" s="112"/>
+      <c r="H147" s="119" t="s">
         <v>32</v>
       </c>
-      <c r="I147" s="115"/>
-      <c r="J147" s="115"/>
-      <c r="K147" s="115"/>
+      <c r="I147" s="119"/>
+      <c r="J147" s="119"/>
+      <c r="K147" s="119"/>
       <c r="L147" s="72" t="s">
         <v>138</v>
       </c>
@@ -10380,13 +10435,13 @@
       <c r="F148" s="84" t="s">
         <v>139</v>
       </c>
-      <c r="G148" s="119"/>
-      <c r="H148" s="120" t="s">
+      <c r="G148" s="111"/>
+      <c r="H148" s="118" t="s">
         <v>33</v>
       </c>
-      <c r="I148" s="120"/>
-      <c r="J148" s="120"/>
-      <c r="K148" s="120"/>
+      <c r="I148" s="118"/>
+      <c r="J148" s="118"/>
+      <c r="K148" s="118"/>
       <c r="L148" s="84" t="s">
         <v>139</v>
       </c>
@@ -10450,24 +10505,24 @@
       <c r="U195" s="24"/>
     </row>
     <row r="198" spans="2:21" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="E198" s="123" t="s">
+      <c r="E198" s="120" t="s">
         <v>39</v>
       </c>
-      <c r="F198" s="123"/>
-      <c r="G198" s="124"/>
+      <c r="F198" s="120"/>
+      <c r="G198" s="121"/>
       <c r="H198" s="26"/>
-      <c r="I198" s="123" t="s">
-        <v>40</v>
-      </c>
-      <c r="J198" s="123"/>
-      <c r="K198" s="125"/>
+      <c r="I198" s="120" t="s">
+        <v>38</v>
+      </c>
+      <c r="J198" s="120"/>
+      <c r="K198" s="122"/>
       <c r="L198" s="26"/>
       <c r="M198" s="26"/>
-      <c r="N198" s="123" t="s">
-        <v>38</v>
-      </c>
-      <c r="O198" s="123"/>
-      <c r="P198" s="125"/>
+      <c r="N198" s="120" t="s">
+        <v>40</v>
+      </c>
+      <c r="O198" s="120"/>
+      <c r="P198" s="122"/>
     </row>
     <row r="199" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E199" s="27"/>
@@ -10543,20 +10598,20 @@
       <c r="F205" s="97" t="s">
         <v>152</v>
       </c>
-      <c r="G205" s="122"/>
+      <c r="G205" s="110"/>
       <c r="H205" s="90"/>
       <c r="I205" s="97" t="s">
         <v>155</v>
       </c>
-      <c r="J205" s="122"/>
-      <c r="K205" s="122"/>
+      <c r="J205" s="110"/>
+      <c r="K205" s="110"/>
       <c r="L205" s="90"/>
       <c r="M205" s="90"/>
       <c r="N205" s="97" t="s">
         <v>157</v>
       </c>
-      <c r="O205" s="122"/>
-      <c r="P205" s="122"/>
+      <c r="O205" s="110"/>
+      <c r="P205" s="110"/>
     </row>
     <row r="206" spans="2:21" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D206" s="93" t="s">
@@ -10566,20 +10621,20 @@
       <c r="F206" s="96" t="s">
         <v>153</v>
       </c>
-      <c r="G206" s="126"/>
+      <c r="G206" s="123"/>
       <c r="H206" s="91"/>
       <c r="I206" s="96" t="s">
         <v>139</v>
       </c>
-      <c r="J206" s="126"/>
-      <c r="K206" s="126"/>
+      <c r="J206" s="123"/>
+      <c r="K206" s="123"/>
       <c r="L206" s="91"/>
       <c r="M206" s="91"/>
       <c r="N206" s="96" t="s">
         <v>139</v>
       </c>
-      <c r="O206" s="126"/>
-      <c r="P206" s="126"/>
+      <c r="O206" s="123"/>
+      <c r="P206" s="123"/>
     </row>
     <row r="207" spans="2:21" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D207" s="92" t="s">
@@ -10589,20 +10644,20 @@
       <c r="F207" s="97" t="s">
         <v>154</v>
       </c>
-      <c r="G207" s="122"/>
+      <c r="G207" s="110"/>
       <c r="H207" s="90"/>
       <c r="I207" s="97" t="s">
         <v>156</v>
       </c>
-      <c r="J207" s="122"/>
-      <c r="K207" s="122"/>
+      <c r="J207" s="110"/>
+      <c r="K207" s="110"/>
       <c r="L207" s="90"/>
       <c r="M207" s="90"/>
       <c r="N207" s="97" t="s">
         <v>156</v>
       </c>
-      <c r="O207" s="122"/>
-      <c r="P207" s="122"/>
+      <c r="O207" s="110"/>
+      <c r="P207" s="110"/>
     </row>
     <row r="208" spans="2:21" x14ac:dyDescent="0.25">
       <c r="E208" s="23"/>
@@ -10630,14 +10685,14 @@
       <c r="J212" s="42"/>
     </row>
     <row r="229" spans="7:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="G229" s="121" t="s">
+      <c r="G229" s="106" t="s">
         <v>50</v>
       </c>
-      <c r="H229" s="121"/>
-      <c r="I229" s="121"/>
-      <c r="J229" s="121"/>
-      <c r="K229" s="121"/>
-      <c r="L229" s="121"/>
+      <c r="H229" s="106"/>
+      <c r="I229" s="106"/>
+      <c r="J229" s="106"/>
+      <c r="K229" s="106"/>
+      <c r="L229" s="106"/>
       <c r="M229" s="25"/>
     </row>
     <row r="259" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
@@ -10661,28 +10716,28 @@
       <c r="J260" s="98"/>
     </row>
     <row r="263" spans="2:13" ht="21" x14ac:dyDescent="0.35">
-      <c r="G263" s="121" t="s">
+      <c r="G263" s="106" t="s">
         <v>44</v>
       </c>
-      <c r="H263" s="121"/>
-      <c r="I263" s="121"/>
-      <c r="J263" s="121"/>
-      <c r="K263" s="121"/>
-      <c r="L263" s="121"/>
+      <c r="H263" s="106"/>
+      <c r="I263" s="106"/>
+      <c r="J263" s="106"/>
+      <c r="K263" s="106"/>
+      <c r="L263" s="106"/>
       <c r="M263" s="25"/>
     </row>
     <row r="266" spans="2:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B266" s="130" t="s">
+      <c r="B266" s="114" t="s">
         <v>51</v>
       </c>
-      <c r="C266" s="130"/>
-      <c r="D266" s="130"/>
+      <c r="C266" s="114"/>
+      <c r="D266" s="114"/>
       <c r="E266" s="26"/>
       <c r="F266" s="26"/>
-      <c r="G266" s="130" t="s">
+      <c r="G266" s="114" t="s">
         <v>52</v>
       </c>
-      <c r="H266" s="130"/>
+      <c r="H266" s="114"/>
     </row>
     <row r="267" spans="2:13" x14ac:dyDescent="0.25">
       <c r="E267" s="37"/>
@@ -10721,80 +10776,72 @@
       <c r="E278" s="37"/>
     </row>
     <row r="279" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B279" s="131" t="s">
+      <c r="B279" s="115" t="s">
         <v>55</v>
       </c>
-      <c r="C279" s="131"/>
-      <c r="D279" s="131"/>
+      <c r="C279" s="115"/>
+      <c r="D279" s="115"/>
       <c r="E279" s="37"/>
-      <c r="G279" s="131" t="s">
+      <c r="G279" s="115" t="s">
         <v>55</v>
       </c>
-      <c r="H279" s="131"/>
+      <c r="H279" s="115"/>
     </row>
     <row r="280" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B280" s="131"/>
-      <c r="C280" s="131"/>
-      <c r="D280" s="131"/>
-      <c r="G280" s="131"/>
-      <c r="H280" s="131"/>
+      <c r="B280" s="78" t="s">
+        <v>156</v>
+      </c>
+      <c r="C280" s="115"/>
+      <c r="D280" s="115"/>
+      <c r="G280" s="78" t="s">
+        <v>170</v>
+      </c>
+      <c r="H280" s="115"/>
     </row>
     <row r="282" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B282" s="26"/>
+      <c r="B282" s="78" t="s">
+        <v>168</v>
+      </c>
       <c r="C282" s="26"/>
       <c r="D282" s="26"/>
       <c r="G282" s="26"/>
     </row>
     <row r="283" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B283" s="26"/>
+      <c r="B283" s="26" t="s">
+        <v>169</v>
+      </c>
       <c r="C283" s="26"/>
       <c r="D283" s="26"/>
       <c r="E283" s="26"/>
     </row>
     <row r="297" spans="7:12" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="G297" s="132" t="s">
+      <c r="G297" s="102" t="s">
         <v>59</v>
       </c>
-      <c r="H297" s="132"/>
-      <c r="I297" s="132"/>
-      <c r="J297" s="132"/>
-      <c r="K297" s="132"/>
-      <c r="L297" s="132"/>
-    </row>
-    <row r="327" spans="4:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="D327" s="128" t="str">
-        <f>"Сеансов больше всего по "&amp;popularDayOfWeek</f>
-        <v xml:space="preserve">Сеансов больше всего по </v>
-      </c>
-      <c r="E327" s="128"/>
-      <c r="F327" s="128"/>
-      <c r="G327" s="128"/>
-      <c r="H327" s="128"/>
-      <c r="I327" s="128"/>
-      <c r="J327" s="128"/>
-      <c r="K327" s="128"/>
-    </row>
-    <row r="328" spans="4:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="D328" s="128" t="str">
-        <f>"Коэф. конверсий выше по "&amp;moreConversionDayOfWeek</f>
-        <v xml:space="preserve">Коэф. конверсий выше по </v>
-      </c>
-      <c r="E328" s="128"/>
-      <c r="F328" s="128"/>
-      <c r="G328" s="128"/>
-      <c r="H328" s="128"/>
-      <c r="I328" s="128"/>
-      <c r="J328" s="128"/>
-      <c r="K328" s="128"/>
-    </row>
-    <row r="331" spans="4:11" ht="21" x14ac:dyDescent="0.35">
-      <c r="G331" s="121" t="s">
+      <c r="H297" s="102"/>
+      <c r="I297" s="102"/>
+      <c r="J297" s="102"/>
+      <c r="K297" s="102"/>
+      <c r="L297" s="102"/>
+    </row>
+    <row r="327">
+      <c r="D327" t="s" s="78">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="328">
+      <c r="D328" t="s" s="78">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="331" spans="4:12" ht="21" x14ac:dyDescent="0.35">
+      <c r="G331" s="106" t="s">
         <v>69</v>
       </c>
-      <c r="H331" s="121"/>
-      <c r="I331" s="121"/>
-      <c r="J331" s="121"/>
-      <c r="K331" s="121"/>
+      <c r="H331" s="106"/>
+      <c r="I331" s="106"/>
+      <c r="J331" s="106"/>
+      <c r="K331" s="106"/>
     </row>
     <row r="361" spans="4:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D361" s="26" t="s">
@@ -10804,136 +10851,136 @@
       <c r="F361" s="26"/>
       <c r="G361" s="26"/>
       <c r="H361" s="26"/>
-      <c r="K361" s="129">
+      <c r="K361" s="113">
         <f>popularHours</f>
         <v>0</v>
       </c>
-      <c r="L361" s="129"/>
-      <c r="M361" s="129"/>
-      <c r="N361" s="129"/>
+      <c r="L361" s="113"/>
+      <c r="M361" s="113"/>
+      <c r="N361" s="113"/>
     </row>
     <row r="366" spans="4:14" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="F366" s="132" t="s">
+      <c r="F366" s="102" t="s">
         <v>71</v>
       </c>
-      <c r="G366" s="132"/>
-      <c r="H366" s="132"/>
-      <c r="I366" s="132"/>
-      <c r="J366" s="132"/>
-      <c r="K366" s="132"/>
-      <c r="L366" s="132"/>
+      <c r="G366" s="102"/>
+      <c r="H366" s="102"/>
+      <c r="I366" s="102"/>
+      <c r="J366" s="102"/>
+      <c r="K366" s="102"/>
+      <c r="L366" s="102"/>
       <c r="M366" s="43"/>
     </row>
     <row r="370" spans="2:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B370" s="106" t="s">
+      <c r="B370" s="137" t="s">
         <v>72</v>
       </c>
-      <c r="C370" s="106"/>
-      <c r="D370" s="106"/>
-      <c r="E370" s="106"/>
-      <c r="F370" s="106"/>
-      <c r="G370" s="106"/>
-      <c r="H370" s="104">
+      <c r="C370" s="137"/>
+      <c r="D370" s="137"/>
+      <c r="E370" s="137"/>
+      <c r="F370" s="137"/>
+      <c r="G370" s="137"/>
+      <c r="H370" s="135">
         <f>keyWasClicked</f>
         <v>0</v>
       </c>
-      <c r="I370" s="104"/>
+      <c r="I370" s="135"/>
     </row>
     <row r="371" spans="2:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B371" s="107" t="s">
+      <c r="B371" s="138" t="s">
         <v>73</v>
       </c>
-      <c r="C371" s="107"/>
-      <c r="D371" s="107"/>
-      <c r="E371" s="107"/>
-      <c r="F371" s="107"/>
-      <c r="G371" s="107"/>
-      <c r="H371" s="105">
+      <c r="C371" s="138"/>
+      <c r="D371" s="138"/>
+      <c r="E371" s="138"/>
+      <c r="F371" s="138"/>
+      <c r="G371" s="138"/>
+      <c r="H371" s="136">
         <f>keyReachGoal</f>
         <v>0</v>
       </c>
-      <c r="I371" s="105"/>
+      <c r="I371" s="136"/>
     </row>
     <row r="372" spans="2:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B372" s="108" t="s">
+      <c r="B372" s="139" t="s">
         <v>74</v>
       </c>
-      <c r="C372" s="108"/>
-      <c r="D372" s="108"/>
-      <c r="E372" s="108"/>
-      <c r="F372" s="108"/>
-      <c r="G372" s="108"/>
-      <c r="H372" s="104">
+      <c r="C372" s="139"/>
+      <c r="D372" s="139"/>
+      <c r="E372" s="139"/>
+      <c r="F372" s="139"/>
+      <c r="G372" s="139"/>
+      <c r="H372" s="135">
         <f>keyHasConversationPer</f>
         <v>0</v>
       </c>
-      <c r="I372" s="104"/>
+      <c r="I372" s="135"/>
     </row>
     <row r="376" spans="2:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K376" s="133" t="s">
+      <c r="K376" s="116" t="s">
         <v>83</v>
       </c>
-      <c r="L376" s="133"/>
-      <c r="M376" s="133"/>
-      <c r="N376" s="133"/>
-      <c r="O376" s="101">
+      <c r="L376" s="116"/>
+      <c r="M376" s="116"/>
+      <c r="N376" s="116"/>
+      <c r="O376" s="132">
         <f>sendAll</f>
         <v>0</v>
       </c>
-      <c r="P376" s="101"/>
-      <c r="Q376" s="101"/>
+      <c r="P376" s="132"/>
+      <c r="Q376" s="132"/>
     </row>
     <row r="377" spans="2:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K377" s="134" t="s">
+      <c r="K377" s="117" t="s">
         <v>84</v>
       </c>
-      <c r="L377" s="134"/>
-      <c r="M377" s="134"/>
-      <c r="N377" s="134"/>
-      <c r="O377" s="102">
+      <c r="L377" s="117"/>
+      <c r="M377" s="117"/>
+      <c r="N377" s="117"/>
+      <c r="O377" s="133">
         <f>costConversation</f>
         <v>0</v>
       </c>
-      <c r="P377" s="102"/>
-      <c r="Q377" s="102"/>
+      <c r="P377" s="133"/>
+      <c r="Q377" s="133"/>
     </row>
     <row r="378" spans="2:17" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K378" s="133" t="s">
+      <c r="K378" s="116" t="s">
         <v>85</v>
       </c>
-      <c r="L378" s="133"/>
-      <c r="M378" s="133"/>
-      <c r="N378" s="133"/>
-      <c r="O378" s="103">
+      <c r="L378" s="116"/>
+      <c r="M378" s="116"/>
+      <c r="N378" s="116"/>
+      <c r="O378" s="134">
         <f>effecientConversation</f>
         <v>0</v>
       </c>
-      <c r="P378" s="103"/>
-      <c r="Q378" s="103"/>
+      <c r="P378" s="134"/>
+      <c r="Q378" s="134"/>
     </row>
     <row r="388" spans="3:16" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="G388" s="132" t="s">
+      <c r="G388" s="102" t="s">
         <v>86</v>
       </c>
-      <c r="H388" s="132"/>
-      <c r="I388" s="132"/>
-      <c r="J388" s="132"/>
-      <c r="K388" s="132"/>
-      <c r="L388" s="132"/>
+      <c r="H388" s="102"/>
+      <c r="I388" s="102"/>
+      <c r="J388" s="102"/>
+      <c r="K388" s="102"/>
+      <c r="L388" s="102"/>
       <c r="M388" s="43"/>
     </row>
     <row r="391" spans="3:16" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C391" s="139" t="s">
+      <c r="C391" s="109" t="s">
         <v>87</v>
       </c>
-      <c r="D391" s="139"/>
-      <c r="E391" s="139"/>
-      <c r="F391" s="139" t="s">
+      <c r="D391" s="109"/>
+      <c r="E391" s="109"/>
+      <c r="F391" s="109" t="s">
         <v>88</v>
       </c>
-      <c r="G391" s="139"/>
-      <c r="H391" s="139"/>
-      <c r="I391" s="139"/>
+      <c r="G391" s="109"/>
+      <c r="H391" s="109"/>
+      <c r="I391" s="109"/>
       <c r="J391" s="52"/>
       <c r="K391" s="53" t="s">
         <v>89</v>
@@ -10945,253 +10992,345 @@
       <c r="N391" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="O391" s="139" t="s">
+      <c r="O391" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="P391" s="139"/>
+      <c r="P391" s="109"/>
     </row>
     <row r="392" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C392" s="138"/>
-      <c r="D392" s="138"/>
-      <c r="E392" s="138"/>
-      <c r="F392" s="138"/>
-      <c r="G392" s="138"/>
-      <c r="H392" s="138"/>
-      <c r="I392" s="138"/>
+      <c r="C392" s="107"/>
+      <c r="D392" s="107"/>
+      <c r="E392" s="107"/>
+      <c r="F392" s="107"/>
+      <c r="G392" s="107"/>
+      <c r="H392" s="107"/>
+      <c r="I392" s="107"/>
       <c r="J392" s="47"/>
       <c r="K392" s="48"/>
       <c r="L392" s="49"/>
       <c r="M392" s="49"/>
       <c r="N392" s="47"/>
-      <c r="O392" s="138"/>
-      <c r="P392" s="138"/>
+      <c r="O392" s="107"/>
+      <c r="P392" s="107"/>
     </row>
     <row r="393" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C393" s="127"/>
-      <c r="D393" s="127"/>
-      <c r="E393" s="127"/>
-      <c r="F393" s="127"/>
-      <c r="G393" s="127"/>
-      <c r="H393" s="127"/>
-      <c r="I393" s="127"/>
+      <c r="C393" s="108"/>
+      <c r="D393" s="108"/>
+      <c r="E393" s="108"/>
+      <c r="F393" s="108"/>
+      <c r="G393" s="108"/>
+      <c r="H393" s="108"/>
+      <c r="I393" s="108"/>
       <c r="J393" s="46"/>
       <c r="K393" s="50"/>
       <c r="L393" s="51"/>
       <c r="M393" s="51"/>
       <c r="N393" s="46"/>
-      <c r="O393" s="127"/>
-      <c r="P393" s="127"/>
+      <c r="O393" s="108"/>
+      <c r="P393" s="108"/>
     </row>
     <row r="394" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C394" s="138"/>
-      <c r="D394" s="138"/>
-      <c r="E394" s="138"/>
-      <c r="F394" s="138"/>
-      <c r="G394" s="138"/>
-      <c r="H394" s="138"/>
-      <c r="I394" s="138"/>
+      <c r="C394" s="107"/>
+      <c r="D394" s="107"/>
+      <c r="E394" s="107"/>
+      <c r="F394" s="107"/>
+      <c r="G394" s="107"/>
+      <c r="H394" s="107"/>
+      <c r="I394" s="107"/>
       <c r="J394" s="47"/>
       <c r="K394" s="48"/>
       <c r="L394" s="49"/>
       <c r="M394" s="49"/>
       <c r="N394" s="47"/>
-      <c r="O394" s="138"/>
-      <c r="P394" s="138"/>
+      <c r="O394" s="107"/>
+      <c r="P394" s="107"/>
     </row>
     <row r="395" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C395" s="127"/>
-      <c r="D395" s="127"/>
-      <c r="E395" s="127"/>
-      <c r="F395" s="127"/>
-      <c r="G395" s="127"/>
-      <c r="H395" s="127"/>
-      <c r="I395" s="127"/>
+      <c r="C395" s="108"/>
+      <c r="D395" s="108"/>
+      <c r="E395" s="108"/>
+      <c r="F395" s="108"/>
+      <c r="G395" s="108"/>
+      <c r="H395" s="108"/>
+      <c r="I395" s="108"/>
       <c r="J395" s="46"/>
       <c r="K395" s="50"/>
       <c r="L395" s="51"/>
       <c r="M395" s="51"/>
       <c r="N395" s="46"/>
-      <c r="O395" s="127"/>
-      <c r="P395" s="127"/>
+      <c r="O395" s="108"/>
+      <c r="P395" s="108"/>
     </row>
     <row r="396" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C396" s="138"/>
-      <c r="D396" s="138"/>
-      <c r="E396" s="138"/>
-      <c r="F396" s="138"/>
-      <c r="G396" s="138"/>
-      <c r="H396" s="138"/>
-      <c r="I396" s="138"/>
+      <c r="C396" s="107"/>
+      <c r="D396" s="107"/>
+      <c r="E396" s="107"/>
+      <c r="F396" s="107"/>
+      <c r="G396" s="107"/>
+      <c r="H396" s="107"/>
+      <c r="I396" s="107"/>
       <c r="J396" s="47"/>
       <c r="K396" s="48"/>
       <c r="L396" s="49"/>
       <c r="M396" s="49"/>
       <c r="N396" s="47"/>
-      <c r="O396" s="138"/>
-      <c r="P396" s="138"/>
+      <c r="O396" s="107"/>
+      <c r="P396" s="107"/>
     </row>
     <row r="397" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C397" s="135"/>
-      <c r="D397" s="135"/>
-      <c r="E397" s="135"/>
-      <c r="F397" s="135"/>
-      <c r="G397" s="135"/>
-      <c r="H397" s="135"/>
-      <c r="I397" s="135"/>
+      <c r="C397" s="104"/>
+      <c r="D397" s="104"/>
+      <c r="E397" s="104"/>
+      <c r="F397" s="104"/>
+      <c r="G397" s="104"/>
+      <c r="H397" s="104"/>
+      <c r="I397" s="104"/>
       <c r="J397" s="55"/>
       <c r="K397" s="56"/>
       <c r="L397" s="57"/>
       <c r="M397" s="57"/>
       <c r="N397" s="55"/>
-      <c r="O397" s="135"/>
-      <c r="P397" s="135"/>
+      <c r="O397" s="104"/>
+      <c r="P397" s="104"/>
     </row>
     <row r="398" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C398" s="140"/>
-      <c r="D398" s="140"/>
-      <c r="E398" s="140"/>
-      <c r="F398" s="140"/>
-      <c r="G398" s="140"/>
-      <c r="H398" s="140"/>
-      <c r="I398" s="140"/>
+      <c r="C398" s="103"/>
+      <c r="D398" s="103"/>
+      <c r="E398" s="103"/>
+      <c r="F398" s="103"/>
+      <c r="G398" s="103"/>
+      <c r="H398" s="103"/>
+      <c r="I398" s="103"/>
       <c r="J398" s="58"/>
       <c r="K398" s="59"/>
       <c r="L398" s="60"/>
       <c r="M398" s="60"/>
       <c r="N398" s="58"/>
-      <c r="O398" s="140"/>
-      <c r="P398" s="140"/>
+      <c r="O398" s="103"/>
+      <c r="P398" s="103"/>
     </row>
     <row r="399" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C399" s="135"/>
-      <c r="D399" s="135"/>
-      <c r="E399" s="135"/>
-      <c r="F399" s="135"/>
-      <c r="G399" s="135"/>
-      <c r="H399" s="135"/>
-      <c r="I399" s="135"/>
+      <c r="C399" s="104"/>
+      <c r="D399" s="104"/>
+      <c r="E399" s="104"/>
+      <c r="F399" s="104"/>
+      <c r="G399" s="104"/>
+      <c r="H399" s="104"/>
+      <c r="I399" s="104"/>
       <c r="J399" s="55"/>
       <c r="K399" s="56"/>
       <c r="L399" s="57"/>
       <c r="M399" s="57"/>
       <c r="N399" s="55"/>
-      <c r="O399" s="135"/>
-      <c r="P399" s="135"/>
+      <c r="O399" s="104"/>
+      <c r="P399" s="104"/>
     </row>
     <row r="400" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C400" s="140"/>
-      <c r="D400" s="140"/>
-      <c r="E400" s="140"/>
-      <c r="F400" s="140"/>
-      <c r="G400" s="140"/>
-      <c r="H400" s="140"/>
-      <c r="I400" s="140"/>
+      <c r="C400" s="103"/>
+      <c r="D400" s="103"/>
+      <c r="E400" s="103"/>
+      <c r="F400" s="103"/>
+      <c r="G400" s="103"/>
+      <c r="H400" s="103"/>
+      <c r="I400" s="103"/>
       <c r="J400" s="58"/>
       <c r="K400" s="59"/>
       <c r="L400" s="60"/>
       <c r="M400" s="60"/>
       <c r="N400" s="58"/>
-      <c r="O400" s="140"/>
-      <c r="P400" s="140"/>
+      <c r="O400" s="103"/>
+      <c r="P400" s="103"/>
     </row>
     <row r="401" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C401" s="135"/>
-      <c r="D401" s="135"/>
-      <c r="E401" s="135"/>
-      <c r="F401" s="135"/>
-      <c r="G401" s="135"/>
-      <c r="H401" s="135"/>
-      <c r="I401" s="135"/>
+      <c r="C401" s="104"/>
+      <c r="D401" s="104"/>
+      <c r="E401" s="104"/>
+      <c r="F401" s="104"/>
+      <c r="G401" s="104"/>
+      <c r="H401" s="104"/>
+      <c r="I401" s="104"/>
       <c r="J401" s="55"/>
       <c r="K401" s="56"/>
       <c r="L401" s="57"/>
       <c r="M401" s="57"/>
       <c r="N401" s="55"/>
-      <c r="O401" s="135"/>
-      <c r="P401" s="135"/>
+      <c r="O401" s="104"/>
+      <c r="P401" s="104"/>
     </row>
     <row r="402" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C402" s="136"/>
-      <c r="D402" s="136"/>
-      <c r="E402" s="136"/>
-      <c r="F402" s="136"/>
-      <c r="G402" s="136"/>
-      <c r="H402" s="136"/>
-      <c r="I402" s="136"/>
+      <c r="C402" s="101"/>
+      <c r="D402" s="101"/>
+      <c r="E402" s="101"/>
+      <c r="F402" s="101"/>
+      <c r="G402" s="101"/>
+      <c r="H402" s="101"/>
+      <c r="I402" s="101"/>
       <c r="J402" s="64"/>
       <c r="K402" s="65"/>
       <c r="L402" s="66"/>
       <c r="M402" s="66"/>
       <c r="N402" s="64"/>
-      <c r="O402" s="136"/>
-      <c r="P402" s="136"/>
+      <c r="O402" s="101"/>
+      <c r="P402" s="101"/>
     </row>
     <row r="403" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C403" s="137"/>
-      <c r="D403" s="137"/>
-      <c r="E403" s="137"/>
-      <c r="F403" s="137"/>
-      <c r="G403" s="137"/>
-      <c r="H403" s="137"/>
-      <c r="I403" s="137"/>
+      <c r="C403" s="105"/>
+      <c r="D403" s="105"/>
+      <c r="E403" s="105"/>
+      <c r="F403" s="105"/>
+      <c r="G403" s="105"/>
+      <c r="H403" s="105"/>
+      <c r="I403" s="105"/>
       <c r="J403" s="61"/>
       <c r="K403" s="62"/>
       <c r="L403" s="63"/>
       <c r="M403" s="63"/>
       <c r="N403" s="61"/>
-      <c r="O403" s="137"/>
-      <c r="P403" s="137"/>
+      <c r="O403" s="105"/>
+      <c r="P403" s="105"/>
     </row>
     <row r="404" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C404" s="136"/>
-      <c r="D404" s="136"/>
-      <c r="E404" s="136"/>
-      <c r="F404" s="136"/>
-      <c r="G404" s="136"/>
-      <c r="H404" s="136"/>
-      <c r="I404" s="136"/>
+      <c r="C404" s="101"/>
+      <c r="D404" s="101"/>
+      <c r="E404" s="101"/>
+      <c r="F404" s="101"/>
+      <c r="G404" s="101"/>
+      <c r="H404" s="101"/>
+      <c r="I404" s="101"/>
       <c r="J404" s="64"/>
       <c r="K404" s="65"/>
       <c r="L404" s="66"/>
       <c r="M404" s="66"/>
       <c r="N404" s="64"/>
-      <c r="O404" s="136"/>
-      <c r="P404" s="136"/>
+      <c r="O404" s="101"/>
+      <c r="P404" s="101"/>
     </row>
     <row r="405" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C405" s="137"/>
-      <c r="D405" s="137"/>
-      <c r="E405" s="137"/>
-      <c r="F405" s="137"/>
-      <c r="G405" s="137"/>
-      <c r="H405" s="137"/>
-      <c r="I405" s="137"/>
+      <c r="C405" s="105"/>
+      <c r="D405" s="105"/>
+      <c r="E405" s="105"/>
+      <c r="F405" s="105"/>
+      <c r="G405" s="105"/>
+      <c r="H405" s="105"/>
+      <c r="I405" s="105"/>
       <c r="J405" s="61"/>
       <c r="K405" s="62"/>
       <c r="L405" s="63"/>
       <c r="M405" s="63"/>
       <c r="N405" s="61"/>
-      <c r="O405" s="137"/>
-      <c r="P405" s="137"/>
+      <c r="O405" s="105"/>
+      <c r="P405" s="105"/>
     </row>
     <row r="406" spans="3:16" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="C406" s="136"/>
-      <c r="D406" s="136"/>
-      <c r="E406" s="136"/>
-      <c r="F406" s="136"/>
-      <c r="G406" s="136"/>
-      <c r="H406" s="136"/>
-      <c r="I406" s="136"/>
+      <c r="C406" s="101"/>
+      <c r="D406" s="101"/>
+      <c r="E406" s="101"/>
+      <c r="F406" s="101"/>
+      <c r="G406" s="101"/>
+      <c r="H406" s="101"/>
+      <c r="I406" s="101"/>
       <c r="J406" s="64"/>
       <c r="K406" s="65"/>
       <c r="L406" s="66"/>
       <c r="M406" s="66"/>
       <c r="N406" s="64"/>
-      <c r="O406" s="136"/>
-      <c r="P406" s="136"/>
+      <c r="O406" s="101"/>
+      <c r="P406" s="101"/>
     </row>
   </sheetData>
-  <mergeCells count="118">
+  <mergeCells count="116">
+    <mergeCell ref="K124:N124"/>
+    <mergeCell ref="F105:P105"/>
+    <mergeCell ref="K110:N110"/>
+    <mergeCell ref="K116:N116"/>
+    <mergeCell ref="K113:N113"/>
+    <mergeCell ref="K120:N120"/>
+    <mergeCell ref="I128:N128"/>
+    <mergeCell ref="F137:G137"/>
+    <mergeCell ref="F138:G138"/>
+    <mergeCell ref="H137:J137"/>
+    <mergeCell ref="H138:J138"/>
+    <mergeCell ref="K137:L137"/>
+    <mergeCell ref="K138:L138"/>
+    <mergeCell ref="F141:G141"/>
+    <mergeCell ref="F142:G142"/>
+    <mergeCell ref="H146:K146"/>
+    <mergeCell ref="H147:K147"/>
+    <mergeCell ref="H148:K148"/>
+    <mergeCell ref="G263:L263"/>
+    <mergeCell ref="H141:K141"/>
+    <mergeCell ref="N205:P205"/>
+    <mergeCell ref="G229:L229"/>
+    <mergeCell ref="H142:K142"/>
+    <mergeCell ref="H143:K143"/>
+    <mergeCell ref="H144:K144"/>
+    <mergeCell ref="H145:K145"/>
+    <mergeCell ref="L192:O192"/>
+    <mergeCell ref="E198:G198"/>
+    <mergeCell ref="N198:P198"/>
+    <mergeCell ref="I198:K198"/>
+    <mergeCell ref="F205:G205"/>
+    <mergeCell ref="F206:G206"/>
+    <mergeCell ref="F207:G207"/>
+    <mergeCell ref="I206:K206"/>
+    <mergeCell ref="I207:K207"/>
+    <mergeCell ref="N206:P206"/>
+    <mergeCell ref="N207:P207"/>
+    <mergeCell ref="B266:D266"/>
+    <mergeCell ref="G266:H266"/>
+    <mergeCell ref="B280:D280"/>
+    <mergeCell ref="G280:H280"/>
+    <mergeCell ref="B279:D279"/>
+    <mergeCell ref="G279:H279"/>
+    <mergeCell ref="G297:L297"/>
+    <mergeCell ref="F366:L366"/>
+    <mergeCell ref="K376:N376"/>
+    <mergeCell ref="H370:I370"/>
+    <mergeCell ref="H371:I371"/>
+    <mergeCell ref="H372:I372"/>
+    <mergeCell ref="B370:G370"/>
+    <mergeCell ref="B371:G371"/>
+    <mergeCell ref="B372:G372"/>
+    <mergeCell ref="F393:I393"/>
+    <mergeCell ref="O393:P393"/>
+    <mergeCell ref="I205:K205"/>
+    <mergeCell ref="F146:G146"/>
+    <mergeCell ref="F147:G147"/>
+    <mergeCell ref="F148:G148"/>
+    <mergeCell ref="F145:G145"/>
+    <mergeCell ref="F143:G143"/>
+    <mergeCell ref="F144:G144"/>
+    <mergeCell ref="G331:K331"/>
+    <mergeCell ref="K361:N361"/>
+    <mergeCell ref="K377:N377"/>
+    <mergeCell ref="K378:N378"/>
+    <mergeCell ref="O376:Q376"/>
+    <mergeCell ref="O377:Q377"/>
+    <mergeCell ref="O378:Q378"/>
+    <mergeCell ref="F397:I397"/>
+    <mergeCell ref="O397:P397"/>
+    <mergeCell ref="F404:I404"/>
+    <mergeCell ref="O404:P404"/>
+    <mergeCell ref="C405:E405"/>
+    <mergeCell ref="F405:I405"/>
+    <mergeCell ref="O405:P405"/>
+    <mergeCell ref="L191:O191"/>
+    <mergeCell ref="C394:E394"/>
+    <mergeCell ref="F394:I394"/>
+    <mergeCell ref="O394:P394"/>
+    <mergeCell ref="C395:E395"/>
+    <mergeCell ref="F395:I395"/>
+    <mergeCell ref="O395:P395"/>
+    <mergeCell ref="C396:E396"/>
+    <mergeCell ref="F396:I396"/>
+    <mergeCell ref="O396:P396"/>
+    <mergeCell ref="O391:P391"/>
+    <mergeCell ref="C391:E391"/>
+    <mergeCell ref="F391:I391"/>
+    <mergeCell ref="C392:E392"/>
+    <mergeCell ref="F392:I392"/>
+    <mergeCell ref="O392:P392"/>
+    <mergeCell ref="C393:E393"/>
     <mergeCell ref="C406:E406"/>
     <mergeCell ref="F406:I406"/>
     <mergeCell ref="O406:P406"/>
@@ -11216,100 +11355,6 @@
     <mergeCell ref="O403:P403"/>
     <mergeCell ref="C404:E404"/>
     <mergeCell ref="C397:E397"/>
-    <mergeCell ref="F397:I397"/>
-    <mergeCell ref="O397:P397"/>
-    <mergeCell ref="F404:I404"/>
-    <mergeCell ref="O404:P404"/>
-    <mergeCell ref="C405:E405"/>
-    <mergeCell ref="F405:I405"/>
-    <mergeCell ref="O405:P405"/>
-    <mergeCell ref="L191:O191"/>
-    <mergeCell ref="C394:E394"/>
-    <mergeCell ref="F394:I394"/>
-    <mergeCell ref="O394:P394"/>
-    <mergeCell ref="C395:E395"/>
-    <mergeCell ref="F395:I395"/>
-    <mergeCell ref="O395:P395"/>
-    <mergeCell ref="C396:E396"/>
-    <mergeCell ref="F396:I396"/>
-    <mergeCell ref="O396:P396"/>
-    <mergeCell ref="O391:P391"/>
-    <mergeCell ref="C391:E391"/>
-    <mergeCell ref="F391:I391"/>
-    <mergeCell ref="C392:E392"/>
-    <mergeCell ref="F392:I392"/>
-    <mergeCell ref="O392:P392"/>
-    <mergeCell ref="C393:E393"/>
-    <mergeCell ref="F393:I393"/>
-    <mergeCell ref="O393:P393"/>
-    <mergeCell ref="I205:K205"/>
-    <mergeCell ref="F146:G146"/>
-    <mergeCell ref="F147:G147"/>
-    <mergeCell ref="F148:G148"/>
-    <mergeCell ref="F145:G145"/>
-    <mergeCell ref="F143:G143"/>
-    <mergeCell ref="F144:G144"/>
-    <mergeCell ref="D327:K327"/>
-    <mergeCell ref="D328:K328"/>
-    <mergeCell ref="G331:K331"/>
-    <mergeCell ref="K361:N361"/>
-    <mergeCell ref="B266:D266"/>
-    <mergeCell ref="G266:H266"/>
-    <mergeCell ref="B280:D280"/>
-    <mergeCell ref="G280:H280"/>
-    <mergeCell ref="B279:D279"/>
-    <mergeCell ref="G279:H279"/>
-    <mergeCell ref="G297:L297"/>
-    <mergeCell ref="F366:L366"/>
-    <mergeCell ref="K376:N376"/>
-    <mergeCell ref="K377:N377"/>
-    <mergeCell ref="K378:N378"/>
-    <mergeCell ref="F141:G141"/>
-    <mergeCell ref="F142:G142"/>
-    <mergeCell ref="H146:K146"/>
-    <mergeCell ref="H147:K147"/>
-    <mergeCell ref="H148:K148"/>
-    <mergeCell ref="G263:L263"/>
-    <mergeCell ref="H141:K141"/>
-    <mergeCell ref="N205:P205"/>
-    <mergeCell ref="G229:L229"/>
-    <mergeCell ref="H142:K142"/>
-    <mergeCell ref="H143:K143"/>
-    <mergeCell ref="H144:K144"/>
-    <mergeCell ref="H145:K145"/>
-    <mergeCell ref="L192:O192"/>
-    <mergeCell ref="E198:G198"/>
-    <mergeCell ref="N198:P198"/>
-    <mergeCell ref="I198:K198"/>
-    <mergeCell ref="F205:G205"/>
-    <mergeCell ref="F206:G206"/>
-    <mergeCell ref="F207:G207"/>
-    <mergeCell ref="I206:K206"/>
-    <mergeCell ref="I207:K207"/>
-    <mergeCell ref="N206:P206"/>
-    <mergeCell ref="N207:P207"/>
-    <mergeCell ref="K124:N124"/>
-    <mergeCell ref="F105:P105"/>
-    <mergeCell ref="K110:N110"/>
-    <mergeCell ref="K116:N116"/>
-    <mergeCell ref="K113:N113"/>
-    <mergeCell ref="K120:N120"/>
-    <mergeCell ref="I128:N128"/>
-    <mergeCell ref="F137:G137"/>
-    <mergeCell ref="F138:G138"/>
-    <mergeCell ref="H137:J137"/>
-    <mergeCell ref="H138:J138"/>
-    <mergeCell ref="K137:L137"/>
-    <mergeCell ref="K138:L138"/>
-    <mergeCell ref="O376:Q376"/>
-    <mergeCell ref="O377:Q377"/>
-    <mergeCell ref="O378:Q378"/>
-    <mergeCell ref="H370:I370"/>
-    <mergeCell ref="H371:I371"/>
-    <mergeCell ref="H372:I372"/>
-    <mergeCell ref="B370:G370"/>
-    <mergeCell ref="B371:G371"/>
-    <mergeCell ref="B372:G372"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="95" orientation="landscape" r:id="rId1"/>
@@ -11320,10 +11365,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Лист2"/>
-  <dimension ref="A1:AJ8"/>
+  <dimension ref="A1:AH18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView topLeftCell="O1" workbookViewId="0">
+      <selection activeCell="U1" sqref="U1:V1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11334,7 +11379,7 @@
     <col min="4" max="4" bestFit="true" customWidth="true" style="10" width="43.5703125" collapsed="false"/>
     <col min="5" max="5" customWidth="true" style="12" width="18.7109375" collapsed="false"/>
     <col min="6" max="6" style="12" width="9.140625" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" style="14" width="10.140625" collapsed="false"/>
+    <col min="7" max="7" customWidth="true" style="13" width="10.140625" collapsed="false"/>
     <col min="8" max="8" customWidth="true" style="13" width="16.7109375" collapsed="false"/>
     <col min="9" max="9" bestFit="true" customWidth="true" style="13" width="11.85546875" collapsed="false"/>
     <col min="10" max="10" customWidth="true" style="32" width="19.5703125" collapsed="false"/>
@@ -11348,25 +11393,23 @@
     <col min="18" max="18" bestFit="true" customWidth="true" style="30" width="9.28515625" collapsed="false"/>
     <col min="19" max="19" bestFit="true" customWidth="true" style="30" width="15.7109375" collapsed="false"/>
     <col min="20" max="20" bestFit="true" customWidth="true" style="30" width="21.42578125" collapsed="false"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="44" width="18.7109375" collapsed="false"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="44" width="26.85546875" collapsed="false"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="34" width="11.42578125" collapsed="false"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" style="34" width="18.0" collapsed="false"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" style="34" width="23.5703125" collapsed="false"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="44" width="23.5703125" collapsed="false"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="40" width="14.5703125" collapsed="false"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="40" width="20.85546875" collapsed="false"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" style="40" width="13.7109375" collapsed="false"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" style="40" width="22.42578125" collapsed="false"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" style="41" width="10.0" collapsed="false"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="41" width="23.0" collapsed="false"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" style="41" width="16.42578125" collapsed="false"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" style="41" width="21.42578125" collapsed="false"/>
-    <col min="35" max="35" customWidth="true" style="9" width="14.140625" collapsed="false"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" style="9" width="17.7109375" collapsed="false"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="34" width="11.42578125" collapsed="false"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="34" width="18.0" collapsed="false"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="34" width="23.5703125" collapsed="false"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="44" width="23.5703125" collapsed="false"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="40" width="14.5703125" collapsed="false"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="40" width="20.85546875" collapsed="false"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="40" width="13.7109375" collapsed="false"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="40" width="22.42578125" collapsed="false"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" style="41" width="10.0" collapsed="false"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" style="41" width="23.0" collapsed="false"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" style="41" width="16.42578125" collapsed="false"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="41" width="21.42578125" collapsed="false"/>
+    <col min="33" max="33" customWidth="true" style="9" width="14.140625" collapsed="false"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" style="9" width="17.7109375" collapsed="false"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -11385,7 +11428,7 @@
       <c r="F1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="G1" s="13" t="s">
         <v>12</v>
       </c>
       <c r="H1" s="13" t="s">
@@ -11427,56 +11470,50 @@
       <c r="T1" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="U1" s="44" t="s">
-        <v>63</v>
-      </c>
-      <c r="V1" s="44" t="s">
-        <v>64</v>
+      <c r="U1" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="V1" s="33" t="s">
+        <v>66</v>
       </c>
       <c r="W1" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="X1" s="33" t="s">
-        <v>66</v>
-      </c>
-      <c r="Y1" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="Z1" s="44" t="s">
+      <c r="X1" s="44" t="s">
         <v>68</v>
       </c>
+      <c r="Y1" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z1" s="39" t="s">
+        <v>76</v>
+      </c>
       <c r="AA1" s="39" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="AB1" s="39" t="s">
-        <v>76</v>
-      </c>
-      <c r="AC1" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="AD1" s="39" t="s">
         <v>78</v>
       </c>
+      <c r="AC1" s="41" t="s">
+        <v>81</v>
+      </c>
+      <c r="AD1" s="41" t="s">
+        <v>82</v>
+      </c>
       <c r="AE1" s="41" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="AF1" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="AG1" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="AH1" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="AJ1" s="3" t="s">
+      <c r="AH1" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="n">
         <v>65.0</v>
       </c>
@@ -11519,8 +11556,26 @@
       <c r="N2" t="n">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="O2" t="s">
+        <v>166</v>
+      </c>
+      <c r="P2" t="n">
+        <v>473.0</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R2" t="s">
+        <v>171</v>
+      </c>
+      <c r="S2" t="n">
+        <v>178.0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="n">
         <v>8.0</v>
       </c>
@@ -11557,8 +11612,26 @@
       <c r="N3" t="n">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="O3" t="s">
+        <v>167</v>
+      </c>
+      <c r="P3" t="n">
+        <v>467.0</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="R3" t="s">
+        <v>172</v>
+      </c>
+      <c r="S3" t="n">
+        <v>142.0</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4" t="n">
         <v>1.0</v>
       </c>
@@ -11595,8 +11668,17 @@
       <c r="N4" t="n">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="R4" t="s">
+        <v>173</v>
+      </c>
+      <c r="S4" t="n">
+        <v>170.0</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5" t="n">
         <v>9.0</v>
       </c>
@@ -11633,8 +11715,17 @@
       <c r="N5" t="n">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="R5" t="s">
+        <v>174</v>
+      </c>
+      <c r="S5" t="n">
+        <v>217.0</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6" t="n">
         <v>890.0</v>
       </c>
@@ -11671,8 +11762,17 @@
       <c r="N6" t="n">
         <v>0.0</v>
       </c>
-    </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="R6" t="s">
+        <v>175</v>
+      </c>
+      <c r="S6" t="n">
+        <v>97.0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" t="n">
         <v>76.0</v>
       </c>
@@ -11700,8 +11800,17 @@
       <c r="K7" t="n">
         <v>154.0</v>
       </c>
-    </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.25">
+      <c r="R7" t="s">
+        <v>176</v>
+      </c>
+      <c r="S7" t="n">
+        <v>114.0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="C8" t="n">
         <v>0.0</v>
       </c>
@@ -11723,7 +11832,26 @@
       <c r="K8" t="n">
         <v>8.0</v>
       </c>
-    </row>
+      <c r="R8" t="s">
+        <v>177</v>
+      </c>
+      <c r="S8" t="n">
+        <v>132.0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
AdvertAnalitycDAO work if use user Direct.exel
</commit_message>
<xml_diff>
--- a/ready/report1.xlsx
+++ b/ready/report1.xlsx
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="179">
   <si>
     <t>quality</t>
   </si>
@@ -619,13 +619,10 @@
     <t>женский</t>
   </si>
   <si>
-    <t>На сайте больше женщин</t>
+    <t>На сайте больше мужчин</t>
   </si>
   <si>
     <t>Коэф. конверсии выше у женщин</t>
-  </si>
-  <si>
-    <t>�</t>
   </si>
   <si>
     <t>Пятница</t>
@@ -10794,7 +10791,7 @@
       <c r="C280" s="115"/>
       <c r="D280" s="115"/>
       <c r="G280" s="78" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="H280" s="115"/>
     </row>
@@ -10826,12 +10823,12 @@
     </row>
     <row r="327">
       <c r="D327" t="s" s="78">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="328">
       <c r="D328" t="s" s="78">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="331" spans="4:12" ht="21" x14ac:dyDescent="0.35">
@@ -11566,7 +11563,7 @@
         <v>0.0</v>
       </c>
       <c r="R2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="S2" t="n">
         <v>178.0</v>
@@ -11622,7 +11619,7 @@
         <v>0.0</v>
       </c>
       <c r="R3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S3" t="n">
         <v>142.0</v>
@@ -11669,7 +11666,7 @@
         <v>0.0</v>
       </c>
       <c r="R4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="S4" t="n">
         <v>170.0</v>
@@ -11716,7 +11713,7 @@
         <v>0.0</v>
       </c>
       <c r="R5" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="S5" t="n">
         <v>217.0</v>
@@ -11763,7 +11760,7 @@
         <v>0.0</v>
       </c>
       <c r="R6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="S6" t="n">
         <v>97.0</v>
@@ -11801,7 +11798,7 @@
         <v>154.0</v>
       </c>
       <c r="R7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="S7" t="n">
         <v>114.0</v>
@@ -11833,7 +11830,7 @@
         <v>8.0</v>
       </c>
       <c r="R8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="S8" t="n">
         <v>132.0</v>

</xml_diff>

<commit_message>
search and context work correct detail source
</commit_message>
<xml_diff>
--- a/ready/report1.xlsx
+++ b/ready/report1.xlsx
@@ -30,14 +30,14 @@
     <definedName name="costs">report!$P$392</definedName>
     <definedName name="costWithoutConversation">ChanelTrafic!$Y$2</definedName>
     <definedName name="countAdvert">report!$H$138</definedName>
-    <definedName name="countConversation">ChanelTrafic!$H$2:$H$6</definedName>
+    <definedName name="countConversation">ChanelTrafic!$H$2:$H$8</definedName>
     <definedName name="countGetGoals">report!$K$120</definedName>
     <definedName name="CpaCost">report!$I$128</definedName>
     <definedName name="ctr">report!$R$392</definedName>
-    <definedName name="dayVisited">ChanelTrafic!$G$2:$G$6</definedName>
-    <definedName name="dayWeek">ChanelTrafic!$R$2:$R$6</definedName>
-    <definedName name="dayWeekConversation">ChanelTrafic!$T$2:$T$6</definedName>
-    <definedName name="dayWeekVisited">ChanelTrafic!$S$2:$S$6</definedName>
+    <definedName name="dayVisited">ChanelTrafic!$G$2:$G$8</definedName>
+    <definedName name="dayWeek">ChanelTrafic!$R$2:$R$8</definedName>
+    <definedName name="dayWeekConversation">ChanelTrafic!$T$2:$T$8</definedName>
+    <definedName name="dayWeekVisited">ChanelTrafic!$S$2:$S$8</definedName>
     <definedName name="detailConversation">report!$D$64</definedName>
     <definedName name="detailVisited">report!$D$63</definedName>
     <definedName name="effecientConversation">report!$K$124</definedName>
@@ -46,8 +46,8 @@
     <definedName name="expansive">report!$N$392:$N$406</definedName>
     <definedName name="femaleConversation">report!$B$280</definedName>
     <definedName name="femaleConversationPer">report!$B$280</definedName>
-    <definedName name="goal">ChanelTrafic!$E$2:$E$7</definedName>
-    <definedName name="goalQuality">ChanelTrafic!$F$2:$F$7</definedName>
+    <definedName name="goal">ChanelTrafic!$E$2:$E$8</definedName>
+    <definedName name="goalQuality">ChanelTrafic!$F$2:$F$8</definedName>
     <definedName name="hoursOfDay">ChanelTrafic!$U$2:$U$1</definedName>
     <definedName name="hoursOfDayConversation">ChanelTrafic!$W$2:$W$1</definedName>
     <definedName name="hoursOfDayVisited">ChanelTrafic!$V$2:$V$1</definedName>
@@ -74,7 +74,7 @@
     <definedName name="popularDayOfWeek">report!$D$325</definedName>
     <definedName name="popularHours">report!$D$358</definedName>
     <definedName name="position">report!$K$392</definedName>
-    <definedName name="quality">ChanelTrafic!$A$2:$A$6</definedName>
+    <definedName name="quality">ChanelTrafic!$A$2:$A$7</definedName>
     <definedName name="qualityClick">report!$K$113</definedName>
     <definedName name="qualityDetail">ChanelTrafic!$C$2:$C$7</definedName>
     <definedName name="qualityDetailper">ChanelTrafic!#REF!</definedName>
@@ -88,11 +88,11 @@
     <definedName name="regionAgeLider">report!$D$259</definedName>
     <definedName name="regionConversLider">report!$E$192</definedName>
     <definedName name="regionLider">report!$E$191</definedName>
-    <definedName name="regionName">ChanelTrafic!$J$2:$J$7</definedName>
-    <definedName name="regionQuality">ChanelTrafic!$K$2:$K$7</definedName>
+    <definedName name="regionName">ChanelTrafic!$J$2:$J$8</definedName>
+    <definedName name="regionQuality">ChanelTrafic!$K$2:$K$8</definedName>
     <definedName name="sendAll">report!$K$116</definedName>
     <definedName name="sendall2">report!$P$376</definedName>
-    <definedName name="source">ChanelTrafic!$B$2:$B$6</definedName>
+    <definedName name="source">ChanelTrafic!$B$2:$B$7</definedName>
     <definedName name="sourceDetail">ChanelTrafic!$C$2:$C$8</definedName>
     <definedName name="sourceDetailPer">ChanelTrafic!$D$2:$D$8</definedName>
     <definedName name="tabConversation">report!$I$212</definedName>
@@ -101,7 +101,7 @@
     <definedName name="userConversation">ChanelTrafic!$N$2:$N$6</definedName>
     <definedName name="userVisited">ChanelTrafic!$M$2:$M$6</definedName>
     <definedName name="visited">ChanelTrafic!#REF!</definedName>
-    <definedName name="visitedDiv10">ChanelTrafic!$I$2:$I$6</definedName>
+    <definedName name="visitedDiv10">ChanelTrafic!$I$2:$I$8</definedName>
     <definedName name="wasSpend">ChanelTrafic!#REF!</definedName>
     <definedName name="wasSpendNotReachGoal">ChanelTrafic!#REF!</definedName>
     <definedName name="whichConversationMore">report!$B$285</definedName>
@@ -134,7 +134,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="245">
   <si>
     <t>quality</t>
   </si>
@@ -208,9 +208,6 @@
     <t>Стоимость</t>
   </si>
   <si>
-    <t>Количество</t>
-  </si>
-  <si>
     <t>Цена 1-го</t>
   </si>
   <si>
@@ -232,9 +229,6 @@
     <t>ОБРАЩЕНИЙ</t>
   </si>
   <si>
-    <t>КОНВЕРСИЯ</t>
-  </si>
-  <si>
     <t>ЦЕНА ОБРАЩЕНИЯ</t>
   </si>
   <si>
@@ -445,130 +439,133 @@
     <t>ТЕКСТ</t>
   </si>
   <si>
-    <t>Переходы из поисковых систем (38,46%)</t>
-  </si>
-  <si>
-    <t>Переходы по ссылкам на сайтах (30,43%)</t>
-  </si>
-  <si>
-    <t>Переходы по рекламе (21,94%)</t>
-  </si>
-  <si>
-    <t>Прямые заходы (21,43%)</t>
-  </si>
-  <si>
-    <t>Внутренние переходы (11,54%)</t>
-  </si>
-  <si>
-    <t>Болше всего трафика - Переходы по рекламе (155,00)</t>
-  </si>
-  <si>
-    <t>Самый высокий % конверсии - Переходы из поисковых систем (38,46%)</t>
-  </si>
-  <si>
-    <t>mosgid.ru (0,00)</t>
-  </si>
-  <si>
-    <t>Яндекс (50,00)</t>
-  </si>
-  <si>
-    <t>Google (33,33)</t>
-  </si>
-  <si>
-    <t>Google Adwords (29,73)</t>
-  </si>
-  <si>
-    <t>link.2gis.ru (0,00)</t>
-  </si>
-  <si>
-    <t>Яндекс: Директ (19,08)</t>
-  </si>
-  <si>
-    <t>Яндекс: Не определено (9,09)</t>
-  </si>
-  <si>
-    <t>Болше всего трафика - Яндекс: Директ (131,00)</t>
-  </si>
-  <si>
-    <t>Самый высокий % конверсии - Яндекс (50,00%)</t>
+    <t>CTR %</t>
+  </si>
+  <si>
+    <t>КОНВЕРСИЯ %</t>
+  </si>
+  <si>
+    <t>Количество обращений</t>
+  </si>
+  <si>
+    <t>Переходы из социальных сетей (50,00%)</t>
+  </si>
+  <si>
+    <t>Переходы по ссылкам на сайтах (65,58%)</t>
+  </si>
+  <si>
+    <t>Переходы из поисковых систем (76,10%)</t>
+  </si>
+  <si>
+    <t>Внутренние переходы (43,11%)</t>
+  </si>
+  <si>
+    <t>Переходы по рекламе (48,85%)</t>
+  </si>
+  <si>
+    <t>Прямые заходы (38,13%)</t>
+  </si>
+  <si>
+    <t>Болше всего трафика - Переходы по рекламе (1573,00)</t>
+  </si>
+  <si>
+    <t>Самый высокий % конверсии - Переходы из поисковых систем (76,10%)</t>
+  </si>
+  <si>
+    <t>Яндекс: Директ (33,48)</t>
+  </si>
+  <si>
+    <t>Google Adwords (39,92)</t>
+  </si>
+  <si>
+    <t>Google (52,38)</t>
+  </si>
+  <si>
+    <t>link.2gis.ru (45,13)</t>
+  </si>
+  <si>
+    <t>Яндекс (52,75)</t>
+  </si>
+  <si>
+    <t>aristokrat-nsk.ru (28,99)</t>
+  </si>
+  <si>
+    <t>news.ngs.ru (58,06)</t>
+  </si>
+  <si>
+    <t>Болше всего трафика - Яндекс: Директ (1156,00)</t>
+  </si>
+  <si>
+    <t>Самый высокий % конверсии - news.ngs.ru (58,06%)</t>
   </si>
   <si>
     <t>Просмотр 3 страниц</t>
   </si>
   <si>
+    <t>Контакты</t>
+  </si>
+  <si>
     <t>Получить бесплатную консультацию (Открытие)</t>
   </si>
   <si>
-    <t>Контакты</t>
-  </si>
-  <si>
     <t>Получить бесплатную консультацию (Отправка)</t>
   </si>
   <si>
+    <t>Консультация арбитражного управляющего (Нажатие)</t>
+  </si>
+  <si>
     <t>Заказать звонок (Открытие)</t>
   </si>
   <si>
-    <t>Консультация арбитражного управляющего (Нажатие)</t>
-  </si>
-  <si>
-    <t>120910</t>
-  </si>
-  <si>
-    <t>129</t>
-  </si>
-  <si>
-    <t>4658,30</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>0,256</t>
-  </si>
-  <si>
-    <t>141,16</t>
-  </si>
-  <si>
-    <t>8.552631578947368%</t>
-  </si>
-  <si>
-    <t>33.881578947368425%</t>
-  </si>
-  <si>
-    <t>81.93353</t>
-  </si>
-  <si>
-    <t>225,00%</t>
-  </si>
-  <si>
-    <t>436,01%</t>
-  </si>
-  <si>
-    <t>Приволжский федеральный округ (50,00%)</t>
-  </si>
-  <si>
-    <t>Сибирский федеральный округ (24,48%)</t>
-  </si>
-  <si>
-    <t>Северо-Западный федеральный округ (0,00%)</t>
-  </si>
-  <si>
-    <t>Уральский федеральный округ (0,00%)</t>
-  </si>
-  <si>
-    <t>Центральный федеральный округ (0,00%)</t>
-  </si>
-  <si>
-    <t>Южный федеральный округ (0,00%)</t>
-  </si>
-  <si>
-    <t>Лидер по посетителям - Сибирский федеральный округ (241,00)</t>
-  </si>
-  <si>
-    <t>% Конверсии больше - Приволжский федеральный округ (50,00%)</t>
-  </si>
-  <si>
-    <t>На долю планшетов и смартфонов приходится 37,60% трафика</t>
+    <t>Заказать звонок (Отправка)</t>
+  </si>
+  <si>
+    <t>1221914</t>
+  </si>
+  <si>
+    <t>1323</t>
+  </si>
+  <si>
+    <t>42726,18</t>
+  </si>
+  <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>0,261</t>
+  </si>
+  <si>
+    <t>123,84</t>
+  </si>
+  <si>
+    <t>Сибирский федеральный округ (54,42%)</t>
+  </si>
+  <si>
+    <t>Приволжский федеральный округ (50,53%)</t>
+  </si>
+  <si>
+    <t>Южный федеральный округ (46,74%)</t>
+  </si>
+  <si>
+    <t>Центральный федеральный округ (42,86%)</t>
+  </si>
+  <si>
+    <t>Уральский федеральный округ (36,67%)</t>
+  </si>
+  <si>
+    <t>Дальневосточный федеральный округ (10,53%)</t>
+  </si>
+  <si>
+    <t>Северо-Западный федеральный округ (11,54%)</t>
+  </si>
+  <si>
+    <t>Лидер по посетителям - Сибирский федеральный округ (2004,00)</t>
+  </si>
+  <si>
+    <t>% Конверсии больше - Сибирский федеральный округ (54,42%)</t>
+  </si>
+  <si>
+    <t>На долю планшетов и смартфонов приходится 29,38% трафика</t>
   </si>
   <si>
     <t>25‑34 года</t>
@@ -580,49 +577,55 @@
     <t>18‑24 года</t>
   </si>
   <si>
+    <t>35‑44 года</t>
+  </si>
+  <si>
     <t>младше 18 лет</t>
   </si>
   <si>
-    <t>35‑44 года</t>
-  </si>
-  <si>
-    <t>Болше всего сеансов у группы - 25‑34 года (94,00)</t>
-  </si>
-  <si>
-    <t>Лучший коэффициент конверсии у группы младше 18 лет (57,14%)</t>
+    <t>Болше всего сеансов у группы - 25‑34 года (739,00)</t>
+  </si>
+  <si>
+    <t>Лучший коэффициент конверсии у группы младше 18 лет (47,89%)</t>
+  </si>
+  <si>
+    <t>женский</t>
   </si>
   <si>
     <t>мужской</t>
   </si>
   <si>
-    <t>женский</t>
-  </si>
-  <si>
     <t>На сайте больше женщин</t>
   </si>
   <si>
-    <t>Коэф. конверсии выше у мужчин</t>
+    <t>Коэф. конверсии выше у женщин</t>
+  </si>
+  <si>
+    <t>Понедельник</t>
+  </si>
+  <si>
+    <t>Среда</t>
   </si>
   <si>
     <t>Четверг</t>
   </si>
   <si>
-    <t>Среда</t>
+    <t>Пятница</t>
+  </si>
+  <si>
+    <t>Вторник</t>
+  </si>
+  <si>
+    <t>Суббота</t>
   </si>
   <si>
     <t>Воскресенье</t>
   </si>
   <si>
-    <t>Пятница</t>
-  </si>
-  <si>
-    <t>Суббота</t>
-  </si>
-  <si>
     <t>Четверг - самый высокий коэф. конверсии</t>
   </si>
   <si>
-    <t>Воскресенье - больше всего сеансов</t>
+    <t>Понедельник - больше всего сеансов</t>
   </si>
   <si>
     <t xml:space="preserve">Конверсии происходят приемущественно в - </t>
@@ -640,16 +643,58 @@
     <t>ad2</t>
   </si>
   <si>
+    <t>company 21</t>
+  </si>
+  <si>
+    <t>ad21</t>
+  </si>
+  <si>
+    <t>company 1</t>
+  </si>
+  <si>
+    <t>ad1</t>
+  </si>
+  <si>
+    <t>company 3</t>
+  </si>
+  <si>
+    <t>ad3</t>
+  </si>
+  <si>
+    <t>company 12</t>
+  </si>
+  <si>
+    <t>ad12</t>
+  </si>
+  <si>
+    <t>company 38</t>
+  </si>
+  <si>
+    <t>ad38</t>
+  </si>
+  <si>
+    <t>company 5</t>
+  </si>
+  <si>
+    <t>ad5</t>
+  </si>
+  <si>
+    <t>company 14</t>
+  </si>
+  <si>
+    <t>ad14</t>
+  </si>
+  <si>
     <t>company 9</t>
   </si>
   <si>
     <t>ad9</t>
   </si>
   <si>
-    <t>company 12</t>
-  </si>
-  <si>
-    <t>ad12</t>
+    <t>company 27</t>
+  </si>
+  <si>
+    <t>ad27</t>
   </si>
   <si>
     <t>company 4</t>
@@ -658,214 +703,172 @@
     <t>ad4</t>
   </si>
   <si>
+    <t>company 8</t>
+  </si>
+  <si>
+    <t>ad8</t>
+  </si>
+  <si>
+    <t>company 24</t>
+  </si>
+  <si>
+    <t>ad24</t>
+  </si>
+  <si>
+    <t>company 6</t>
+  </si>
+  <si>
+    <t>ad6</t>
+  </si>
+  <si>
+    <t>company 19</t>
+  </si>
+  <si>
+    <t>ad19</t>
+  </si>
+  <si>
+    <t>company 20</t>
+  </si>
+  <si>
+    <t>ad20</t>
+  </si>
+  <si>
+    <t>company 13</t>
+  </si>
+  <si>
+    <t>ad13</t>
+  </si>
+  <si>
     <t>company 17</t>
   </si>
   <si>
     <t>ad17</t>
   </si>
   <si>
-    <t>company 5</t>
-  </si>
-  <si>
-    <t>ad5</t>
+    <t>company 29</t>
+  </si>
+  <si>
+    <t>ad29</t>
+  </si>
+  <si>
+    <t>company 28</t>
+  </si>
+  <si>
+    <t>ad28</t>
+  </si>
+  <si>
+    <t>company 35</t>
+  </si>
+  <si>
+    <t>ad35</t>
+  </si>
+  <si>
+    <t>company 7</t>
+  </si>
+  <si>
+    <t>ad7</t>
+  </si>
+  <si>
+    <t>company 10</t>
+  </si>
+  <si>
+    <t>ad10</t>
+  </si>
+  <si>
+    <t>company 11</t>
+  </si>
+  <si>
+    <t>ad11</t>
+  </si>
+  <si>
+    <t>company 15</t>
+  </si>
+  <si>
+    <t>ad15</t>
+  </si>
+  <si>
+    <t>company 16</t>
+  </si>
+  <si>
+    <t>ad16</t>
+  </si>
+  <si>
+    <t>company 18</t>
+  </si>
+  <si>
+    <t>ad18</t>
+  </si>
+  <si>
+    <t>company 22</t>
+  </si>
+  <si>
+    <t>ad22</t>
+  </si>
+  <si>
+    <t>company 23</t>
+  </si>
+  <si>
+    <t>ad23</t>
+  </si>
+  <si>
+    <t>company 25</t>
+  </si>
+  <si>
+    <t>ad25</t>
+  </si>
+  <si>
+    <t>company 26</t>
+  </si>
+  <si>
+    <t>ad26</t>
+  </si>
+  <si>
+    <t>company 30</t>
+  </si>
+  <si>
+    <t>ad30</t>
+  </si>
+  <si>
+    <t>company 31</t>
+  </si>
+  <si>
+    <t>ad31</t>
+  </si>
+  <si>
+    <t>company 34</t>
+  </si>
+  <si>
+    <t>ad34</t>
+  </si>
+  <si>
+    <t>company 32</t>
+  </si>
+  <si>
+    <t>ad32</t>
+  </si>
+  <si>
+    <t>company 33</t>
+  </si>
+  <si>
+    <t>ad33</t>
+  </si>
+  <si>
+    <t>company 36</t>
+  </si>
+  <si>
+    <t>ad36</t>
+  </si>
+  <si>
+    <t>company 39</t>
+  </si>
+  <si>
+    <t>ad39</t>
   </si>
   <si>
     <t>company 37</t>
   </si>
   <si>
     <t>ad37</t>
-  </si>
-  <si>
-    <t>company 10</t>
-  </si>
-  <si>
-    <t>ad10</t>
-  </si>
-  <si>
-    <t>company 21</t>
-  </si>
-  <si>
-    <t>ad21</t>
-  </si>
-  <si>
-    <t>company 31</t>
-  </si>
-  <si>
-    <t>ad31</t>
-  </si>
-  <si>
-    <t>company 14</t>
-  </si>
-  <si>
-    <t>ad14</t>
-  </si>
-  <si>
-    <t>company 11</t>
-  </si>
-  <si>
-    <t>ad11</t>
-  </si>
-  <si>
-    <t>company 26</t>
-  </si>
-  <si>
-    <t>ad26</t>
-  </si>
-  <si>
-    <t>company 28</t>
-  </si>
-  <si>
-    <t>ad28</t>
-  </si>
-  <si>
-    <t>company 34</t>
-  </si>
-  <si>
-    <t>ad34</t>
-  </si>
-  <si>
-    <t>company 23</t>
-  </si>
-  <si>
-    <t>ad23</t>
-  </si>
-  <si>
-    <t>company 22</t>
-  </si>
-  <si>
-    <t>ad22</t>
-  </si>
-  <si>
-    <t>company 38</t>
-  </si>
-  <si>
-    <t>ad38</t>
-  </si>
-  <si>
-    <t>company 29</t>
-  </si>
-  <si>
-    <t>ad29</t>
-  </si>
-  <si>
-    <t>company 36</t>
-  </si>
-  <si>
-    <t>ad36</t>
-  </si>
-  <si>
-    <t>company 1</t>
-  </si>
-  <si>
-    <t>ad1</t>
-  </si>
-  <si>
-    <t>company 3</t>
-  </si>
-  <si>
-    <t>ad3</t>
-  </si>
-  <si>
-    <t>company 6</t>
-  </si>
-  <si>
-    <t>ad6</t>
-  </si>
-  <si>
-    <t>company 7</t>
-  </si>
-  <si>
-    <t>ad7</t>
-  </si>
-  <si>
-    <t>company 8</t>
-  </si>
-  <si>
-    <t>ad8</t>
-  </si>
-  <si>
-    <t>company 13</t>
-  </si>
-  <si>
-    <t>ad13</t>
-  </si>
-  <si>
-    <t>company 15</t>
-  </si>
-  <si>
-    <t>ad15</t>
-  </si>
-  <si>
-    <t>company 16</t>
-  </si>
-  <si>
-    <t>ad16</t>
-  </si>
-  <si>
-    <t>company 18</t>
-  </si>
-  <si>
-    <t>ad18</t>
-  </si>
-  <si>
-    <t>company 19</t>
-  </si>
-  <si>
-    <t>ad19</t>
-  </si>
-  <si>
-    <t>company 20</t>
-  </si>
-  <si>
-    <t>ad20</t>
-  </si>
-  <si>
-    <t>company 24</t>
-  </si>
-  <si>
-    <t>ad24</t>
-  </si>
-  <si>
-    <t>company 27</t>
-  </si>
-  <si>
-    <t>ad27</t>
-  </si>
-  <si>
-    <t>company 25</t>
-  </si>
-  <si>
-    <t>ad25</t>
-  </si>
-  <si>
-    <t>company 30</t>
-  </si>
-  <si>
-    <t>ad30</t>
-  </si>
-  <si>
-    <t>company 35</t>
-  </si>
-  <si>
-    <t>ad35</t>
-  </si>
-  <si>
-    <t>company 33</t>
-  </si>
-  <si>
-    <t>ad33</t>
-  </si>
-  <si>
-    <t>company 32</t>
-  </si>
-  <si>
-    <t>ad32</t>
-  </si>
-  <si>
-    <t>company 39</t>
-  </si>
-  <si>
-    <t>ad39</t>
   </si>
 </sst>
 </file>
@@ -1492,21 +1495,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="23" borderId="4" xfId="6" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1537,10 +1525,19 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="10" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1570,6 +1567,9 @@
     <xf numFmtId="0" fontId="10" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1581,6 +1581,9 @@
     </xf>
     <xf numFmtId="10" fontId="10" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="19" borderId="0" xfId="5" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -7756,12 +7759,12 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="0" y="200482"/>
-          <a:ext cx="5225704" cy="772392"/>
+          <a:off x="0" y="199787"/>
+          <a:ext cx="4840782" cy="769715"/>
         </a:xfrm>
         <a:prstGeom prst="trapezoid">
           <a:avLst>
-            <a:gd name="adj" fmla="val 53885"/>
+            <a:gd name="adj" fmla="val 50089"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -7831,8 +7834,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-10800000">
-        <a:off x="914498" y="200482"/>
-        <a:ext cx="3396707" cy="772392"/>
+        <a:off x="847136" y="199787"/>
+        <a:ext cx="3146508" cy="769715"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{69CA1DAA-1002-439B-95E6-9B03B9A978F9}">
@@ -7842,12 +7845,12 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="168597" y="928323"/>
-          <a:ext cx="4888508" cy="772392"/>
+          <a:off x="156178" y="925105"/>
+          <a:ext cx="4528424" cy="769715"/>
         </a:xfrm>
         <a:prstGeom prst="trapezoid">
           <a:avLst>
-            <a:gd name="adj" fmla="val 53885"/>
+            <a:gd name="adj" fmla="val 50089"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -7919,8 +7922,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-10800000">
-        <a:off x="1024086" y="928323"/>
-        <a:ext cx="3177530" cy="772392"/>
+        <a:off x="948653" y="925105"/>
+        <a:ext cx="2943475" cy="769715"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{238952AD-046B-41C1-B6E4-2C5149FAC37B}">
@@ -7930,12 +7933,12 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="376346" y="1667302"/>
-          <a:ext cx="4473010" cy="772392"/>
+          <a:off x="348625" y="1661523"/>
+          <a:ext cx="4143531" cy="769715"/>
         </a:xfrm>
         <a:prstGeom prst="trapezoid">
           <a:avLst>
-            <a:gd name="adj" fmla="val 53885"/>
+            <a:gd name="adj" fmla="val 50089"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -8007,8 +8010,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-10800000">
-        <a:off x="1159123" y="1667302"/>
-        <a:ext cx="2907457" cy="772392"/>
+        <a:off x="1073743" y="1661523"/>
+        <a:ext cx="2693295" cy="769715"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{425953AF-BAA2-4E7A-916B-2A82294152AD}">
@@ -8018,12 +8021,12 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="619750" y="2395144"/>
-          <a:ext cx="3986202" cy="772392"/>
+          <a:off x="574100" y="2386841"/>
+          <a:ext cx="3692581" cy="769715"/>
         </a:xfrm>
         <a:prstGeom prst="trapezoid">
           <a:avLst>
-            <a:gd name="adj" fmla="val 53885"/>
+            <a:gd name="adj" fmla="val 50089"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -8095,8 +8098,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-10800000">
-        <a:off x="1317336" y="2395144"/>
-        <a:ext cx="2591031" cy="772392"/>
+        <a:off x="1220302" y="2386841"/>
+        <a:ext cx="2400177" cy="769715"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{5A06E787-2B65-46E6-9A04-2968475748A6}">
@@ -8106,12 +8109,12 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="888135" y="3122985"/>
-          <a:ext cx="3449433" cy="772392"/>
+          <a:off x="822715" y="3112160"/>
+          <a:ext cx="3195350" cy="769715"/>
         </a:xfrm>
         <a:prstGeom prst="trapezoid">
           <a:avLst>
-            <a:gd name="adj" fmla="val 53885"/>
+            <a:gd name="adj" fmla="val 50089"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -8183,8 +8186,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-10800000">
-        <a:off x="1491786" y="3122985"/>
-        <a:ext cx="2242131" cy="772392"/>
+        <a:off x="1381902" y="3112160"/>
+        <a:ext cx="2076977" cy="769715"/>
       </dsp:txXfrm>
     </dsp:sp>
     <dsp:sp modelId="{9D67B753-3B31-4AF4-8047-2E5F38D41F74}">
@@ -8194,12 +8197,12 @@
       </dsp:nvSpPr>
       <dsp:spPr>
         <a:xfrm rot="10800000">
-          <a:off x="1046368" y="3861964"/>
-          <a:ext cx="3132966" cy="986979"/>
+          <a:off x="969293" y="3848578"/>
+          <a:ext cx="2902194" cy="983557"/>
         </a:xfrm>
         <a:prstGeom prst="trapezoid">
           <a:avLst>
-            <a:gd name="adj" fmla="val 53885"/>
+            <a:gd name="adj" fmla="val 50089"/>
           </a:avLst>
         </a:prstGeom>
         <a:solidFill>
@@ -8277,8 +8280,8 @@
         </a:p>
       </dsp:txBody>
       <dsp:txXfrm rot="-10800000">
-        <a:off x="1046368" y="3861964"/>
-        <a:ext cx="3132966" cy="986979"/>
+        <a:off x="969293" y="3848578"/>
+        <a:ext cx="2902194" cy="983557"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -10308,8 +10311,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="B1:W407"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A216" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="M193" sqref="M193"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A129" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="H138" sqref="H138:K138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10337,37 +10340,37 @@
   <sheetData>
     <row r="1" spans="8:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="H1" s="45" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31">
       <c r="D31" t="s" s="100">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="32">
       <c r="D32" t="s" s="100">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="36" spans="7:7" ht="23.25" x14ac:dyDescent="0.35">
       <c r="G36" s="45" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="63">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="63" spans="4:4" ht="19.5" x14ac:dyDescent="0.25">
       <c r="D63" t="s" s="100">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="64">
       <c r="D64" t="s" s="100">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="8:8" ht="23.25" x14ac:dyDescent="0.35">
       <c r="H70" s="45" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="85" spans="8:8" ht="23.25" x14ac:dyDescent="0.35">
@@ -10395,62 +10398,62 @@
     <row r="107" spans="7:17" ht="6.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="110" spans="7:17" ht="21" x14ac:dyDescent="0.35">
       <c r="K110" s="95" t="s">
-        <v>125</v>
-      </c>
-      <c r="L110" s="130"/>
-      <c r="M110" s="130"/>
-      <c r="N110" s="130"/>
-      <c r="O110" s="130"/>
+        <v>128</v>
+      </c>
+      <c r="L110" s="128"/>
+      <c r="M110" s="128"/>
+      <c r="N110" s="128"/>
+      <c r="O110" s="128"/>
     </row>
     <row r="113" spans="9:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="K113" s="95" t="s">
-        <v>126</v>
-      </c>
-      <c r="L113" s="130"/>
-      <c r="M113" s="130"/>
-      <c r="N113" s="130"/>
-      <c r="O113" s="130"/>
+        <v>129</v>
+      </c>
+      <c r="L113" s="128"/>
+      <c r="M113" s="128"/>
+      <c r="N113" s="128"/>
+      <c r="O113" s="128"/>
     </row>
     <row r="116" spans="9:15" ht="21" x14ac:dyDescent="0.35">
       <c r="K116" s="95" t="s">
-        <v>127</v>
-      </c>
-      <c r="L116" s="131"/>
-      <c r="M116" s="131"/>
-      <c r="N116" s="131"/>
-      <c r="O116" s="131"/>
+        <v>130</v>
+      </c>
+      <c r="L116" s="129"/>
+      <c r="M116" s="129"/>
+      <c r="N116" s="129"/>
+      <c r="O116" s="129"/>
     </row>
     <row r="120" spans="9:15" ht="21" x14ac:dyDescent="0.35">
       <c r="K120" s="95" t="s">
-        <v>128</v>
-      </c>
-      <c r="L120" s="130"/>
-      <c r="M120" s="130"/>
-      <c r="N120" s="130"/>
-      <c r="O120" s="130"/>
+        <v>131</v>
+      </c>
+      <c r="L120" s="128"/>
+      <c r="M120" s="128"/>
+      <c r="N120" s="128"/>
+      <c r="O120" s="128"/>
     </row>
     <row r="124" spans="9:15" ht="21" x14ac:dyDescent="0.35">
       <c r="I124" s="19"/>
       <c r="J124" s="19"/>
       <c r="K124" s="95" t="s">
-        <v>129</v>
-      </c>
-      <c r="L124" s="129"/>
-      <c r="M124" s="129"/>
-      <c r="N124" s="129"/>
-      <c r="O124" s="129"/>
+        <v>132</v>
+      </c>
+      <c r="L124" s="127"/>
+      <c r="M124" s="127"/>
+      <c r="N124" s="127"/>
+      <c r="O124" s="127"/>
     </row>
     <row r="127" spans="9:15" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="128" spans="9:15" ht="21" x14ac:dyDescent="0.35">
       <c r="I128" s="95" t="s">
-        <v>130</v>
-      </c>
-      <c r="J128" s="124"/>
-      <c r="K128" s="124"/>
-      <c r="L128" s="124"/>
-      <c r="M128" s="124"/>
-      <c r="N128" s="124"/>
-      <c r="O128" s="124"/>
+        <v>133</v>
+      </c>
+      <c r="J128" s="119"/>
+      <c r="K128" s="119"/>
+      <c r="L128" s="119"/>
+      <c r="M128" s="119"/>
+      <c r="N128" s="119"/>
+      <c r="O128" s="119"/>
     </row>
     <row r="129" spans="6:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K129" s="16"/>
@@ -10461,37 +10464,37 @@
     <row r="134" spans="6:14" ht="41.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="136" spans="6:14" ht="73.5" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="137" spans="6:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="F137" s="125" t="s">
+      <c r="F137" s="120" t="s">
         <v>23</v>
       </c>
-      <c r="G137" s="125"/>
-      <c r="H137" s="125" t="s">
+      <c r="G137" s="120"/>
+      <c r="H137" s="120" t="s">
+        <v>103</v>
+      </c>
+      <c r="I137" s="120"/>
+      <c r="J137" s="120"/>
+      <c r="K137" s="120"/>
+      <c r="L137" s="120" t="s">
         <v>24</v>
       </c>
-      <c r="I137" s="125"/>
-      <c r="J137" s="125"/>
-      <c r="K137" s="125"/>
-      <c r="L137" s="125" t="s">
-        <v>25</v>
-      </c>
-      <c r="M137" s="125"/>
+      <c r="M137" s="120"/>
       <c r="N137" s="49"/>
     </row>
     <row r="138" spans="6:14" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F138" s="98" t="n">
-        <v>8573.725967407227</v>
-      </c>
-      <c r="G138" s="126"/>
+        <v>42726.1796875</v>
+      </c>
+      <c r="G138" s="121"/>
       <c r="H138" s="98" t="n">
-        <v>120910.0</v>
-      </c>
-      <c r="I138" s="126"/>
-      <c r="J138" s="126"/>
-      <c r="K138" s="126"/>
+        <v>345.0</v>
+      </c>
+      <c r="I138" s="121"/>
+      <c r="J138" s="121"/>
+      <c r="K138" s="121"/>
       <c r="L138" s="98" t="n">
-        <v>0.07090998236214727</v>
-      </c>
-      <c r="M138" s="126"/>
+        <v>123.84400177001953</v>
+      </c>
+      <c r="M138" s="121"/>
       <c r="N138" s="50"/>
     </row>
     <row r="139" spans="6:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -10518,143 +10521,143 @@
     </row>
     <row r="141" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F141" s="94" t="n">
-        <v>134.57167053222656</v>
-      </c>
-      <c r="G141" s="132"/>
-      <c r="H141" s="126" t="s">
-        <v>26</v>
-      </c>
-      <c r="I141" s="126"/>
-      <c r="J141" s="126"/>
-      <c r="K141" s="126"/>
+        <v>10725.3701171875</v>
+      </c>
+      <c r="G141" s="130"/>
+      <c r="H141" s="121" t="s">
+        <v>25</v>
+      </c>
+      <c r="I141" s="121"/>
+      <c r="J141" s="121"/>
+      <c r="K141" s="121"/>
       <c r="L141" s="94" t="n">
-        <v>8439.154296875</v>
-      </c>
-      <c r="M141" s="132"/>
+        <v>32000.810546875</v>
+      </c>
+      <c r="M141" s="130"/>
       <c r="N141" s="51"/>
     </row>
     <row r="142" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F142" s="98" t="n">
-        <v>304.0</v>
-      </c>
-      <c r="G142" s="128"/>
-      <c r="H142" s="133" t="s">
-        <v>27</v>
-      </c>
-      <c r="I142" s="133"/>
-      <c r="J142" s="133"/>
-      <c r="K142" s="133"/>
+        <v>6811.0</v>
+      </c>
+      <c r="G142" s="122"/>
+      <c r="H142" s="131" t="s">
+        <v>26</v>
+      </c>
+      <c r="I142" s="131"/>
+      <c r="J142" s="131"/>
+      <c r="K142" s="131"/>
       <c r="L142" s="98" t="n">
-        <v>120606.0</v>
-      </c>
-      <c r="M142" s="128"/>
+        <v>1215103.0</v>
+      </c>
+      <c r="M142" s="122"/>
       <c r="N142" s="51"/>
     </row>
     <row r="143" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F143" s="94" t="n">
-        <v>26.0</v>
-      </c>
-      <c r="G143" s="132"/>
-      <c r="H143" s="126" t="s">
-        <v>28</v>
-      </c>
-      <c r="I143" s="126"/>
-      <c r="J143" s="126"/>
-      <c r="K143" s="126"/>
+        <v>372.0</v>
+      </c>
+      <c r="G143" s="130"/>
+      <c r="H143" s="121" t="s">
+        <v>27</v>
+      </c>
+      <c r="I143" s="121"/>
+      <c r="J143" s="121"/>
+      <c r="K143" s="121"/>
       <c r="L143" s="94" t="n">
-        <v>103.0</v>
-      </c>
-      <c r="M143" s="132"/>
+        <v>951.0</v>
+      </c>
+      <c r="M143" s="130"/>
       <c r="N143" s="51"/>
     </row>
     <row r="144" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F144" s="98" t="s">
-        <v>131</v>
-      </c>
-      <c r="G144" s="128"/>
-      <c r="H144" s="133" t="s">
-        <v>29</v>
-      </c>
-      <c r="I144" s="133"/>
-      <c r="J144" s="133"/>
-      <c r="K144" s="133"/>
-      <c r="L144" s="98" t="s">
-        <v>132</v>
-      </c>
-      <c r="M144" s="128"/>
+      <c r="F144" s="98" t="n">
+        <v>5.461753046542358</v>
+      </c>
+      <c r="G144" s="122"/>
+      <c r="H144" s="131" t="s">
+        <v>101</v>
+      </c>
+      <c r="I144" s="131"/>
+      <c r="J144" s="131"/>
+      <c r="K144" s="131"/>
+      <c r="L144" s="98" t="n">
+        <v>0.0782649701301042</v>
+      </c>
+      <c r="M144" s="122"/>
       <c r="N144" s="51"/>
     </row>
     <row r="145" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F145" s="94" t="n">
-        <v>5.175833225250244</v>
-      </c>
-      <c r="G145" s="132"/>
-      <c r="H145" s="126" t="s">
-        <v>30</v>
-      </c>
-      <c r="I145" s="126"/>
-      <c r="J145" s="126"/>
-      <c r="K145" s="126"/>
-      <c r="L145" s="94" t="s">
-        <v>133</v>
-      </c>
-      <c r="M145" s="132"/>
+        <v>28.831640243530273</v>
+      </c>
+      <c r="G145" s="130"/>
+      <c r="H145" s="121" t="s">
+        <v>29</v>
+      </c>
+      <c r="I145" s="121"/>
+      <c r="J145" s="121"/>
+      <c r="K145" s="121"/>
+      <c r="L145" s="94" t="n">
+        <v>33.64964294433594</v>
+      </c>
+      <c r="M145" s="130"/>
       <c r="N145" s="51"/>
     </row>
     <row r="146" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F146" s="98" t="n">
-        <v>225.0</v>
-      </c>
-      <c r="G146" s="128"/>
-      <c r="H146" s="133" t="s">
-        <v>31</v>
-      </c>
-      <c r="I146" s="133"/>
-      <c r="J146" s="133"/>
-      <c r="K146" s="133"/>
+        <v>111.0</v>
+      </c>
+      <c r="G146" s="122"/>
+      <c r="H146" s="131" t="s">
+        <v>30</v>
+      </c>
+      <c r="I146" s="131"/>
+      <c r="J146" s="131"/>
+      <c r="K146" s="131"/>
       <c r="L146" s="98" t="n">
-        <v>436.010009765625</v>
-      </c>
-      <c r="M146" s="128"/>
+        <v>234.0</v>
+      </c>
+      <c r="M146" s="122"/>
       <c r="N146" s="51"/>
     </row>
     <row r="147" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="F147" s="94" t="s">
-        <v>134</v>
-      </c>
-      <c r="G147" s="132"/>
-      <c r="H147" s="126" t="s">
-        <v>32</v>
-      </c>
-      <c r="I147" s="126"/>
-      <c r="J147" s="126"/>
-      <c r="K147" s="126"/>
-      <c r="L147" s="94" t="s">
-        <v>135</v>
-      </c>
-      <c r="M147" s="132"/>
+      <c r="F147" s="94" t="n">
+        <v>29.838709677419356</v>
+      </c>
+      <c r="G147" s="130"/>
+      <c r="H147" s="121" t="s">
+        <v>102</v>
+      </c>
+      <c r="I147" s="121"/>
+      <c r="J147" s="121"/>
+      <c r="K147" s="121"/>
+      <c r="L147" s="94" t="n">
+        <v>24.605678233438486</v>
+      </c>
+      <c r="M147" s="130"/>
       <c r="N147" s="51"/>
     </row>
     <row r="148" spans="6:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F148" s="98" t="n">
-        <v>8.619999885559082</v>
-      </c>
-      <c r="G148" s="128"/>
-      <c r="H148" s="133" t="s">
-        <v>33</v>
-      </c>
-      <c r="I148" s="133"/>
-      <c r="J148" s="133"/>
-      <c r="K148" s="133"/>
+        <v>3291.81005859375</v>
+      </c>
+      <c r="G148" s="122"/>
+      <c r="H148" s="131" t="s">
+        <v>31</v>
+      </c>
+      <c r="I148" s="131"/>
+      <c r="J148" s="131"/>
+      <c r="K148" s="131"/>
       <c r="L148" s="98" t="n">
-        <v>81.11000061035156</v>
-      </c>
-      <c r="M148" s="128"/>
+        <v>16487.75</v>
+      </c>
+      <c r="M148" s="122"/>
       <c r="N148" s="51"/>
     </row>
     <row r="162" spans="5:23" ht="23.25" x14ac:dyDescent="0.25">
       <c r="H162" s="22" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="166" spans="5:23" ht="23.25" x14ac:dyDescent="0.25">
@@ -10679,12 +10682,12 @@
     </row>
     <row r="191">
       <c r="E191" t="s" s="100">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="192">
       <c r="E192" t="s" s="100">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="195" spans="2:23" ht="21" x14ac:dyDescent="0.35">
@@ -10712,30 +10715,30 @@
     </row>
     <row r="196" spans="2:23" ht="23.25" x14ac:dyDescent="0.25">
       <c r="H196" s="22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="203" spans="2:23" ht="21" x14ac:dyDescent="0.35">
+      <c r="D203" s="123" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="203" spans="2:23" ht="21" x14ac:dyDescent="0.35">
-      <c r="D203" s="112" t="s">
-        <v>39</v>
-      </c>
-      <c r="E203" s="112"/>
-      <c r="F203" s="112"/>
-      <c r="G203" s="113"/>
-      <c r="H203" s="114" t="s">
+      <c r="E203" s="123"/>
+      <c r="F203" s="123"/>
+      <c r="G203" s="124"/>
+      <c r="H203" s="125" t="s">
+        <v>36</v>
+      </c>
+      <c r="I203" s="123"/>
+      <c r="J203" s="123"/>
+      <c r="K203" s="126"/>
+      <c r="L203" s="141" t="s">
         <v>38</v>
       </c>
-      <c r="I203" s="112"/>
-      <c r="J203" s="112"/>
-      <c r="K203" s="115"/>
-      <c r="L203" s="116" t="s">
-        <v>40</v>
-      </c>
-      <c r="M203" s="112"/>
-      <c r="N203" s="112"/>
-      <c r="O203" s="112"/>
-      <c r="P203" s="112"/>
-      <c r="Q203" s="115"/>
+      <c r="M203" s="123"/>
+      <c r="N203" s="123"/>
+      <c r="O203" s="123"/>
+      <c r="P203" s="123"/>
+      <c r="Q203" s="126"/>
     </row>
     <row r="204" spans="2:23" x14ac:dyDescent="0.25">
       <c r="E204" s="26"/>
@@ -10823,86 +10826,86 @@
       <c r="B211" s="52"/>
       <c r="C211" s="52"/>
       <c r="D211" s="55" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E211" s="110"/>
       <c r="F211" s="99" t="n">
-        <v>160.0</v>
-      </c>
-      <c r="G211" s="120"/>
+        <v>1628.0</v>
+      </c>
+      <c r="G211" s="115"/>
       <c r="H211" s="53"/>
       <c r="I211" s="99" t="n">
-        <v>64.0</v>
-      </c>
-      <c r="J211" s="120"/>
-      <c r="K211" s="120"/>
+        <v>479.0</v>
+      </c>
+      <c r="J211" s="115"/>
+      <c r="K211" s="115"/>
       <c r="L211" s="60"/>
       <c r="M211" s="53"/>
       <c r="N211" s="53"/>
       <c r="O211" s="99" t="n">
-        <v>33.0</v>
-      </c>
-      <c r="P211" s="120"/>
-      <c r="Q211" s="120"/>
+        <v>200.0</v>
+      </c>
+      <c r="P211" s="115"/>
+      <c r="Q211" s="115"/>
     </row>
     <row r="212" spans="2:17" ht="21" x14ac:dyDescent="0.35">
       <c r="B212" s="52"/>
       <c r="C212" s="52"/>
       <c r="D212" s="56" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E212" s="111"/>
       <c r="F212" s="95" t="n">
-        <v>53.0</v>
-      </c>
-      <c r="G212" s="119"/>
+        <v>617.0</v>
+      </c>
+      <c r="G212" s="114"/>
       <c r="H212" s="54"/>
       <c r="I212" s="95" t="n">
-        <v>25.0</v>
-      </c>
-      <c r="J212" s="119"/>
-      <c r="K212" s="119"/>
+        <v>128.0</v>
+      </c>
+      <c r="J212" s="114"/>
+      <c r="K212" s="114"/>
       <c r="L212" s="61"/>
       <c r="M212" s="54"/>
       <c r="N212" s="54"/>
       <c r="O212" s="95" t="n">
-        <v>7.0</v>
-      </c>
-      <c r="P212" s="119"/>
-      <c r="Q212" s="119"/>
+        <v>49.0</v>
+      </c>
+      <c r="P212" s="114"/>
+      <c r="Q212" s="114"/>
     </row>
     <row r="213" spans="2:17" ht="18.75" x14ac:dyDescent="0.25">
       <c r="D213" s="55" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E213" s="110"/>
       <c r="F213" s="99" t="n">
-        <v>62.01550387596899</v>
-      </c>
-      <c r="G213" s="120"/>
+        <v>70.44569450454348</v>
+      </c>
+      <c r="G213" s="115"/>
       <c r="H213" s="53"/>
       <c r="I213" s="99" t="n">
-        <v>24.8062015503876</v>
-      </c>
-      <c r="J213" s="120"/>
-      <c r="K213" s="120"/>
+        <v>20.726958026828214</v>
+      </c>
+      <c r="J213" s="115"/>
+      <c r="K213" s="115"/>
       <c r="L213" s="60"/>
       <c r="M213" s="53"/>
       <c r="N213" s="53"/>
       <c r="O213" s="99" t="n">
-        <v>12.790697674418606</v>
-      </c>
-      <c r="P213" s="120"/>
-      <c r="Q213" s="120"/>
+        <v>8.654262224145391</v>
+      </c>
+      <c r="P213" s="115"/>
+      <c r="Q213" s="115"/>
     </row>
     <row r="215" spans="2:17" x14ac:dyDescent="0.25">
       <c r="D215" t="s" s="100">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="229" spans="8:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="H229" s="22" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J229" s="23"/>
       <c r="K229" s="23"/>
@@ -10912,7 +10915,7 @@
     </row>
     <row r="259" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D259" s="100" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E259" s="58"/>
       <c r="F259" s="58"/>
@@ -10922,7 +10925,7 @@
     </row>
     <row r="260" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
       <c r="D260" s="100" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E260" s="58"/>
       <c r="F260" s="58"/>
@@ -10932,7 +10935,7 @@
     </row>
     <row r="263" spans="2:14" ht="23.25" x14ac:dyDescent="0.35">
       <c r="H263" s="22" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="I263" s="23"/>
       <c r="J263" s="23"/>
@@ -10942,17 +10945,17 @@
       <c r="N263" s="24"/>
     </row>
     <row r="266" spans="2:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="B266" s="127" t="s">
-        <v>51</v>
-      </c>
-      <c r="C266" s="127"/>
-      <c r="D266" s="127"/>
+      <c r="B266" s="136" t="s">
+        <v>49</v>
+      </c>
+      <c r="C266" s="136"/>
+      <c r="D266" s="136"/>
       <c r="E266" s="44"/>
       <c r="F266" s="44"/>
-      <c r="G266" s="127" t="s">
-        <v>52</v>
-      </c>
-      <c r="H266" s="127"/>
+      <c r="G266" s="136" t="s">
+        <v>50</v>
+      </c>
+      <c r="H266" s="136"/>
     </row>
     <row r="267" spans="2:14" x14ac:dyDescent="0.25">
       <c r="E267" s="36"/>
@@ -10991,27 +10994,27 @@
       <c r="E278" s="36"/>
     </row>
     <row r="279" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B279" s="139" t="s">
-        <v>55</v>
-      </c>
-      <c r="C279" s="139"/>
-      <c r="D279" s="139"/>
+      <c r="B279" s="138" t="s">
+        <v>53</v>
+      </c>
+      <c r="C279" s="138"/>
+      <c r="D279" s="138"/>
       <c r="E279" s="36"/>
-      <c r="G279" s="139" t="s">
-        <v>55</v>
-      </c>
-      <c r="H279" s="139"/>
+      <c r="G279" s="138" t="s">
+        <v>53</v>
+      </c>
+      <c r="H279" s="138"/>
     </row>
     <row r="280" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B280" s="101" t="n">
-        <v>29.20353982300885</v>
-      </c>
-      <c r="C280" s="138"/>
-      <c r="D280" s="138"/>
+        <v>35.91269841269841</v>
+      </c>
+      <c r="C280" s="137"/>
+      <c r="D280" s="137"/>
       <c r="G280" s="101" t="n">
-        <v>43.56435643564357</v>
-      </c>
-      <c r="H280" s="138"/>
+        <v>36.60418963616318</v>
+      </c>
+      <c r="H280" s="137"/>
     </row>
     <row r="282" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C282" s="25"/>
@@ -11025,17 +11028,17 @@
     </row>
     <row r="284" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B284" s="100" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="285" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B285" s="100" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="296" spans="8:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="H296" s="63" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="297" spans="8:13" ht="23.25" x14ac:dyDescent="0.35">
@@ -11047,12 +11050,12 @@
     </row>
     <row r="325">
       <c r="D325" t="s" s="100">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="326">
       <c r="D326" t="s" s="100">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="327" spans="4:13" ht="21" x14ac:dyDescent="0.35">
@@ -11079,7 +11082,7 @@
     </row>
     <row r="329" spans="4:13" ht="23.25" x14ac:dyDescent="0.35">
       <c r="H329" s="63" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="331" spans="4:13" ht="21" x14ac:dyDescent="0.35">
@@ -11090,7 +11093,7 @@
     </row>
     <row r="358">
       <c r="D358" t="s" s="100">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="361" spans="4:15" ht="18.75" x14ac:dyDescent="0.3">
@@ -11106,7 +11109,7 @@
     </row>
     <row r="365" spans="4:15" ht="23.25" x14ac:dyDescent="0.35">
       <c r="H365" s="63" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="366" spans="4:15" ht="4.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
@@ -11122,92 +11125,92 @@
     <row r="367" spans="4:15" ht="7.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="368" spans="4:15" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="370" spans="2:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B370" s="122" t="s">
-        <v>72</v>
-      </c>
-      <c r="C370" s="122"/>
-      <c r="D370" s="122"/>
-      <c r="E370" s="122"/>
-      <c r="F370" s="122"/>
-      <c r="G370" s="122"/>
+      <c r="B370" s="117" t="s">
+        <v>70</v>
+      </c>
+      <c r="C370" s="117"/>
+      <c r="D370" s="117"/>
+      <c r="E370" s="117"/>
+      <c r="F370" s="117"/>
+      <c r="G370" s="117"/>
       <c r="H370" t="n" s="99">
         <v>40.0</v>
       </c>
-      <c r="I370" s="134"/>
+      <c r="I370" s="132"/>
     </row>
     <row r="371" spans="2:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B371" s="136" t="s">
-        <v>73</v>
-      </c>
-      <c r="C371" s="136"/>
-      <c r="D371" s="136"/>
-      <c r="E371" s="136"/>
-      <c r="F371" s="136"/>
-      <c r="G371" s="136"/>
+      <c r="B371" s="134" t="s">
+        <v>71</v>
+      </c>
+      <c r="C371" s="134"/>
+      <c r="D371" s="134"/>
+      <c r="E371" s="134"/>
+      <c r="F371" s="134"/>
+      <c r="G371" s="134"/>
       <c r="H371" t="n" s="95">
-        <v>19.0</v>
-      </c>
-      <c r="I371" s="135"/>
+        <v>18.0</v>
+      </c>
+      <c r="I371" s="133"/>
     </row>
     <row r="372" spans="2:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B372" s="137" t="s">
-        <v>74</v>
-      </c>
-      <c r="C372" s="137"/>
-      <c r="D372" s="137"/>
-      <c r="E372" s="137"/>
-      <c r="F372" s="137"/>
-      <c r="G372" s="137"/>
+      <c r="B372" s="135" t="s">
+        <v>72</v>
+      </c>
+      <c r="C372" s="135"/>
+      <c r="D372" s="135"/>
+      <c r="E372" s="135"/>
+      <c r="F372" s="135"/>
+      <c r="G372" s="135"/>
       <c r="H372" t="n" s="99">
-        <v>47.5</v>
-      </c>
-      <c r="I372" s="134"/>
+        <v>45.0</v>
+      </c>
+      <c r="I372" s="132"/>
     </row>
     <row r="376" spans="2:18" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K376" s="122" t="s">
-        <v>97</v>
-      </c>
-      <c r="L376" s="122"/>
-      <c r="M376" s="122"/>
-      <c r="N376" s="122"/>
-      <c r="O376" s="122"/>
+      <c r="K376" s="117" t="s">
+        <v>95</v>
+      </c>
+      <c r="L376" s="117"/>
+      <c r="M376" s="117"/>
+      <c r="N376" s="117"/>
+      <c r="O376" s="117"/>
       <c r="P376" t="n" s="99">
-        <v>8.432134913892863</v>
-      </c>
-      <c r="Q376" s="123"/>
-      <c r="R376" s="123"/>
+        <v>8.412686038395297</v>
+      </c>
+      <c r="Q376" s="118"/>
+      <c r="R376" s="118"/>
     </row>
     <row r="377" spans="2:18" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K377" s="121" t="s">
-        <v>96</v>
-      </c>
-      <c r="L377" s="121"/>
-      <c r="M377" s="121"/>
-      <c r="N377" s="121"/>
-      <c r="O377" s="121"/>
+      <c r="K377" s="116" t="s">
+        <v>94</v>
+      </c>
+      <c r="L377" s="116"/>
+      <c r="M377" s="116"/>
+      <c r="N377" s="116"/>
+      <c r="O377" s="116"/>
       <c r="P377" t="n" s="95">
-        <v>4.00516885342107</v>
-      </c>
-      <c r="Q377" s="140"/>
-      <c r="R377" s="140"/>
+        <v>3.8844839191140155</v>
+      </c>
+      <c r="Q377" s="139"/>
+      <c r="R377" s="139"/>
     </row>
     <row r="378" spans="2:18" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K378" s="122" t="s">
-        <v>95</v>
-      </c>
-      <c r="L378" s="122"/>
-      <c r="M378" s="122"/>
-      <c r="N378" s="122"/>
-      <c r="O378" s="122"/>
+      <c r="K378" s="117" t="s">
+        <v>93</v>
+      </c>
+      <c r="L378" s="117"/>
+      <c r="M378" s="117"/>
+      <c r="N378" s="117"/>
+      <c r="O378" s="117"/>
       <c r="P378" t="n" s="99">
-        <v>47.49887062198349</v>
-      </c>
-      <c r="Q378" s="141"/>
-      <c r="R378" s="141"/>
+        <v>46.17412205073771</v>
+      </c>
+      <c r="Q378" s="140"/>
+      <c r="R378" s="140"/>
     </row>
     <row r="388" spans="2:20" ht="23.25" x14ac:dyDescent="0.35">
       <c r="H388" s="63" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="I388" s="63"/>
       <c r="J388" s="63"/>
@@ -11217,50 +11220,50 @@
       <c r="N388" s="40"/>
     </row>
     <row r="391" spans="2:20" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B391" s="117" t="s">
+      <c r="B391" s="112" t="s">
+        <v>82</v>
+      </c>
+      <c r="C391" s="112"/>
+      <c r="D391" s="112"/>
+      <c r="E391" s="112"/>
+      <c r="F391" s="112" t="s">
+        <v>83</v>
+      </c>
+      <c r="G391" s="112"/>
+      <c r="H391" s="112"/>
+      <c r="I391" s="112" t="s">
         <v>84</v>
       </c>
-      <c r="C391" s="117"/>
-      <c r="D391" s="117"/>
-      <c r="E391" s="117"/>
-      <c r="F391" s="117" t="s">
+      <c r="J391" s="112"/>
+      <c r="K391" s="73" t="s">
+        <v>90</v>
+      </c>
+      <c r="L391" s="113" t="s">
         <v>85</v>
       </c>
-      <c r="G391" s="117"/>
-      <c r="H391" s="117"/>
-      <c r="I391" s="117" t="s">
+      <c r="M391" s="113"/>
+      <c r="N391" s="113" t="s">
+        <v>91</v>
+      </c>
+      <c r="O391" s="113"/>
+      <c r="P391" s="112" t="s">
         <v>86</v>
       </c>
-      <c r="J391" s="117"/>
-      <c r="K391" s="73" t="s">
+      <c r="Q391" s="112"/>
+      <c r="R391" s="74" t="s">
+        <v>28</v>
+      </c>
+      <c r="S391" s="113" t="s">
         <v>92</v>
       </c>
-      <c r="L391" s="118" t="s">
-        <v>87</v>
-      </c>
-      <c r="M391" s="118"/>
-      <c r="N391" s="118" t="s">
-        <v>93</v>
-      </c>
-      <c r="O391" s="118"/>
-      <c r="P391" s="117" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q391" s="117"/>
-      <c r="R391" s="74" t="s">
-        <v>29</v>
-      </c>
-      <c r="S391" s="118" t="s">
-        <v>94</v>
-      </c>
-      <c r="T391" s="118"/>
+      <c r="T391" s="113"/>
     </row>
     <row r="392">
       <c r="B392" t="s" s="75">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="F392" t="s" s="75">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I392" t="n" s="75">
         <v>20.0</v>
@@ -11286,18 +11289,18 @@
     </row>
     <row r="393" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B393" t="s" s="106">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="C393" s="72"/>
       <c r="D393" s="72"/>
       <c r="E393" s="72"/>
       <c r="F393" t="s" s="106">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G393" s="72"/>
       <c r="H393" s="72"/>
       <c r="I393" t="n" s="106">
-        <v>20.0</v>
+        <v>22.0</v>
       </c>
       <c r="J393" s="72"/>
       <c r="K393" t="n" s="106">
@@ -11312,11 +11315,11 @@
       </c>
       <c r="O393" s="72"/>
       <c r="P393" t="n" s="106">
-        <v>200.27115127779632</v>
+        <v>200.2318945819982</v>
       </c>
       <c r="Q393" s="72"/>
       <c r="R393" t="n" s="106">
-        <v>0.09900990099009901</v>
+        <v>0.11</v>
       </c>
       <c r="S393" t="e" s="106">
         <v>#DIV/0!</v>
@@ -11325,22 +11328,22 @@
     </row>
     <row r="394" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B394" t="s" s="75">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C394" s="72"/>
       <c r="D394" s="72"/>
       <c r="E394" s="72"/>
       <c r="F394" t="s" s="75">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="G394" s="72"/>
       <c r="H394" s="72"/>
       <c r="I394" t="n" s="75">
-        <v>20.0</v>
+        <v>41.0</v>
       </c>
       <c r="J394" s="72"/>
       <c r="K394" t="n" s="75">
-        <v>9.0</v>
+        <v>21.0</v>
       </c>
       <c r="L394" t="n" s="75">
         <v>0.0</v>
@@ -11351,11 +11354,11 @@
       </c>
       <c r="O394" s="72"/>
       <c r="P394" t="n" s="75">
-        <v>200.50758166174148</v>
+        <v>200.77034482105316</v>
       </c>
       <c r="Q394" s="72"/>
       <c r="R394" t="n" s="75">
-        <v>0.09569377990430622</v>
+        <v>0.18552036199095023</v>
       </c>
       <c r="S394" t="e" s="75">
         <v>#DIV/0!</v>
@@ -11364,22 +11367,22 @@
     </row>
     <row r="395" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B395" t="s" s="106">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="C395" s="72"/>
       <c r="D395" s="72"/>
       <c r="E395" s="72"/>
       <c r="F395" t="s" s="106">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G395" s="72"/>
       <c r="H395" s="72"/>
       <c r="I395" t="n" s="106">
-        <v>20.0</v>
+        <v>21.0</v>
       </c>
       <c r="J395" s="72"/>
       <c r="K395" t="n" s="106">
-        <v>12.0</v>
+        <v>1.0</v>
       </c>
       <c r="L395" t="n" s="106">
         <v>0.0</v>
@@ -11390,11 +11393,11 @@
       </c>
       <c r="O395" s="72"/>
       <c r="P395" t="n" s="106">
-        <v>200.83821110502524</v>
+        <v>200.85165462381937</v>
       </c>
       <c r="Q395" s="72"/>
       <c r="R395" t="n" s="106">
-        <v>0.1</v>
+        <v>0.105</v>
       </c>
       <c r="S395" t="e" s="106">
         <v>#DIV/0!</v>
@@ -11403,13 +11406,13 @@
     </row>
     <row r="396" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B396" t="s" s="75">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C396" s="72"/>
       <c r="D396" s="72"/>
       <c r="E396" s="72"/>
       <c r="F396" t="s" s="75">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="G396" s="72"/>
       <c r="H396" s="72"/>
@@ -11418,7 +11421,7 @@
       </c>
       <c r="J396" s="72"/>
       <c r="K396" t="n" s="75">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="L396" t="n" s="75">
         <v>0.0</v>
@@ -11429,11 +11432,11 @@
       </c>
       <c r="O396" s="72"/>
       <c r="P396" t="n" s="75">
-        <v>202.2229957947878</v>
+        <v>201.01351845868186</v>
       </c>
       <c r="Q396" s="72"/>
       <c r="R396" t="n" s="75">
-        <v>0.09803921568627451</v>
+        <v>0.1</v>
       </c>
       <c r="S396" t="e" s="75">
         <v>#DIV/0!</v>
@@ -11442,22 +11445,22 @@
     </row>
     <row r="397" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B397" t="s" s="106">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="C397" s="72"/>
       <c r="D397" s="72"/>
       <c r="E397" s="72"/>
       <c r="F397" t="s" s="106">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="G397" s="72"/>
       <c r="H397" s="72"/>
       <c r="I397" t="n" s="106">
-        <v>37.0</v>
+        <v>32.0</v>
       </c>
       <c r="J397" s="72"/>
       <c r="K397" t="n" s="106">
-        <v>17.0</v>
+        <v>12.0</v>
       </c>
       <c r="L397" t="n" s="106">
         <v>0.0</v>
@@ -11468,11 +11471,11 @@
       </c>
       <c r="O397" s="72"/>
       <c r="P397" t="n" s="106">
-        <v>203.21111547220062</v>
+        <v>201.13715678313164</v>
       </c>
       <c r="Q397" s="72"/>
       <c r="R397" t="n" s="106">
-        <v>0.185</v>
+        <v>0.16</v>
       </c>
       <c r="S397" t="e" s="106">
         <v>#DIV/0!</v>
@@ -11481,13 +11484,13 @@
     </row>
     <row r="398" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B398" t="s" s="75">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C398" s="72"/>
       <c r="D398" s="72"/>
       <c r="E398" s="72"/>
       <c r="F398" t="s" s="75">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G398" s="72"/>
       <c r="H398" s="72"/>
@@ -11496,7 +11499,7 @@
       </c>
       <c r="J398" s="72"/>
       <c r="K398" t="n" s="75">
-        <v>5.0</v>
+        <v>38.0</v>
       </c>
       <c r="L398" t="n" s="75">
         <v>0.0</v>
@@ -11507,7 +11510,7 @@
       </c>
       <c r="O398" s="72"/>
       <c r="P398" t="n" s="75">
-        <v>204.41718498684304</v>
+        <v>201.29367928154147</v>
       </c>
       <c r="Q398" s="72"/>
       <c r="R398" t="n" s="75">
@@ -11520,22 +11523,22 @@
     </row>
     <row r="399" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B399" t="s" s="106">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="C399" s="72"/>
       <c r="D399" s="72"/>
       <c r="E399" s="72"/>
       <c r="F399" t="s" s="106">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="G399" s="72"/>
       <c r="H399" s="72"/>
       <c r="I399" t="n" s="106">
-        <v>20.0</v>
+        <v>25.0</v>
       </c>
       <c r="J399" s="72"/>
       <c r="K399" t="n" s="106">
-        <v>37.0</v>
+        <v>5.0</v>
       </c>
       <c r="L399" t="n" s="106">
         <v>0.0</v>
@@ -11546,11 +11549,11 @@
       </c>
       <c r="O399" s="72"/>
       <c r="P399" t="n" s="106">
-        <v>204.5833943540974</v>
+        <v>201.6427625480135</v>
       </c>
       <c r="Q399" s="72"/>
       <c r="R399" t="n" s="106">
-        <v>0.1</v>
+        <v>0.125</v>
       </c>
       <c r="S399" t="e" s="106">
         <v>#DIV/0!</v>
@@ -11559,22 +11562,22 @@
     </row>
     <row r="400" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B400" t="s" s="75">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C400" s="72"/>
       <c r="D400" s="72"/>
       <c r="E400" s="72"/>
       <c r="F400" t="s" s="75">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="G400" s="72"/>
       <c r="H400" s="72"/>
       <c r="I400" t="n" s="75">
-        <v>30.0</v>
+        <v>20.0</v>
       </c>
       <c r="J400" s="72"/>
       <c r="K400" t="n" s="75">
-        <v>10.0</v>
+        <v>14.0</v>
       </c>
       <c r="L400" t="n" s="75">
         <v>0.0</v>
@@ -11585,11 +11588,11 @@
       </c>
       <c r="O400" s="72"/>
       <c r="P400" t="n" s="75">
-        <v>206.63090715523134</v>
+        <v>201.85030248539763</v>
       </c>
       <c r="Q400" s="72"/>
       <c r="R400" t="n" s="75">
-        <v>0.14285714285714285</v>
+        <v>0.1</v>
       </c>
       <c r="S400" t="e" s="75">
         <v>#DIV/0!</v>
@@ -11598,13 +11601,13 @@
     </row>
     <row r="401" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B401" t="s" s="106">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C401" s="72"/>
       <c r="D401" s="72"/>
       <c r="E401" s="72"/>
       <c r="F401" t="s" s="106">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="G401" s="72"/>
       <c r="H401" s="72"/>
@@ -11613,7 +11616,7 @@
       </c>
       <c r="J401" s="72"/>
       <c r="K401" t="n" s="106">
-        <v>21.0</v>
+        <v>9.0</v>
       </c>
       <c r="L401" t="n" s="106">
         <v>0.0</v>
@@ -11624,7 +11627,7 @@
       </c>
       <c r="O401" s="72"/>
       <c r="P401" t="n" s="106">
-        <v>206.93729166221215</v>
+        <v>202.00484307300738</v>
       </c>
       <c r="Q401" s="72"/>
       <c r="R401" t="n" s="106">
@@ -11637,22 +11640,22 @@
     </row>
     <row r="402" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B402" t="s" s="75">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C402" s="72"/>
       <c r="D402" s="72"/>
       <c r="E402" s="72"/>
       <c r="F402" t="s" s="75">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="G402" s="72"/>
       <c r="H402" s="72"/>
       <c r="I402" t="n" s="75">
-        <v>20.0</v>
+        <v>47.0</v>
       </c>
       <c r="J402" s="72"/>
       <c r="K402" t="n" s="75">
-        <v>31.0</v>
+        <v>27.0</v>
       </c>
       <c r="L402" t="n" s="75">
         <v>0.0</v>
@@ -11663,11 +11666,11 @@
       </c>
       <c r="O402" s="72"/>
       <c r="P402" t="n" s="75">
-        <v>207.2150669472843</v>
+        <v>202.9067858061243</v>
       </c>
       <c r="Q402" s="72"/>
       <c r="R402" t="n" s="75">
-        <v>0.08658008658008658</v>
+        <v>0.235</v>
       </c>
       <c r="S402" t="e" s="75">
         <v>#DIV/0!</v>
@@ -11676,22 +11679,22 @@
     </row>
     <row r="403" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B403" t="s" s="106">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="C403" s="72"/>
       <c r="D403" s="72"/>
       <c r="E403" s="72"/>
       <c r="F403" t="s" s="106">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="G403" s="72"/>
       <c r="H403" s="72"/>
       <c r="I403" t="n" s="106">
-        <v>34.0</v>
+        <v>20.0</v>
       </c>
       <c r="J403" s="72"/>
       <c r="K403" t="n" s="106">
-        <v>14.0</v>
+        <v>4.0</v>
       </c>
       <c r="L403" t="n" s="106">
         <v>0.0</v>
@@ -11702,11 +11705,11 @@
       </c>
       <c r="O403" s="72"/>
       <c r="P403" t="n" s="106">
-        <v>209.16695849871326</v>
+        <v>203.71767543442084</v>
       </c>
       <c r="Q403" s="72"/>
       <c r="R403" t="n" s="106">
-        <v>0.17</v>
+        <v>0.1</v>
       </c>
       <c r="S403" t="e" s="106">
         <v>#DIV/0!</v>
@@ -11715,13 +11718,13 @@
     </row>
     <row r="404" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B404" t="s" s="75">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C404" s="72"/>
       <c r="D404" s="72"/>
       <c r="E404" s="72"/>
       <c r="F404" t="s" s="75">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="G404" s="72"/>
       <c r="H404" s="72"/>
@@ -11730,7 +11733,7 @@
       </c>
       <c r="J404" s="72"/>
       <c r="K404" t="n" s="75">
-        <v>11.0</v>
+        <v>8.0</v>
       </c>
       <c r="L404" t="n" s="75">
         <v>0.0</v>
@@ -11741,11 +11744,11 @@
       </c>
       <c r="O404" s="72"/>
       <c r="P404" t="n" s="75">
-        <v>210.16568436417663</v>
+        <v>203.94785400582757</v>
       </c>
       <c r="Q404" s="72"/>
       <c r="R404" t="n" s="75">
-        <v>0.1</v>
+        <v>0.09615384615384616</v>
       </c>
       <c r="S404" t="e" s="75">
         <v>#DIV/0!</v>
@@ -11754,22 +11757,22 @@
     </row>
     <row r="405" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B405" t="s" s="106">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="C405" s="72"/>
       <c r="D405" s="72"/>
       <c r="E405" s="72"/>
       <c r="F405" t="s" s="106">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G405" s="72"/>
       <c r="H405" s="72"/>
       <c r="I405" t="n" s="106">
-        <v>20.0</v>
+        <v>44.0</v>
       </c>
       <c r="J405" s="72"/>
       <c r="K405" t="n" s="106">
-        <v>26.0</v>
+        <v>24.0</v>
       </c>
       <c r="L405" t="n" s="106">
         <v>0.0</v>
@@ -11780,11 +11783,11 @@
       </c>
       <c r="O405" s="72"/>
       <c r="P405" t="n" s="106">
-        <v>213.63527902505842</v>
+        <v>204.76358258830473</v>
       </c>
       <c r="Q405" s="72"/>
       <c r="R405" t="n" s="106">
-        <v>0.08849557522123894</v>
+        <v>0.22</v>
       </c>
       <c r="S405" t="e" s="106">
         <v>#DIV/0!</v>
@@ -11793,22 +11796,22 @@
     </row>
     <row r="406" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B406" t="s" s="75">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C406" s="72"/>
       <c r="D406" s="72"/>
       <c r="E406" s="72"/>
       <c r="F406" t="s" s="75">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G406" s="72"/>
       <c r="H406" s="72"/>
       <c r="I406" t="n" s="75">
-        <v>48.0</v>
+        <v>20.0</v>
       </c>
       <c r="J406" s="72"/>
       <c r="K406" t="n" s="75">
-        <v>28.0</v>
+        <v>6.0</v>
       </c>
       <c r="L406" t="n" s="75">
         <v>0.0</v>
@@ -11819,11 +11822,11 @@
       </c>
       <c r="O406" s="72"/>
       <c r="P406" t="n" s="75">
-        <v>217.62270883817868</v>
+        <v>205.84458457135042</v>
       </c>
       <c r="Q406" s="72"/>
       <c r="R406" t="n" s="75">
-        <v>0.21052631578947367</v>
+        <v>0.1</v>
       </c>
       <c r="S406" t="e" s="75">
         <v>#DIV/0!</v>
@@ -11832,22 +11835,22 @@
     </row>
     <row r="407" spans="2:20" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B407" t="s" s="106">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="C407" s="72"/>
       <c r="D407" s="72"/>
       <c r="E407" s="72"/>
       <c r="F407" t="s" s="106">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G407" s="72"/>
       <c r="H407" s="72"/>
       <c r="I407" t="n" s="106">
-        <v>54.0</v>
+        <v>39.0</v>
       </c>
       <c r="J407" s="72"/>
       <c r="K407" t="n" s="106">
-        <v>34.0</v>
+        <v>19.0</v>
       </c>
       <c r="L407" t="n" s="106">
         <v>0.0</v>
@@ -11858,11 +11861,11 @@
       </c>
       <c r="O407" s="72"/>
       <c r="P407" t="n" s="106">
-        <v>218.80423391235743</v>
+        <v>206.81612201909155</v>
       </c>
       <c r="Q407" s="72"/>
       <c r="R407" t="n" s="106">
-        <v>0.27</v>
+        <v>0.195</v>
       </c>
       <c r="S407" t="e" s="106">
         <v>#DIV/0!</v>
@@ -11871,16 +11874,16 @@
     </row>
     <row r="408">
       <c r="B408" t="s" s="75">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="F408" t="s" s="75">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="I408" t="n" s="75">
+        <v>40.0</v>
+      </c>
+      <c r="K408" t="n" s="75">
         <v>20.0</v>
-      </c>
-      <c r="K408" t="n" s="75">
-        <v>23.0</v>
       </c>
       <c r="L408" t="n" s="75">
         <v>0.0</v>
@@ -11889,10 +11892,10 @@
         <v>0.0</v>
       </c>
       <c r="P408" t="n" s="75">
-        <v>220.37946694522722</v>
+        <v>207.60488296643686</v>
       </c>
       <c r="R408" t="n" s="75">
-        <v>0.08968609865470852</v>
+        <v>0.18181818181818182</v>
       </c>
       <c r="S408" t="e" s="75">
         <v>#DIV/0!</v>
@@ -11900,16 +11903,16 @@
     </row>
     <row r="409">
       <c r="B409" t="s" s="106">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F409" t="s" s="106">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="I409" t="n" s="106">
-        <v>20.0</v>
+        <v>33.0</v>
       </c>
       <c r="K409" t="n" s="106">
-        <v>22.0</v>
+        <v>13.0</v>
       </c>
       <c r="L409" t="n" s="106">
         <v>0.0</v>
@@ -11918,10 +11921,10 @@
         <v>0.0</v>
       </c>
       <c r="P409" t="n" s="106">
-        <v>220.6014734326706</v>
+        <v>208.67287964642853</v>
       </c>
       <c r="R409" t="n" s="106">
-        <v>0.1</v>
+        <v>0.15492957746478872</v>
       </c>
       <c r="S409" t="e" s="106">
         <v>#DIV/0!</v>
@@ -11929,16 +11932,16 @@
     </row>
     <row r="410">
       <c r="B410" t="s" s="75">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="F410" t="s" s="75">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="I410" t="n" s="75">
-        <v>58.0</v>
+        <v>20.0</v>
       </c>
       <c r="K410" t="n" s="75">
-        <v>38.0</v>
+        <v>17.0</v>
       </c>
       <c r="L410" t="n" s="75">
         <v>0.0</v>
@@ -11947,10 +11950,10 @@
         <v>0.0</v>
       </c>
       <c r="P410" t="n" s="75">
-        <v>223.87658306534837</v>
+        <v>210.4871951515456</v>
       </c>
       <c r="R410" t="n" s="75">
-        <v>0.29</v>
+        <v>0.09216589861751152</v>
       </c>
       <c r="S410" t="e" s="75">
         <v>#DIV/0!</v>
@@ -11958,13 +11961,13 @@
     </row>
     <row r="411">
       <c r="B411" t="s" s="106">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F411" t="s" s="106">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="I411" t="n" s="106">
-        <v>20.0</v>
+        <v>49.0</v>
       </c>
       <c r="K411" t="n" s="106">
         <v>29.0</v>
@@ -11976,10 +11979,10 @@
         <v>0.0</v>
       </c>
       <c r="P411" t="n" s="106">
-        <v>225.8384325183242</v>
+        <v>214.0205870996037</v>
       </c>
       <c r="R411" t="n" s="106">
-        <v>0.08733624454148471</v>
+        <v>0.21397379912663755</v>
       </c>
       <c r="S411" t="e" s="106">
         <v>#DIV/0!</v>
@@ -11987,16 +11990,16 @@
     </row>
     <row r="412">
       <c r="B412" t="s" s="75">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="F412" t="s" s="75">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="I412" t="n" s="75">
-        <v>56.0</v>
+        <v>20.0</v>
       </c>
       <c r="K412" t="n" s="75">
-        <v>36.0</v>
+        <v>28.0</v>
       </c>
       <c r="L412" t="n" s="75">
         <v>0.0</v>
@@ -12005,564 +12008,564 @@
         <v>0.0</v>
       </c>
       <c r="P412" t="n" s="75">
-        <v>230.04033945451658</v>
+        <v>219.55236253488033</v>
       </c>
       <c r="R412" t="n" s="75">
-        <v>0.28</v>
+        <v>0.08771929824561403</v>
       </c>
       <c r="S412" t="e" s="75">
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="413">
-      <c r="B413" t="s" s="84">
-        <v>206</v>
-      </c>
-      <c r="F413" t="s" s="84">
+      <c r="B413" t="s" s="106">
         <v>207</v>
       </c>
-      <c r="I413" t="n" s="84">
-        <v>21.0</v>
-      </c>
-      <c r="K413" t="n" s="84">
-        <v>1.0</v>
-      </c>
-      <c r="L413" t="n" s="84">
-        <v>1.0</v>
-      </c>
-      <c r="N413" t="n" s="84">
-        <v>0.047619047619047616</v>
-      </c>
-      <c r="P413" t="n" s="84">
-        <v>200.7927804980524</v>
-      </c>
-      <c r="R413" t="n" s="84">
-        <v>0.105</v>
-      </c>
-      <c r="S413" t="n" s="84">
-        <v>200.7927804980524</v>
+      <c r="F413" t="s" s="106">
+        <v>208</v>
+      </c>
+      <c r="I413" t="n" s="106">
+        <v>20.0</v>
+      </c>
+      <c r="K413" t="n" s="106">
+        <v>35.0</v>
+      </c>
+      <c r="L413" t="n" s="106">
+        <v>0.0</v>
+      </c>
+      <c r="N413" t="n" s="106">
+        <v>0.0</v>
+      </c>
+      <c r="P413" t="n" s="106">
+        <v>229.07145080062404</v>
+      </c>
+      <c r="R413" t="n" s="106">
+        <v>0.1</v>
+      </c>
+      <c r="S413" t="e" s="106">
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="414">
       <c r="B414" t="s" s="81">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="F414" t="s" s="81">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="I414" t="n" s="81">
         <v>20.0</v>
       </c>
       <c r="K414" t="n" s="81">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="L414" t="n" s="81">
-        <v>3.0</v>
+        <v>7.0</v>
       </c>
       <c r="N414" t="n" s="81">
-        <v>0.15</v>
+        <v>0.35</v>
       </c>
       <c r="P414" t="n" s="81">
-        <v>201.97596530465432</v>
+        <v>201.3006108135353</v>
       </c>
       <c r="R414" t="n" s="81">
-        <v>0.1</v>
+        <v>0.0966183574879227</v>
       </c>
       <c r="S414" t="n" s="81">
-        <v>67.3253217682181</v>
+        <v>28.757230116219326</v>
       </c>
     </row>
     <row r="415">
       <c r="B415" t="s" s="84">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="F415" t="s" s="84">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="I415" t="n" s="84">
         <v>20.0</v>
       </c>
       <c r="K415" t="n" s="84">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
       <c r="L415" t="n" s="84">
-        <v>6.0</v>
+        <v>10.0</v>
       </c>
       <c r="N415" t="n" s="84">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="P415" t="n" s="84">
-        <v>204.44460952520998</v>
+        <v>205.6358657133879</v>
       </c>
       <c r="R415" t="n" s="84">
         <v>0.1</v>
       </c>
       <c r="S415" t="n" s="84">
-        <v>34.074101587535</v>
+        <v>20.56358657133879</v>
       </c>
     </row>
     <row r="416">
       <c r="B416" t="s" s="81">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F416" t="s" s="81">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="I416" t="n" s="81">
-        <v>27.0</v>
+        <v>31.0</v>
       </c>
       <c r="K416" t="n" s="81">
-        <v>7.0</v>
+        <v>11.0</v>
       </c>
       <c r="L416" t="n" s="81">
-        <v>7.0</v>
+        <v>11.0</v>
       </c>
       <c r="N416" t="n" s="81">
-        <v>0.25925925925925924</v>
+        <v>0.3548387096774194</v>
       </c>
       <c r="P416" t="n" s="81">
-        <v>206.61383722314906</v>
+        <v>210.1526237026748</v>
       </c>
       <c r="R416" t="n" s="81">
-        <v>0.135</v>
+        <v>0.14691943127962084</v>
       </c>
       <c r="S416" t="n" s="81">
-        <v>29.516262460449866</v>
+        <v>19.104783972970434</v>
       </c>
     </row>
     <row r="417">
       <c r="B417" t="s" s="84">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F417" t="s" s="84">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I417" t="n" s="84">
         <v>20.0</v>
       </c>
       <c r="K417" t="n" s="84">
-        <v>8.0</v>
+        <v>15.0</v>
       </c>
       <c r="L417" t="n" s="84">
-        <v>8.0</v>
+        <v>15.0</v>
       </c>
       <c r="N417" t="n" s="84">
-        <v>0.4</v>
+        <v>0.75</v>
       </c>
       <c r="P417" t="n" s="84">
-        <v>203.43207135632107</v>
+        <v>205.4330083694221</v>
       </c>
       <c r="R417" t="n" s="84">
-        <v>0.09615384615384616</v>
+        <v>0.09302325581395349</v>
       </c>
       <c r="S417" t="n" s="84">
-        <v>25.429008919540134</v>
+        <v>13.695533891294808</v>
       </c>
     </row>
     <row r="418">
       <c r="B418" t="s" s="81">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="F418" t="s" s="81">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="I418" t="n" s="81">
-        <v>20.0</v>
+        <v>36.0</v>
       </c>
       <c r="K418" t="n" s="81">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="L418" t="n" s="81">
-        <v>13.0</v>
+        <v>16.0</v>
       </c>
       <c r="N418" t="n" s="81">
-        <v>0.65</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="P418" t="n" s="81">
-        <v>207.41548201385626</v>
+        <v>207.59020643956734</v>
       </c>
       <c r="R418" t="n" s="81">
-        <v>0.09389671361502347</v>
+        <v>0.18</v>
       </c>
       <c r="S418" t="n" s="81">
-        <v>15.955037077988944</v>
+        <v>12.974387902472959</v>
       </c>
     </row>
     <row r="419">
       <c r="B419" t="s" s="84">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F419" t="s" s="84">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I419" t="n" s="84">
-        <v>35.0</v>
+        <v>20.0</v>
       </c>
       <c r="K419" t="n" s="84">
-        <v>15.0</v>
+        <v>18.0</v>
       </c>
       <c r="L419" t="n" s="84">
-        <v>15.0</v>
+        <v>18.0</v>
       </c>
       <c r="N419" t="n" s="84">
-        <v>0.42857142857142855</v>
+        <v>0.9</v>
       </c>
       <c r="P419" t="n" s="84">
-        <v>213.9782319324611</v>
+        <v>215.83682948789595</v>
       </c>
       <c r="R419" t="n" s="84">
-        <v>0.175</v>
+        <v>0.1</v>
       </c>
       <c r="S419" t="n" s="84">
-        <v>14.265215462164074</v>
+        <v>11.990934971549775</v>
       </c>
     </row>
     <row r="420">
       <c r="B420" t="s" s="81">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="F420" t="s" s="81">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I420" t="n" s="81">
-        <v>36.0</v>
+        <v>20.0</v>
       </c>
       <c r="K420" t="n" s="81">
-        <v>16.0</v>
+        <v>22.0</v>
       </c>
       <c r="L420" t="n" s="81">
-        <v>16.0</v>
+        <v>22.0</v>
       </c>
       <c r="N420" t="n" s="81">
-        <v>0.4444444444444444</v>
+        <v>1.1</v>
       </c>
       <c r="P420" t="n" s="81">
-        <v>207.0875218409998</v>
+        <v>210.36552514082663</v>
       </c>
       <c r="R420" t="n" s="81">
-        <v>0.16666666666666666</v>
+        <v>0.09009009009009009</v>
       </c>
       <c r="S420" t="n" s="81">
-        <v>12.942970115062488</v>
+        <v>9.562069324583028</v>
       </c>
     </row>
     <row r="421">
       <c r="B421" t="s" s="84">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="F421" t="s" s="84">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="I421" t="n" s="84">
         <v>20.0</v>
       </c>
       <c r="K421" t="n" s="84">
-        <v>18.0</v>
+        <v>23.0</v>
       </c>
       <c r="L421" t="n" s="84">
-        <v>18.0</v>
+        <v>23.0</v>
       </c>
       <c r="N421" t="n" s="84">
-        <v>0.9</v>
+        <v>1.15</v>
       </c>
       <c r="P421" t="n" s="84">
-        <v>209.8739111016345</v>
+        <v>218.49212419241925</v>
       </c>
       <c r="R421" t="n" s="84">
-        <v>0.09174311926605505</v>
+        <v>0.1</v>
       </c>
       <c r="S421" t="n" s="84">
-        <v>11.659661727868583</v>
+        <v>9.499657573583447</v>
       </c>
     </row>
     <row r="422">
       <c r="B422" t="s" s="81">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="F422" t="s" s="81">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="I422" t="n" s="81">
-        <v>20.0</v>
+        <v>45.0</v>
       </c>
       <c r="K422" t="n" s="81">
-        <v>19.0</v>
+        <v>25.0</v>
       </c>
       <c r="L422" t="n" s="81">
-        <v>19.0</v>
+        <v>25.0</v>
       </c>
       <c r="N422" t="n" s="81">
-        <v>0.95</v>
+        <v>0.5555555555555556</v>
       </c>
       <c r="P422" t="n" s="81">
-        <v>200.62865057700844</v>
+        <v>208.15298472229856</v>
       </c>
       <c r="R422" t="n" s="81">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="S422" t="n" s="81">
-        <v>10.559402661947813</v>
+        <v>8.326119388891943</v>
       </c>
     </row>
     <row r="423">
       <c r="B423" t="s" s="84">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F423" t="s" s="84">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="I423" t="n" s="84">
-        <v>40.0</v>
+        <v>20.0</v>
       </c>
       <c r="K423" t="n" s="84">
-        <v>20.0</v>
+        <v>26.0</v>
       </c>
       <c r="L423" t="n" s="84">
-        <v>20.0</v>
+        <v>26.0</v>
       </c>
       <c r="N423" t="n" s="84">
-        <v>0.5</v>
+        <v>1.3</v>
       </c>
       <c r="P423" t="n" s="84">
-        <v>210.09474471953683</v>
+        <v>210.6863307730956</v>
       </c>
       <c r="R423" t="n" s="84">
-        <v>0.2</v>
+        <v>0.08849557522123894</v>
       </c>
       <c r="S423" t="n" s="84">
-        <v>10.504737235976842</v>
+        <v>8.103320414349831</v>
       </c>
     </row>
     <row r="424">
       <c r="B424" t="s" s="81">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="F424" t="s" s="81">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="I424" t="n" s="81">
         <v>20.0</v>
       </c>
       <c r="K424" t="n" s="81">
-        <v>24.0</v>
+        <v>30.0</v>
       </c>
       <c r="L424" t="n" s="81">
-        <v>24.0</v>
+        <v>30.0</v>
       </c>
       <c r="N424" t="n" s="81">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="P424" t="n" s="81">
-        <v>221.77886692473353</v>
+        <v>223.50158053493806</v>
       </c>
       <c r="R424" t="n" s="81">
-        <v>0.08928571428571429</v>
+        <v>0.08695652173913043</v>
       </c>
       <c r="S424" t="n" s="81">
-        <v>9.240786121863897</v>
+        <v>7.450052684497935</v>
       </c>
     </row>
     <row r="425">
       <c r="B425" t="s" s="84">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F425" t="s" s="84">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="I425" t="n" s="84">
         <v>20.0</v>
       </c>
       <c r="K425" t="n" s="84">
-        <v>27.0</v>
+        <v>31.0</v>
       </c>
       <c r="L425" t="n" s="84">
-        <v>27.0</v>
+        <v>31.0</v>
       </c>
       <c r="N425" t="n" s="84">
-        <v>1.35</v>
+        <v>1.55</v>
       </c>
       <c r="P425" t="n" s="84">
-        <v>224.47698134167211</v>
+        <v>220.708081654516</v>
       </c>
       <c r="R425" t="n" s="84">
-        <v>0.1</v>
+        <v>0.08658008658008658</v>
       </c>
       <c r="S425" t="n" s="84">
-        <v>8.313962271913782</v>
+        <v>7.119615537242452</v>
       </c>
     </row>
     <row r="426">
       <c r="B426" t="s" s="81">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="F426" t="s" s="81">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I426" t="n" s="81">
-        <v>45.0</v>
+        <v>54.0</v>
       </c>
       <c r="K426" t="n" s="81">
-        <v>25.0</v>
+        <v>34.0</v>
       </c>
       <c r="L426" t="n" s="81">
-        <v>25.0</v>
+        <v>34.0</v>
       </c>
       <c r="N426" t="n" s="81">
-        <v>0.5555555555555556</v>
+        <v>0.6296296296296297</v>
       </c>
       <c r="P426" t="n" s="81">
-        <v>206.7458301716731</v>
+        <v>229.0242363218559</v>
       </c>
       <c r="R426" t="n" s="81">
-        <v>0.2</v>
+        <v>0.27</v>
       </c>
       <c r="S426" t="n" s="81">
-        <v>8.269833206866924</v>
+        <v>6.736006950642821</v>
       </c>
     </row>
     <row r="427">
       <c r="B427" t="s" s="84">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="F427" t="s" s="84">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="I427" t="n" s="84">
-        <v>50.0</v>
+        <v>20.0</v>
       </c>
       <c r="K427" t="n" s="84">
-        <v>30.0</v>
+        <v>32.0</v>
       </c>
       <c r="L427" t="n" s="84">
-        <v>30.0</v>
+        <v>32.0</v>
       </c>
       <c r="N427" t="n" s="84">
-        <v>0.6</v>
+        <v>1.6</v>
       </c>
       <c r="P427" t="n" s="84">
-        <v>219.88916526372157</v>
+        <v>212.4798340592485</v>
       </c>
       <c r="R427" t="n" s="84">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="S427" t="n" s="84">
-        <v>7.329638842124052</v>
+        <v>6.639994814351516</v>
       </c>
     </row>
     <row r="428">
       <c r="B428" t="s" s="81">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="F428" t="s" s="81">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I428" t="n" s="81">
-        <v>55.0</v>
+        <v>20.0</v>
       </c>
       <c r="K428" t="n" s="81">
-        <v>35.0</v>
+        <v>33.0</v>
       </c>
       <c r="L428" t="n" s="81">
-        <v>35.0</v>
+        <v>33.0</v>
       </c>
       <c r="N428" t="n" s="81">
-        <v>0.6363636363636364</v>
+        <v>1.65</v>
       </c>
       <c r="P428" t="n" s="81">
-        <v>234.6862198246963</v>
+        <v>216.75288458817042</v>
       </c>
       <c r="R428" t="n" s="81">
-        <v>0.275</v>
+        <v>0.1</v>
       </c>
       <c r="S428" t="n" s="81">
-        <v>6.7053205664198945</v>
+        <v>6.568269229944558</v>
       </c>
     </row>
     <row r="429">
       <c r="B429" t="s" s="84">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F429" t="s" s="84">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="I429" t="n" s="84">
-        <v>53.0</v>
+        <v>56.0</v>
       </c>
       <c r="K429" t="n" s="84">
-        <v>33.0</v>
+        <v>36.0</v>
       </c>
       <c r="L429" t="n" s="84">
-        <v>33.0</v>
+        <v>36.0</v>
       </c>
       <c r="N429" t="n" s="84">
-        <v>0.6226415094339622</v>
+        <v>0.6428571428571429</v>
       </c>
       <c r="P429" t="n" s="84">
-        <v>216.13387558812212</v>
+        <v>235.86769517917364</v>
       </c>
       <c r="R429" t="n" s="84">
-        <v>0.22746781115879827</v>
+        <v>0.23728813559322035</v>
       </c>
       <c r="S429" t="n" s="84">
-        <v>6.549511381458246</v>
+        <v>6.5518804216437125</v>
       </c>
     </row>
     <row r="430">
       <c r="B430" t="s" s="81">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="F430" t="s" s="81">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="I430" t="n" s="81">
         <v>20.0</v>
       </c>
       <c r="K430" t="n" s="81">
-        <v>32.0</v>
+        <v>39.0</v>
       </c>
       <c r="L430" t="n" s="81">
-        <v>32.0</v>
+        <v>39.0</v>
       </c>
       <c r="N430" t="n" s="81">
-        <v>1.6</v>
+        <v>1.95</v>
       </c>
       <c r="P430" t="n" s="81">
-        <v>200.97835987708768</v>
+        <v>232.57558831939497</v>
       </c>
       <c r="R430" t="n" s="81">
-        <v>0.08620689655172414</v>
+        <v>0.1</v>
       </c>
       <c r="S430" t="n" s="81">
-        <v>6.28057374615899</v>
+        <v>5.96347662357423</v>
       </c>
     </row>
     <row r="431">
       <c r="B431" t="s" s="84">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="F431" t="s" s="84">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I431" t="n" s="84">
-        <v>59.0</v>
+        <v>20.0</v>
       </c>
       <c r="K431" t="n" s="84">
-        <v>39.0</v>
+        <v>37.0</v>
       </c>
       <c r="L431" t="n" s="84">
-        <v>39.0</v>
+        <v>37.0</v>
       </c>
       <c r="N431" t="n" s="84">
-        <v>0.6610169491525424</v>
+        <v>1.85</v>
       </c>
       <c r="P431" t="n" s="84">
-        <v>214.14174833648048</v>
+        <v>219.92790910159508</v>
       </c>
       <c r="R431" t="n" s="84">
-        <v>0.295</v>
+        <v>0.1</v>
       </c>
       <c r="S431" t="n" s="84">
-        <v>5.490814059909756</v>
+        <v>5.943997543286353</v>
       </c>
     </row>
   </sheetData>
@@ -12577,18 +12580,16 @@
     <mergeCell ref="L147:M147"/>
     <mergeCell ref="L148:M148"/>
     <mergeCell ref="K376:O376"/>
+    <mergeCell ref="L203:Q203"/>
+    <mergeCell ref="B370:G370"/>
+    <mergeCell ref="B371:G371"/>
+    <mergeCell ref="B372:G372"/>
     <mergeCell ref="B266:D266"/>
     <mergeCell ref="G266:H266"/>
     <mergeCell ref="B280:D280"/>
     <mergeCell ref="G280:H280"/>
     <mergeCell ref="B279:D279"/>
     <mergeCell ref="G279:H279"/>
-    <mergeCell ref="H370:I370"/>
-    <mergeCell ref="H371:I371"/>
-    <mergeCell ref="H372:I372"/>
-    <mergeCell ref="B370:G370"/>
-    <mergeCell ref="B371:G371"/>
-    <mergeCell ref="B372:G372"/>
     <mergeCell ref="F141:G141"/>
     <mergeCell ref="F142:G142"/>
     <mergeCell ref="H146:K146"/>
@@ -12626,7 +12627,6 @@
     <mergeCell ref="L146:M146"/>
     <mergeCell ref="D203:G203"/>
     <mergeCell ref="H203:K203"/>
-    <mergeCell ref="L203:Q203"/>
     <mergeCell ref="B391:E391"/>
     <mergeCell ref="F391:H391"/>
     <mergeCell ref="L391:M391"/>
@@ -12640,6 +12640,9 @@
     <mergeCell ref="K377:O377"/>
     <mergeCell ref="K378:O378"/>
     <mergeCell ref="P376:R376"/>
+    <mergeCell ref="H370:I370"/>
+    <mergeCell ref="H371:I371"/>
+    <mergeCell ref="H372:I372"/>
     <mergeCell ref="B392:E392"/>
     <mergeCell ref="F392:H392"/>
     <mergeCell ref="I392:J392"/>
@@ -12992,369 +12995,423 @@
         <v>15</v>
       </c>
       <c r="J1" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K1" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="L1" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="M1" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="N1" s="34" t="s">
-        <v>47</v>
-      </c>
       <c r="O1" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="P1" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q1" s="37" t="s">
+      <c r="R1" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="R1" s="29" t="s">
+      <c r="S1" s="29" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="S1" s="29" t="s">
-        <v>61</v>
-      </c>
-      <c r="T1" s="29" t="s">
-        <v>62</v>
-      </c>
       <c r="U1" s="32" t="s">
+        <v>63</v>
+      </c>
+      <c r="V1" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="W1" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="V1" s="32" t="s">
-        <v>66</v>
-      </c>
-      <c r="W1" s="32" t="s">
-        <v>67</v>
-      </c>
       <c r="X1" s="32" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="Y1" s="32" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A2" t="n">
-        <v>26.0</v>
+        <v>2.0</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0</v>
+        <v>1156.0</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="E2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="F2" t="n">
-        <v>75.0</v>
+        <v>664.0</v>
       </c>
       <c r="G2" t="n" s="109">
-        <v>42697.0</v>
+        <v>42704.0</v>
       </c>
       <c r="H2" t="n">
-        <v>23.0</v>
+        <v>31.0</v>
       </c>
       <c r="I2" t="n">
-        <v>52.0</v>
+        <v>107.0</v>
       </c>
       <c r="J2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="K2" t="n">
-        <v>2.0</v>
+        <v>2004.0</v>
       </c>
       <c r="L2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M2" t="n">
-        <v>94.0</v>
+        <v>739.0</v>
       </c>
       <c r="N2" t="n">
-        <v>36.0</v>
+        <v>283.0</v>
       </c>
       <c r="O2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P2" t="n">
-        <v>101.0</v>
+        <v>1008.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>44.0</v>
+        <v>362.0</v>
       </c>
       <c r="R2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="S2" t="n">
-        <v>56.0</v>
+        <v>433.0</v>
       </c>
       <c r="T2" t="n">
-        <v>28.0</v>
+        <v>159.0</v>
       </c>
       <c r="X2" t="n" s="99">
-        <v>21.0</v>
+        <v>22.0</v>
       </c>
       <c r="Y2" t="n" s="99">
-        <v>4.426966060471791</v>
+        <v>4.528202119281283</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A3" t="n">
-        <v>23.0</v>
+        <v>197.0</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C3" t="n">
-        <v>6.0</v>
+        <v>238.0</v>
       </c>
       <c r="D3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="F3" t="n">
-        <v>28.0</v>
+        <v>226.0</v>
       </c>
       <c r="G3" t="n" s="109">
-        <v>42698.0</v>
+        <v>42705.0</v>
       </c>
       <c r="H3" t="n">
-        <v>28.0</v>
+        <v>32.0</v>
       </c>
       <c r="I3" t="n">
-        <v>56.0</v>
+        <v>107.0</v>
       </c>
       <c r="J3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="K3" t="n">
-        <v>241.0</v>
+        <v>55.0</v>
       </c>
       <c r="L3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M3" t="n">
-        <v>66.0</v>
+        <v>706.0</v>
       </c>
       <c r="N3" t="n">
-        <v>21.0</v>
+        <v>263.0</v>
       </c>
       <c r="O3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="P3" t="n">
-        <v>113.0</v>
+        <v>907.0</v>
       </c>
       <c r="Q3" t="n">
-        <v>33.0</v>
+        <v>332.0</v>
       </c>
       <c r="R3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="S3" t="n">
-        <v>52.0</v>
+        <v>417.0</v>
       </c>
       <c r="T3" t="n">
-        <v>23.0</v>
+        <v>148.0</v>
       </c>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" t="n">
-        <v>155.0</v>
+        <v>202.0</v>
       </c>
       <c r="B4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C4" t="n">
-        <v>24.0</v>
+        <v>105.0</v>
       </c>
       <c r="D4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="E4" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="F4" t="n">
-        <v>24.0</v>
+        <v>157.0</v>
       </c>
       <c r="G4" t="n" s="109">
-        <v>42699.0</v>
+        <v>42706.0</v>
       </c>
       <c r="H4" t="n">
-        <v>12.0</v>
+        <v>32.0</v>
       </c>
       <c r="I4" t="n">
-        <v>45.0</v>
+        <v>92.0</v>
       </c>
       <c r="J4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="K4" t="n">
-        <v>3.0</v>
+        <v>27.0</v>
       </c>
       <c r="L4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="M4" t="n">
-        <v>30.0</v>
+        <v>235.0</v>
       </c>
       <c r="N4" t="n">
-        <v>13.0</v>
+        <v>74.0</v>
       </c>
       <c r="R4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S4" t="n">
-        <v>58.0</v>
+        <v>375.0</v>
       </c>
       <c r="T4" t="n">
-        <v>14.0</v>
+        <v>139.0</v>
       </c>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" t="n">
-        <v>28.0</v>
+        <v>138.0</v>
       </c>
       <c r="B5" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C5" t="n">
-        <v>37.0</v>
+        <v>113.0</v>
       </c>
       <c r="D5" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="E5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="F5" t="n">
-        <v>17.0</v>
+        <v>77.0</v>
       </c>
       <c r="G5" t="n" s="109">
-        <v>42700.0</v>
+        <v>42709.0</v>
       </c>
       <c r="H5" t="n">
-        <v>8.0</v>
+        <v>93.0</v>
       </c>
       <c r="I5" t="n">
-        <v>47.0</v>
+        <v>179.0</v>
       </c>
       <c r="J5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K5" t="n">
-        <v>1.0</v>
+        <v>56.0</v>
       </c>
       <c r="L5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M5" t="n">
-        <v>7.0</v>
+        <v>198.0</v>
       </c>
       <c r="N5" t="n">
-        <v>4.0</v>
+        <v>49.0</v>
       </c>
       <c r="R5" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="S5" t="n">
-        <v>45.0</v>
+        <v>340.0</v>
       </c>
       <c r="T5" t="n">
-        <v>12.0</v>
+        <v>119.0</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A6" t="n">
-        <v>26.0</v>
+        <v>1573.0</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C6" t="n">
-        <v>0.0</v>
+        <v>91.0</v>
       </c>
       <c r="D6" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="E6" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="F6" t="n">
-        <v>9.0</v>
+        <v>41.0</v>
       </c>
       <c r="G6" t="n" s="109">
-        <v>42701.0</v>
+        <v>42710.0</v>
       </c>
       <c r="H6" t="n">
-        <v>14.0</v>
+        <v>34.0</v>
       </c>
       <c r="I6" t="n">
-        <v>58.0</v>
+        <v>106.0</v>
       </c>
       <c r="J6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="K6" t="n">
-        <v>2.0</v>
+        <v>17.0</v>
       </c>
       <c r="L6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M6" t="n">
-        <v>22.0</v>
+        <v>71.0</v>
       </c>
       <c r="N6" t="n">
-        <v>2.0</v>
+        <v>34.0</v>
       </c>
       <c r="R6" t="s">
+        <v>159</v>
+      </c>
+      <c r="S6" t="n">
+        <v>321.0</v>
+      </c>
+      <c r="T6" t="n">
+        <v>94.0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A7" t="n">
+        <v>199.0</v>
+      </c>
+      <c r="B7" t="s">
+        <v>109</v>
+      </c>
+      <c r="C7" t="n">
+        <v>138.0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7" t="n">
+        <v>38.0</v>
+      </c>
+      <c r="G7" t="n" s="109">
+        <v>42711.0</v>
+      </c>
+      <c r="H7" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="I7" t="n">
+        <v>112.0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>139</v>
+      </c>
+      <c r="K7" t="n">
+        <v>19.0</v>
+      </c>
+      <c r="R7" t="s">
         <v>160</v>
       </c>
-      <c r="S6" t="n">
-        <v>47.0</v>
-      </c>
-      <c r="T6" t="n">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="C7" t="n">
-        <v>131.0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>115</v>
-      </c>
-      <c r="E7" t="s">
-        <v>124</v>
-      </c>
-      <c r="F7" t="n">
-        <v>5.0</v>
-      </c>
-      <c r="J7" t="s">
-        <v>141</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1.0</v>
+      <c r="S7" t="n">
+        <v>227.0</v>
+      </c>
+      <c r="T7" t="n">
+        <v>78.0</v>
       </c>
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.25">
       <c r="C8" t="n">
-        <v>11.0</v>
+        <v>62.0</v>
       </c>
       <c r="D8" t="s">
-        <v>116</v>
+        <v>118</v>
+      </c>
+      <c r="E8" t="s">
+        <v>127</v>
+      </c>
+      <c r="F8" t="n">
+        <v>22.0</v>
+      </c>
+      <c r="G8" t="n" s="109">
+        <v>42716.0</v>
+      </c>
+      <c r="H8" t="n">
+        <v>31.0</v>
+      </c>
+      <c r="I8" t="n">
+        <v>93.0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>140</v>
+      </c>
+      <c r="K8" t="n">
+        <v>33.0</v>
+      </c>
+      <c r="R8" t="s">
+        <v>161</v>
+      </c>
+      <c r="S8" t="n">
+        <v>198.0</v>
+      </c>
+      <c r="T8" t="n">
+        <v>59.0</v>
       </c>
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.25"/>
@@ -13390,68 +13447,68 @@
   <sheetData>
     <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="87" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B1" s="88" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C1" s="89" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="90" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="91" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C2" s="92" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A3" s="93" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B3" s="94" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C3" s="95" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="96" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B4" s="94" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C4" s="95" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="97" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B5" s="98" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C5" s="99" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A6" s="100" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B6" s="101" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C6" s="102" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
@@ -13486,14 +13543,14 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B13" s="48"/>
       <c r="C13" s="47"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="43" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B14" s="48"/>
       <c r="C14" s="47"/>
@@ -13535,235 +13592,235 @@
     </row>
     <row r="24" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A24" s="145" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B24" s="145"/>
       <c r="C24" s="145"/>
       <c r="D24" s="145"/>
       <c r="E24" s="145" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F24" s="145"/>
       <c r="G24" s="145"/>
       <c r="H24" s="145" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I24" s="145"/>
       <c r="J24" s="67" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K24" s="142" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L24" s="142"/>
       <c r="M24" s="142" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N24" s="142"/>
       <c r="O24" s="145" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P24" s="145"/>
       <c r="Q24" s="67" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R24" s="142" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S24" s="142"/>
     </row>
     <row r="25" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A25" s="143" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B25" s="143"/>
       <c r="C25" s="143"/>
       <c r="D25" s="143"/>
       <c r="E25" s="143" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F25" s="143"/>
       <c r="G25" s="143"/>
       <c r="H25" s="143" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I25" s="143"/>
       <c r="J25" s="68" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K25" s="144" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L25" s="144"/>
       <c r="M25" s="144" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N25" s="144"/>
       <c r="O25" s="143" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P25" s="143"/>
       <c r="Q25" s="68" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R25" s="144" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S25" s="144"/>
     </row>
     <row r="26" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A26" s="149" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B26" s="149"/>
       <c r="C26" s="149"/>
       <c r="D26" s="149"/>
       <c r="E26" s="149" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F26" s="149"/>
       <c r="G26" s="149"/>
       <c r="H26" s="149" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I26" s="149"/>
       <c r="J26" s="66" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K26" s="146" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L26" s="146"/>
       <c r="M26" s="146" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N26" s="146"/>
       <c r="O26" s="149" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P26" s="149"/>
       <c r="Q26" s="66" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R26" s="146" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S26" s="146"/>
     </row>
     <row r="27" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A27" s="147" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B27" s="147"/>
       <c r="C27" s="147"/>
       <c r="D27" s="147"/>
       <c r="E27" s="147" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F27" s="147"/>
       <c r="G27" s="147"/>
       <c r="H27" s="147" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I27" s="147"/>
       <c r="J27" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K27" s="148" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L27" s="148"/>
       <c r="M27" s="148" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N27" s="148"/>
       <c r="O27" s="147" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P27" s="147"/>
       <c r="Q27" s="69" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R27" s="148" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S27" s="148"/>
     </row>
     <row r="28" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A28" s="153" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B28" s="153"/>
       <c r="C28" s="153"/>
       <c r="D28" s="153"/>
       <c r="E28" s="153" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F28" s="153"/>
       <c r="G28" s="153"/>
       <c r="H28" s="153" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I28" s="153"/>
       <c r="J28" s="70" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K28" s="150" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L28" s="150"/>
       <c r="M28" s="150" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N28" s="150"/>
       <c r="O28" s="153" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P28" s="153"/>
       <c r="Q28" s="70" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R28" s="150" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S28" s="150"/>
     </row>
     <row r="29" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A29" s="151" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B29" s="151"/>
       <c r="C29" s="151"/>
       <c r="D29" s="151"/>
       <c r="E29" s="151" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F29" s="151"/>
       <c r="G29" s="151"/>
       <c r="H29" s="151" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="I29" s="151"/>
       <c r="J29" s="71" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="K29" s="152" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L29" s="152"/>
       <c r="M29" s="152" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="N29" s="152"/>
       <c r="O29" s="151" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P29" s="151"/>
       <c r="Q29" s="71" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="R29" s="152" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="S29" s="152"/>
     </row>
@@ -13989,7 +14046,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="30" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -13997,7 +14054,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -14005,7 +14062,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="34" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -14013,7 +14070,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="34" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -14021,7 +14078,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B21">
         <v>20</v>
@@ -14029,7 +14086,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="42" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B22">
         <v>21</v>
@@ -14037,7 +14094,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="42" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B23">
         <v>22</v>
@@ -14045,7 +14102,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B24">
         <v>23</v>
@@ -14053,7 +14110,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" s="37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B25">
         <v>24</v>
@@ -14061,7 +14118,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="37" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B26">
         <v>25</v>
@@ -14069,7 +14126,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B27">
         <v>26</v>
@@ -14077,7 +14134,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="29" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B28">
         <v>27</v>
@@ -14085,7 +14142,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B29">
         <v>28</v>
@@ -14093,7 +14150,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B30">
         <v>29</v>
@@ -14101,7 +14158,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="41" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B31">
         <v>30</v>
@@ -14109,7 +14166,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B32">
         <v>31</v>
@@ -14117,7 +14174,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B33">
         <v>32</v>
@@ -14125,7 +14182,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="32" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B34">
         <v>33</v>
@@ -14133,7 +14190,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="41" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B35">
         <v>34</v>
@@ -14141,7 +14198,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B36">
         <v>35</v>
@@ -14149,7 +14206,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="38" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B37">
         <v>36</v>
@@ -14157,7 +14214,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="38" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B38">
         <v>37</v>
@@ -14165,7 +14222,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="38" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B39">
         <v>38</v>
@@ -14173,7 +14230,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="39" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B40">
         <v>39</v>
@@ -14181,7 +14238,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="39" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B41">
         <v>40</v>
@@ -14189,7 +14246,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B42">
         <v>41</v>
@@ -14197,7 +14254,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B43">
         <v>42</v>

</xml_diff>